<commit_message>
Initial commit R2015b.  Version  4p1.
</commit_message>
<xml_diff>
--- a/Scripts_Data/CFR_Results.xlsx
+++ b/Scripts_Data/CFR_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R15a\Scripts_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R15b\Scripts_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -213,10 +213,10 @@
     <t>CFL v4.0</t>
   </si>
   <si>
-    <t>8.5.1.281278 (R2015a) Service Pack 1</t>
-  </si>
-  <si>
-    <t>09-Mar-2018 23:14:00</t>
+    <t>8.6.0.267246 (R2015b)</t>
+  </si>
+  <si>
+    <t>09-Mar-2018 11:51:27</t>
   </si>
 </sst>
 </file>
@@ -798,25 +798,25 @@
         <v>2560</v>
       </c>
       <c r="E4" s="14">
-        <v>0.23699999999999999</v>
+        <v>1.472</v>
       </c>
       <c r="F4" s="15">
         <v>2560</v>
       </c>
       <c r="G4" s="14">
-        <v>0.18</v>
+        <v>0.216</v>
       </c>
       <c r="H4" s="15">
         <v>2560</v>
       </c>
       <c r="I4" s="14">
-        <v>0.17899999999999999</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="J4" s="15">
         <v>2560</v>
       </c>
       <c r="K4" s="14">
-        <v>0.18</v>
+        <v>0.22600000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -833,19 +833,19 @@
         <v>674</v>
       </c>
       <c r="E5" s="11">
-        <v>8.3000000000000004E-2</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="F5" s="4">
         <v>948</v>
       </c>
       <c r="G5" s="11">
-        <v>7.3999999999999996E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="H5" s="4">
         <v>731</v>
       </c>
       <c r="I5" s="11">
-        <v>7.8E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="J5" s="4">
         <v>1063</v>
@@ -868,7 +868,7 @@
         <v>311</v>
       </c>
       <c r="E6" s="11">
-        <v>9.5000000000000001E-2</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="F6" s="4">
         <v>365</v>
@@ -880,13 +880,13 @@
         <v>317</v>
       </c>
       <c r="I6" s="11">
-        <v>5.1999999999999998E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="J6" s="4">
         <v>397</v>
       </c>
       <c r="K6" s="11">
-        <v>6.0999999999999999E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -903,25 +903,25 @@
         <v>3742</v>
       </c>
       <c r="E7" s="11">
-        <v>1.673</v>
+        <v>2.0190000000000001</v>
       </c>
       <c r="F7" s="4">
         <v>4949</v>
       </c>
       <c r="G7" s="11">
-        <v>2.548</v>
+        <v>2.4950000000000001</v>
       </c>
       <c r="H7" s="4">
         <v>5144</v>
       </c>
       <c r="I7" s="11">
-        <v>2.681</v>
+        <v>2.5139999999999998</v>
       </c>
       <c r="J7" s="4">
         <v>6216</v>
       </c>
       <c r="K7" s="11">
-        <v>3.5539999999999998</v>
+        <v>3.5819999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -938,25 +938,25 @@
         <v>2040</v>
       </c>
       <c r="E8" s="11">
-        <v>0.19800000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="F8" s="4">
         <v>2611</v>
       </c>
       <c r="G8" s="11">
-        <v>0.223</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="H8" s="4">
         <v>2284</v>
       </c>
       <c r="I8" s="11">
-        <v>0.19500000000000001</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="J8" s="4">
         <v>2928</v>
       </c>
       <c r="K8" s="11">
-        <v>0.26800000000000002</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -970,28 +970,28 @@
         <v>1.2</v>
       </c>
       <c r="D9" s="4">
-        <v>605</v>
+        <v>613</v>
       </c>
       <c r="E9" s="11">
-        <v>0.14199999999999999</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="F9" s="4">
-        <v>611</v>
+        <v>567</v>
       </c>
       <c r="G9" s="11">
-        <v>0.11600000000000001</v>
+        <v>0.109</v>
       </c>
       <c r="H9" s="4">
-        <v>690</v>
+        <v>745</v>
       </c>
       <c r="I9" s="11">
-        <v>0.112</v>
+        <v>0.123</v>
       </c>
       <c r="J9" s="4">
-        <v>571</v>
+        <v>510</v>
       </c>
       <c r="K9" s="11">
-        <v>0.121</v>
+        <v>0.113</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1008,25 +1008,25 @@
         <v>200</v>
       </c>
       <c r="E10" s="11">
-        <v>5.2999999999999999E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F10" s="4">
         <v>207</v>
       </c>
       <c r="G10" s="11">
-        <v>3.3000000000000002E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="H10" s="4">
         <v>213</v>
       </c>
       <c r="I10" s="11">
-        <v>2.9000000000000001E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="J10" s="4">
         <v>221</v>
       </c>
       <c r="K10" s="11">
-        <v>3.1E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1043,25 +1043,25 @@
         <v>9852</v>
       </c>
       <c r="E11" s="11">
-        <v>2.3719999999999999</v>
+        <v>2.6440000000000001</v>
       </c>
       <c r="F11" s="4">
         <v>18626</v>
       </c>
       <c r="G11" s="11">
-        <v>5.3029999999999999</v>
+        <v>6.8090000000000002</v>
       </c>
       <c r="H11" s="4">
         <v>10967</v>
       </c>
       <c r="I11" s="11">
-        <v>3.8090000000000002</v>
+        <v>3.9670000000000001</v>
       </c>
       <c r="J11" s="4">
         <v>21511</v>
       </c>
       <c r="K11" s="11">
-        <v>8.0690000000000008</v>
+        <v>8.4350000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1078,25 +1078,25 @@
         <v>1211</v>
       </c>
       <c r="E12" s="11">
-        <v>0.112</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="F12" s="4">
         <v>1211</v>
       </c>
       <c r="G12" s="11">
-        <v>5.0999999999999997E-2</v>
+        <v>0.06</v>
       </c>
       <c r="H12" s="4">
         <v>1211</v>
       </c>
       <c r="I12" s="11">
-        <v>5.2999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="J12" s="4">
         <v>1211</v>
       </c>
       <c r="K12" s="11">
-        <v>5.6000000000000001E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1113,25 +1113,25 @@
         <v>1300</v>
       </c>
       <c r="E13" s="11">
-        <v>0.16300000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="F13" s="3">
         <v>1422</v>
       </c>
       <c r="G13" s="11">
-        <v>0.161</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="H13" s="4">
         <v>1394</v>
       </c>
       <c r="I13" s="11">
-        <v>0.14899999999999999</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="J13" s="4">
         <v>1483</v>
       </c>
       <c r="K13" s="11">
-        <v>0.19</v>
+        <v>0.191</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1145,28 +1145,28 @@
         <v>45</v>
       </c>
       <c r="D14" s="4">
-        <v>5738</v>
+        <v>5808</v>
       </c>
       <c r="E14" s="11">
-        <v>0.41399999999999998</v>
+        <v>0.495</v>
       </c>
       <c r="F14" s="3">
-        <v>5738</v>
+        <v>5808</v>
       </c>
       <c r="G14" s="11">
-        <v>0.32400000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="H14" s="4">
-        <v>5738</v>
+        <v>5808</v>
       </c>
       <c r="I14" s="11">
-        <v>0.313</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="J14" s="4">
-        <v>5738</v>
+        <v>5808</v>
       </c>
       <c r="K14" s="11">
-        <v>0.316</v>
+        <v>0.39500000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1183,13 +1183,13 @@
         <v>732</v>
       </c>
       <c r="E15" s="11">
-        <v>9.9000000000000005E-2</v>
+        <v>0.113</v>
       </c>
       <c r="F15" s="3">
         <v>857</v>
       </c>
       <c r="G15" s="11">
-        <v>7.6999999999999999E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="H15" s="3">
         <v>807</v>
@@ -1201,7 +1201,7 @@
         <v>983</v>
       </c>
       <c r="K15" s="11">
-        <v>9.0999999999999998E-2</v>
+        <v>0.10199999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1218,25 +1218,25 @@
         <v>1305</v>
       </c>
       <c r="E16" s="11">
-        <v>0.13200000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F16" s="3">
         <v>1400</v>
       </c>
       <c r="G16" s="11">
-        <v>0.11799999999999999</v>
+        <v>0.126</v>
       </c>
       <c r="H16" s="3">
         <v>1415</v>
       </c>
       <c r="I16" s="11">
-        <v>0.107</v>
+        <v>0.124</v>
       </c>
       <c r="J16" s="3">
         <v>1478</v>
       </c>
       <c r="K16" s="11">
-        <v>0.123</v>
+        <v>0.13400000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1253,25 +1253,25 @@
         <v>6337</v>
       </c>
       <c r="E17" s="11">
-        <v>1.0169999999999999</v>
+        <v>1.3520000000000001</v>
       </c>
       <c r="F17" s="3">
         <v>6769</v>
       </c>
       <c r="G17" s="11">
-        <v>1.1879999999999999</v>
+        <v>1.3839999999999999</v>
       </c>
       <c r="H17" s="3">
         <v>5922</v>
       </c>
       <c r="I17" s="11">
-        <v>1.032</v>
+        <v>1.2889999999999999</v>
       </c>
       <c r="J17" s="3">
         <v>6371</v>
       </c>
       <c r="K17" s="11">
-        <v>1.2250000000000001</v>
+        <v>1.6359999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1288,25 +1288,25 @@
         <v>277</v>
       </c>
       <c r="E18" s="11">
-        <v>0.09</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F18" s="3">
         <v>313</v>
       </c>
       <c r="G18" s="11">
-        <v>0.06</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="H18" s="3">
         <v>308</v>
       </c>
       <c r="I18" s="11">
-        <v>5.5E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="J18" s="3">
         <v>330</v>
       </c>
       <c r="K18" s="11">
-        <v>6.5000000000000002E-2</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1320,28 +1320,28 @@
         <v>30</v>
       </c>
       <c r="D19" s="4">
-        <v>3449</v>
+        <v>3454</v>
       </c>
       <c r="E19" s="11">
-        <v>0.56200000000000006</v>
+        <v>0.90900000000000003</v>
       </c>
       <c r="F19" s="3">
-        <v>3674</v>
+        <v>3682</v>
       </c>
       <c r="G19" s="11">
-        <v>0.58099999999999996</v>
+        <v>0.748</v>
       </c>
       <c r="H19" s="3">
-        <v>3532</v>
+        <v>3499</v>
       </c>
       <c r="I19" s="11">
-        <v>0.51900000000000002</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="J19" s="3">
-        <v>3794</v>
+        <v>3835</v>
       </c>
       <c r="K19" s="11">
-        <v>0.64100000000000001</v>
+        <v>0.83499999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1355,28 +1355,28 @@
         <v>50</v>
       </c>
       <c r="D20" s="4">
-        <v>6767</v>
+        <v>6945</v>
       </c>
       <c r="E20" s="11">
-        <v>0.71299999999999997</v>
+        <v>1.143</v>
       </c>
       <c r="F20" s="3">
-        <v>7253</v>
+        <v>7209</v>
       </c>
       <c r="G20" s="11">
-        <v>0.78600000000000003</v>
+        <v>1.05</v>
       </c>
       <c r="H20" s="3">
-        <v>98173</v>
+        <v>99540</v>
       </c>
       <c r="I20" s="11">
-        <v>10.266</v>
+        <v>11.587999999999999</v>
       </c>
       <c r="J20" s="3">
-        <v>99430</v>
+        <v>99405</v>
       </c>
       <c r="K20" s="11">
-        <v>10.833</v>
+        <v>12.962999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1393,25 +1393,25 @@
         <v>3513</v>
       </c>
       <c r="E21" s="11">
-        <v>0.32900000000000001</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="F21" s="3">
         <v>4658</v>
       </c>
       <c r="G21" s="11">
-        <v>0.51600000000000001</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="H21" s="3">
         <v>4063</v>
       </c>
       <c r="I21" s="11">
-        <v>0.373</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="J21" s="3">
         <v>4027</v>
       </c>
       <c r="K21" s="11">
-        <v>0.41699999999999998</v>
+        <v>0.46400000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1425,28 +1425,28 @@
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <v>1898</v>
+        <v>2318</v>
       </c>
       <c r="E22" s="11">
-        <v>3.5979999999999999</v>
+        <v>3.948</v>
       </c>
       <c r="F22" s="3">
-        <v>1898</v>
+        <v>2318</v>
       </c>
       <c r="G22" s="11">
-        <v>3.8980000000000001</v>
+        <v>3.524</v>
       </c>
       <c r="H22" s="3">
-        <v>1898</v>
+        <v>2318</v>
       </c>
       <c r="I22" s="11">
-        <v>4.0449999999999999</v>
+        <v>3.536</v>
       </c>
       <c r="J22" s="3">
-        <v>1898</v>
+        <v>2318</v>
       </c>
       <c r="K22" s="11">
-        <v>4.0469999999999997</v>
+        <v>3.6930000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1460,28 +1460,28 @@
         <v>15</v>
       </c>
       <c r="D23" s="4">
-        <v>3116</v>
+        <v>3073</v>
       </c>
       <c r="E23" s="11">
-        <v>1.032</v>
+        <v>1.0980000000000001</v>
       </c>
       <c r="F23" s="3">
-        <v>3140</v>
+        <v>3077</v>
       </c>
       <c r="G23" s="11">
-        <v>1.1279999999999999</v>
+        <v>1.1839999999999999</v>
       </c>
       <c r="H23" s="3">
-        <v>3773</v>
+        <v>3723</v>
       </c>
       <c r="I23" s="11">
-        <v>1.3859999999999999</v>
+        <v>1.4259999999999999</v>
       </c>
       <c r="J23" s="3">
-        <v>3699</v>
+        <v>3633</v>
       </c>
       <c r="K23" s="11">
-        <v>1.367</v>
+        <v>1.4650000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1495,28 +1495,28 @@
         <v>4</v>
       </c>
       <c r="D24" s="4">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E24" s="11">
-        <v>5.7000000000000002E-2</v>
+        <v>0.156</v>
       </c>
       <c r="F24" s="3">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G24" s="11">
-        <v>2.1999999999999999E-2</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="H24" s="3">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I24" s="11">
-        <v>0.02</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="J24" s="3">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K24" s="11">
-        <v>2.4E-2</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1533,25 +1533,25 @@
         <v>4726</v>
       </c>
       <c r="E25" s="11">
-        <v>3.3969999999999998</v>
+        <v>3.9220000000000002</v>
       </c>
       <c r="F25" s="3">
         <v>5178</v>
       </c>
       <c r="G25" s="11">
-        <v>4.8440000000000003</v>
+        <v>4.5709999999999997</v>
       </c>
       <c r="H25" s="3">
         <v>4554</v>
       </c>
       <c r="I25" s="11">
-        <v>4.0510000000000002</v>
+        <v>3.82</v>
       </c>
       <c r="J25" s="3">
         <v>5129</v>
       </c>
       <c r="K25" s="11">
-        <v>4.923</v>
+        <v>4.4320000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1565,28 +1565,28 @@
         <v>12</v>
       </c>
       <c r="D26" s="4">
-        <v>13452</v>
+        <v>13098</v>
       </c>
       <c r="E26" s="11">
-        <v>6.0510000000000002</v>
+        <v>6.81</v>
       </c>
       <c r="F26" s="3">
-        <v>13762</v>
+        <v>11877</v>
       </c>
       <c r="G26" s="11">
-        <v>6.97</v>
+        <v>6.4649999999999999</v>
       </c>
       <c r="H26" s="3">
-        <v>20167</v>
+        <v>22049</v>
       </c>
       <c r="I26" s="11">
-        <v>10.521000000000001</v>
+        <v>11.522</v>
       </c>
       <c r="J26" s="3">
-        <v>23170</v>
+        <v>22779</v>
       </c>
       <c r="K26" s="11">
-        <v>12.265000000000001</v>
+        <v>11.706</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1600,28 +1600,28 @@
         <v>20</v>
       </c>
       <c r="D27" s="9">
-        <v>3439</v>
+        <v>3451</v>
       </c>
       <c r="E27" s="11">
-        <v>2.016</v>
+        <v>2.222</v>
       </c>
       <c r="F27" s="3">
-        <v>4261</v>
+        <v>4110</v>
       </c>
       <c r="G27" s="11">
-        <v>3.22</v>
+        <v>3.3980000000000001</v>
       </c>
       <c r="H27" s="3">
         <v>3538</v>
       </c>
       <c r="I27" s="11">
-        <v>2.2120000000000002</v>
+        <v>2.2109999999999999</v>
       </c>
       <c r="J27" s="3">
-        <v>5032</v>
+        <v>5557</v>
       </c>
       <c r="K27" s="11">
-        <v>4.71</v>
+        <v>6.1289999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1638,7 +1638,7 @@
         <v>940</v>
       </c>
       <c r="E28" s="11">
-        <v>0.13900000000000001</v>
+        <v>0.154</v>
       </c>
       <c r="F28" s="3">
         <v>1004</v>
@@ -1650,13 +1650,13 @@
         <v>967</v>
       </c>
       <c r="I28" s="11">
-        <v>0.112</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="J28" s="3">
         <v>1061</v>
       </c>
       <c r="K28" s="11">
-        <v>0.151</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1673,25 +1673,25 @@
         <v>710</v>
       </c>
       <c r="E29" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="F29" s="3">
         <v>833</v>
       </c>
       <c r="G29" s="11">
-        <v>0.14899999999999999</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H29" s="3">
         <v>747</v>
       </c>
       <c r="I29" s="11">
-        <v>0.128</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="J29" s="3">
         <v>860</v>
       </c>
       <c r="K29" s="11">
-        <v>0.158</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1708,25 +1708,25 @@
         <v>10343</v>
       </c>
       <c r="E30" s="11">
-        <v>11.117000000000001</v>
+        <v>13.141</v>
       </c>
       <c r="F30" s="3">
         <v>12272</v>
       </c>
       <c r="G30" s="11">
-        <v>22.859000000000002</v>
+        <v>25.661999999999999</v>
       </c>
       <c r="H30" s="3">
         <v>11659</v>
       </c>
       <c r="I30" s="11">
-        <v>18.172999999999998</v>
+        <v>19.334</v>
       </c>
       <c r="J30" s="3">
         <v>21192</v>
       </c>
       <c r="K30" s="11">
-        <v>80.010000000000005</v>
+        <v>89.869</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1743,25 +1743,25 @@
         <v>663</v>
       </c>
       <c r="E31" s="11">
-        <v>0.184</v>
+        <v>0.16</v>
       </c>
       <c r="F31" s="3">
         <v>894</v>
       </c>
       <c r="G31" s="11">
-        <v>0.184</v>
+        <v>0.192</v>
       </c>
       <c r="H31" s="3">
         <v>660</v>
       </c>
       <c r="I31" s="11">
-        <v>0.107</v>
+        <v>0.108</v>
       </c>
       <c r="J31" s="3">
         <v>933</v>
       </c>
       <c r="K31" s="11">
-        <v>0.20499999999999999</v>
+        <v>0.19700000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1778,25 +1778,25 @@
         <v>2422</v>
       </c>
       <c r="E32" s="11">
-        <v>1.294</v>
+        <v>1.268</v>
       </c>
       <c r="F32" s="3">
         <v>5303</v>
       </c>
       <c r="G32" s="11">
-        <v>8.5129999999999999</v>
+        <v>8.8840000000000003</v>
       </c>
       <c r="H32" s="3">
         <v>2512</v>
       </c>
       <c r="I32" s="11">
-        <v>1.391</v>
+        <v>1.306</v>
       </c>
       <c r="J32" s="3">
         <v>6180</v>
       </c>
       <c r="K32" s="11">
-        <v>11.342000000000001</v>
+        <v>12.259</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1813,25 +1813,25 @@
         <v>2635</v>
       </c>
       <c r="E33" s="11">
-        <v>0.52400000000000002</v>
+        <v>0.79</v>
       </c>
       <c r="F33" s="3">
         <v>4096</v>
       </c>
       <c r="G33" s="11">
-        <v>0.98</v>
+        <v>1.296</v>
       </c>
       <c r="H33" s="3">
         <v>3029</v>
       </c>
       <c r="I33" s="11">
-        <v>0.76300000000000001</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="J33" s="3">
         <v>4353</v>
       </c>
       <c r="K33" s="11">
-        <v>1.2150000000000001</v>
+        <v>1.2609999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1845,28 +1845,28 @@
         <v>3</v>
       </c>
       <c r="D34" s="4">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="E34" s="11">
-        <v>0.13700000000000001</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="F34" s="3">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="G34" s="11">
-        <v>0.35399999999999998</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="H34" s="3">
-        <v>520</v>
+        <v>481</v>
       </c>
       <c r="I34" s="11">
-        <v>0.127</v>
+        <v>0.114</v>
       </c>
       <c r="J34" s="3">
-        <v>886</v>
+        <v>868</v>
       </c>
       <c r="K34" s="11">
-        <v>0.45</v>
+        <v>0.38200000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1883,25 +1883,25 @@
         <v>1667</v>
       </c>
       <c r="E35" s="11">
-        <v>0.29099999999999998</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="F35" s="3">
         <v>3127</v>
       </c>
       <c r="G35" s="11">
-        <v>0.873</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="H35" s="3">
         <v>1739</v>
       </c>
       <c r="I35" s="11">
-        <v>0.255</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="J35" s="3">
         <v>3225</v>
       </c>
       <c r="K35" s="11">
-        <v>1.1000000000000001</v>
+        <v>0.92700000000000005</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1918,25 +1918,25 @@
         <v>4473</v>
       </c>
       <c r="E36" s="11">
-        <v>0.84099999999999997</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="F36" s="3">
         <v>6767</v>
       </c>
       <c r="G36" s="11">
-        <v>1.986</v>
+        <v>2.17</v>
       </c>
       <c r="H36" s="3">
         <v>4576</v>
       </c>
       <c r="I36" s="11">
-        <v>0.88</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="J36" s="3">
         <v>6779</v>
       </c>
       <c r="K36" s="11">
-        <v>2.165</v>
+        <v>2.4590000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1953,25 +1953,25 @@
         <v>5619</v>
       </c>
       <c r="E37" s="11">
-        <v>0.63900000000000001</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="F37" s="3">
         <v>8361</v>
       </c>
       <c r="G37" s="11">
-        <v>2.2719999999999998</v>
+        <v>2.6819999999999999</v>
       </c>
       <c r="H37" s="3">
         <v>5671</v>
       </c>
       <c r="I37" s="11">
-        <v>0.69399999999999995</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="J37" s="3">
         <v>8452</v>
       </c>
       <c r="K37" s="11">
-        <v>2.81</v>
+        <v>3.0310000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1988,25 +1988,25 @@
         <v>4175</v>
       </c>
       <c r="E38" s="11">
-        <v>0.98299999999999998</v>
+        <v>1.1879999999999999</v>
       </c>
       <c r="F38" s="3">
         <v>4632</v>
       </c>
       <c r="G38" s="11">
-        <v>1.603</v>
+        <v>1.7529999999999999</v>
       </c>
       <c r="H38" s="3">
         <v>4256</v>
       </c>
       <c r="I38" s="11">
-        <v>1.43</v>
+        <v>1.23</v>
       </c>
       <c r="J38" s="3">
         <v>4807</v>
       </c>
       <c r="K38" s="11">
-        <v>1.87</v>
+        <v>1.974</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2023,25 +2023,25 @@
         <v>4964</v>
       </c>
       <c r="E39" s="11">
-        <v>0.54800000000000004</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="F39" s="3">
         <v>5451</v>
       </c>
       <c r="G39" s="11">
-        <v>0.70899999999999996</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="H39" s="3">
         <v>4879</v>
       </c>
       <c r="I39" s="11">
-        <v>0.56000000000000005</v>
+        <v>0.63</v>
       </c>
       <c r="J39" s="3">
         <v>5234</v>
       </c>
       <c r="K39" s="11">
-        <v>0.80400000000000005</v>
+        <v>0.81399999999999995</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2055,28 +2055,28 @@
         <v>36</v>
       </c>
       <c r="D40" s="4">
-        <v>4200</v>
+        <v>4175</v>
       </c>
       <c r="E40" s="11">
-        <v>1.657</v>
+        <v>1.9450000000000001</v>
       </c>
       <c r="F40" s="3">
-        <v>4799</v>
+        <v>4596</v>
       </c>
       <c r="G40" s="11">
-        <v>2.3540000000000001</v>
+        <v>2.6480000000000001</v>
       </c>
       <c r="H40" s="3">
-        <v>4213</v>
+        <v>4185</v>
       </c>
       <c r="I40" s="11">
-        <v>1.8340000000000001</v>
+        <v>2.181</v>
       </c>
       <c r="J40" s="3">
-        <v>4593</v>
+        <v>4635</v>
       </c>
       <c r="K40" s="11">
-        <v>2.3319999999999999</v>
+        <v>3.012</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2093,25 +2093,25 @@
         <v>4601</v>
       </c>
       <c r="E41" s="11">
-        <v>1.248</v>
+        <v>1.361</v>
       </c>
       <c r="F41" s="3">
         <v>4556</v>
       </c>
       <c r="G41" s="11">
-        <v>1.792</v>
+        <v>1.8939999999999999</v>
       </c>
       <c r="H41" s="3">
         <v>4746</v>
       </c>
       <c r="I41" s="11">
-        <v>1.5720000000000001</v>
+        <v>1.7090000000000001</v>
       </c>
       <c r="J41" s="3">
         <v>4615</v>
       </c>
       <c r="K41" s="11">
-        <v>2.0779999999999998</v>
+        <v>2.0249999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2128,25 +2128,25 @@
         <v>6024</v>
       </c>
       <c r="E42" s="11">
-        <v>0.65800000000000003</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="F42" s="3">
         <v>6475</v>
       </c>
       <c r="G42" s="11">
-        <v>0.91900000000000004</v>
+        <v>1.177</v>
       </c>
       <c r="H42" s="3">
         <v>6388</v>
       </c>
       <c r="I42" s="11">
-        <v>0.80300000000000005</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="J42" s="3">
         <v>6781</v>
       </c>
       <c r="K42" s="11">
-        <v>0.96799999999999997</v>
+        <v>1.3759999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2163,25 +2163,25 @@
         <v>1231</v>
       </c>
       <c r="E43" s="11">
-        <v>0.28599999999999998</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="F43" s="3">
         <v>1385</v>
       </c>
       <c r="G43" s="11">
-        <v>0.40799999999999997</v>
+        <v>0.5</v>
       </c>
       <c r="H43" s="3">
         <v>1249</v>
       </c>
       <c r="I43" s="11">
-        <v>0.28100000000000003</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="J43" s="3">
         <v>1503</v>
       </c>
       <c r="K43" s="11">
-        <v>0.51800000000000002</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2195,28 +2195,28 @@
         <v>24</v>
       </c>
       <c r="D44" s="4">
-        <v>7738</v>
+        <v>7839</v>
       </c>
       <c r="E44" s="11">
-        <v>3.7080000000000002</v>
+        <v>4.7089999999999996</v>
       </c>
       <c r="F44" s="3">
-        <v>6575</v>
+        <v>6402</v>
       </c>
       <c r="G44" s="11">
-        <v>6.0110000000000001</v>
+        <v>6.3289999999999997</v>
       </c>
       <c r="H44" s="3">
-        <v>8262</v>
+        <v>8393</v>
       </c>
       <c r="I44" s="11">
-        <v>4.6920000000000002</v>
+        <v>4.9640000000000004</v>
       </c>
       <c r="J44" s="3">
-        <v>6458</v>
+        <v>6653</v>
       </c>
       <c r="K44" s="11">
-        <v>6.3490000000000002</v>
+        <v>6.4619999999999997</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2227,31 +2227,31 @@
         <v>55</v>
       </c>
       <c r="C45" s="11">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D45" s="4">
-        <v>2560</v>
+        <v>4789</v>
       </c>
       <c r="E45" s="11">
-        <v>0.21299999999999999</v>
+        <v>4.7160000000000002</v>
       </c>
       <c r="F45" s="3">
-        <v>2560</v>
+        <v>4789</v>
       </c>
       <c r="G45" s="11">
-        <v>0.17100000000000001</v>
+        <v>4.5110000000000001</v>
       </c>
       <c r="H45" s="3">
-        <v>2560</v>
+        <v>4789</v>
       </c>
       <c r="I45" s="11">
-        <v>0.17499999999999999</v>
+        <v>4.899</v>
       </c>
       <c r="J45" s="3">
-        <v>2560</v>
+        <v>4789</v>
       </c>
       <c r="K45" s="11">
-        <v>0.17799999999999999</v>
+        <v>4.5019999999999998</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2265,28 +2265,28 @@
         <v>8.5</v>
       </c>
       <c r="D46" s="4">
-        <v>2604</v>
+        <v>2565</v>
       </c>
       <c r="E46" s="11">
-        <v>26.937999999999999</v>
+        <v>18.984000000000002</v>
       </c>
       <c r="F46" s="3">
-        <v>2604</v>
+        <v>2565</v>
       </c>
       <c r="G46" s="11">
-        <v>25.885999999999999</v>
+        <v>19.010999999999999</v>
       </c>
       <c r="H46" s="3">
-        <v>2604</v>
+        <v>2565</v>
       </c>
       <c r="I46" s="11">
-        <v>25.498000000000001</v>
+        <v>18.683</v>
       </c>
       <c r="J46" s="3">
-        <v>2604</v>
+        <v>2565</v>
       </c>
       <c r="K46" s="11">
-        <v>25.105</v>
+        <v>18.646000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2303,7 +2303,7 @@
         <v>8673</v>
       </c>
       <c r="E47" s="11">
-        <v>4.1820000000000004</v>
+        <v>4.2709999999999999</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>44</v>
@@ -2338,7 +2338,7 @@
         <v>8919</v>
       </c>
       <c r="E48" s="11">
-        <v>5.1959999999999997</v>
+        <v>5.3570000000000002</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>44</v>
@@ -2373,7 +2373,7 @@
         <v>15052</v>
       </c>
       <c r="E49" s="11">
-        <v>10.097</v>
+        <v>10.231999999999999</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>44</v>
@@ -2408,7 +2408,7 @@
         <v>11289</v>
       </c>
       <c r="E50" s="11">
-        <v>7.9009999999999998</v>
+        <v>8.1929999999999996</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>44</v>
@@ -2443,7 +2443,7 @@
         <v>8973</v>
       </c>
       <c r="E51" s="11">
-        <v>5.2619999999999996</v>
+        <v>5.26</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>44</v>
@@ -2478,7 +2478,7 @@
         <v>11694</v>
       </c>
       <c r="E52" s="11">
-        <v>12.606999999999999</v>
+        <v>11.776999999999999</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>44</v>
@@ -2510,10 +2510,10 @@
         <v>41.28</v>
       </c>
       <c r="D53" s="2">
-        <v>11510</v>
+        <v>11318</v>
       </c>
       <c r="E53" s="11">
-        <v>8.5579999999999998</v>
+        <v>8.3559999999999999</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>44</v>
@@ -2548,7 +2548,7 @@
         <v>12142</v>
       </c>
       <c r="E54" s="11">
-        <v>13.308999999999999</v>
+        <v>13.596</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>44</v>
@@ -2580,10 +2580,10 @@
         <v>27.71</v>
       </c>
       <c r="D55" s="2">
-        <v>9020</v>
+        <v>8758</v>
       </c>
       <c r="E55" s="11">
-        <v>9.5960000000000001</v>
+        <v>9.5679999999999996</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>44</v>
@@ -2618,6 +2618,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100525B94EEF47D42499A62120CC90E0AB3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e706cd362d7e41030bb8c72a7c62a9d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c85acdc-a394-4ae0-8c72-fb4a95b3d573" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55e2521e7df4d5c11309cefaa7c01562" ns2:_="">
     <xsd:import namespace="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
@@ -2762,18 +2773,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2819,29 +2828,10 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2863,25 +2853,35 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630E037-F79E-4175-B540-A23B306F8900}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE6D0D52-57FE-48CB-8E43-11384E6CFEE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630E037-F79E-4175-B540-A23B306F8900}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Initial commit R2016a.  Version 4p1.
</commit_message>
<xml_diff>
--- a/Scripts_Data/CFR_Results.xlsx
+++ b/Scripts_Data/CFR_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R15b\Scripts_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R16a\Scripts_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -213,10 +213,10 @@
     <t>CFL v4.0</t>
   </si>
   <si>
-    <t>8.6.0.267246 (R2015b)</t>
-  </si>
-  <si>
-    <t>09-Mar-2018 11:51:27</t>
+    <t>9.0.0.341360 (R2016a)</t>
+  </si>
+  <si>
+    <t>09-Mar-2018 10:12:47</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:K55"/>
+      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,28 +795,28 @@
         <v>6</v>
       </c>
       <c r="D4" s="15">
-        <v>2560</v>
+        <v>2387</v>
       </c>
       <c r="E4" s="14">
-        <v>1.472</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="F4" s="15">
-        <v>2560</v>
+        <v>2387</v>
       </c>
       <c r="G4" s="14">
-        <v>0.216</v>
+        <v>0.17</v>
       </c>
       <c r="H4" s="15">
-        <v>2560</v>
+        <v>2387</v>
       </c>
       <c r="I4" s="14">
-        <v>0.22500000000000001</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="J4" s="15">
-        <v>2560</v>
+        <v>2387</v>
       </c>
       <c r="K4" s="14">
-        <v>0.22600000000000001</v>
+        <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -833,25 +833,25 @@
         <v>674</v>
       </c>
       <c r="E5" s="11">
-        <v>0.36699999999999999</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="F5" s="4">
-        <v>948</v>
+        <v>959</v>
       </c>
       <c r="G5" s="11">
-        <v>7.8E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="H5" s="4">
         <v>731</v>
       </c>
       <c r="I5" s="11">
-        <v>5.8999999999999997E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="J5" s="4">
-        <v>1063</v>
+        <v>1028</v>
       </c>
       <c r="K5" s="11">
-        <v>9.2999999999999999E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -868,25 +868,25 @@
         <v>311</v>
       </c>
       <c r="E6" s="11">
-        <v>0.14099999999999999</v>
+        <v>0.113</v>
       </c>
       <c r="F6" s="4">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G6" s="11">
-        <v>5.8000000000000003E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="H6" s="4">
         <v>317</v>
       </c>
       <c r="I6" s="11">
-        <v>4.8000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="J6" s="4">
         <v>397</v>
       </c>
       <c r="K6" s="11">
-        <v>5.6000000000000001E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -900,28 +900,28 @@
         <v>3</v>
       </c>
       <c r="D7" s="4">
-        <v>3742</v>
+        <v>3822</v>
       </c>
       <c r="E7" s="11">
-        <v>2.0190000000000001</v>
+        <v>2.0859999999999999</v>
       </c>
       <c r="F7" s="4">
-        <v>4949</v>
+        <v>4763</v>
       </c>
       <c r="G7" s="11">
-        <v>2.4950000000000001</v>
+        <v>2.6480000000000001</v>
       </c>
       <c r="H7" s="4">
-        <v>5144</v>
+        <v>5140</v>
       </c>
       <c r="I7" s="11">
-        <v>2.5139999999999998</v>
+        <v>2.843</v>
       </c>
       <c r="J7" s="4">
-        <v>6216</v>
+        <v>6055</v>
       </c>
       <c r="K7" s="11">
-        <v>3.5819999999999999</v>
+        <v>3.8330000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -935,28 +935,28 @@
         <v>5</v>
       </c>
       <c r="D8" s="4">
-        <v>2040</v>
+        <v>2061</v>
       </c>
       <c r="E8" s="11">
-        <v>0.25</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F8" s="4">
-        <v>2611</v>
+        <v>2626</v>
       </c>
       <c r="G8" s="11">
-        <v>0.26400000000000001</v>
+        <v>0.40100000000000002</v>
       </c>
       <c r="H8" s="4">
-        <v>2284</v>
+        <v>2271</v>
       </c>
       <c r="I8" s="11">
-        <v>0.20300000000000001</v>
+        <v>0.222</v>
       </c>
       <c r="J8" s="4">
-        <v>2928</v>
+        <v>2981</v>
       </c>
       <c r="K8" s="11">
-        <v>0.36</v>
+        <v>0.36699999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -970,28 +970,28 @@
         <v>1.2</v>
       </c>
       <c r="D9" s="4">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="E9" s="11">
-        <v>0.16300000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="F9" s="4">
-        <v>567</v>
+        <v>500</v>
       </c>
       <c r="G9" s="11">
-        <v>0.109</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="H9" s="4">
         <v>745</v>
       </c>
       <c r="I9" s="11">
-        <v>0.123</v>
+        <v>0.127</v>
       </c>
       <c r="J9" s="4">
-        <v>510</v>
+        <v>601</v>
       </c>
       <c r="K9" s="11">
-        <v>0.113</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1008,25 +1008,25 @@
         <v>200</v>
       </c>
       <c r="E10" s="11">
-        <v>5.6000000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="F10" s="4">
         <v>207</v>
       </c>
       <c r="G10" s="11">
-        <v>2.9000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="H10" s="4">
         <v>213</v>
       </c>
       <c r="I10" s="11">
-        <v>2.7E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J10" s="4">
         <v>221</v>
       </c>
       <c r="K10" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1040,28 +1040,28 @@
         <v>5</v>
       </c>
       <c r="D11" s="4">
-        <v>9852</v>
+        <v>10055</v>
       </c>
       <c r="E11" s="11">
-        <v>2.6440000000000001</v>
+        <v>2.879</v>
       </c>
       <c r="F11" s="4">
-        <v>18626</v>
+        <v>18811</v>
       </c>
       <c r="G11" s="11">
-        <v>6.8090000000000002</v>
+        <v>7.54</v>
       </c>
       <c r="H11" s="4">
-        <v>10967</v>
+        <v>12458</v>
       </c>
       <c r="I11" s="11">
-        <v>3.9670000000000001</v>
+        <v>5.4349999999999996</v>
       </c>
       <c r="J11" s="4">
-        <v>21511</v>
+        <v>21397</v>
       </c>
       <c r="K11" s="11">
-        <v>8.4350000000000005</v>
+        <v>8.5030000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1078,25 +1078,25 @@
         <v>1211</v>
       </c>
       <c r="E12" s="11">
-        <v>0.10199999999999999</v>
+        <v>0.107</v>
       </c>
       <c r="F12" s="4">
         <v>1211</v>
       </c>
       <c r="G12" s="11">
-        <v>0.06</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="H12" s="4">
         <v>1211</v>
       </c>
       <c r="I12" s="11">
-        <v>0.06</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="J12" s="4">
         <v>1211</v>
       </c>
       <c r="K12" s="11">
-        <v>6.5000000000000002E-2</v>
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1110,28 +1110,28 @@
         <v>10</v>
       </c>
       <c r="D13" s="4">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="E13" s="11">
-        <v>0.17199999999999999</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="F13" s="3">
-        <v>1422</v>
+        <v>1412</v>
       </c>
       <c r="G13" s="11">
-        <v>0.17899999999999999</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="H13" s="4">
-        <v>1394</v>
+        <v>1396</v>
       </c>
       <c r="I13" s="11">
-        <v>0.14699999999999999</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="J13" s="4">
-        <v>1483</v>
+        <v>1487</v>
       </c>
       <c r="K13" s="11">
-        <v>0.191</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1145,28 +1145,28 @@
         <v>45</v>
       </c>
       <c r="D14" s="4">
-        <v>5808</v>
+        <v>5555</v>
       </c>
       <c r="E14" s="11">
-        <v>0.495</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="F14" s="3">
-        <v>5808</v>
+        <v>5555</v>
       </c>
       <c r="G14" s="11">
-        <v>0.4</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="H14" s="4">
-        <v>5808</v>
+        <v>5555</v>
       </c>
       <c r="I14" s="11">
-        <v>0.38300000000000001</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="J14" s="4">
-        <v>5808</v>
+        <v>5555</v>
       </c>
       <c r="K14" s="11">
-        <v>0.39500000000000002</v>
+        <v>0.26400000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1183,25 +1183,25 @@
         <v>732</v>
       </c>
       <c r="E15" s="11">
-        <v>0.113</v>
+        <v>0.121</v>
       </c>
       <c r="F15" s="3">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="G15" s="11">
-        <v>8.1000000000000003E-2</v>
+        <v>0.08</v>
       </c>
       <c r="H15" s="3">
         <v>807</v>
       </c>
       <c r="I15" s="11">
-        <v>7.0999999999999994E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J15" s="3">
-        <v>983</v>
+        <v>934</v>
       </c>
       <c r="K15" s="11">
-        <v>0.10199999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1218,25 +1218,25 @@
         <v>1305</v>
       </c>
       <c r="E16" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="F16" s="3">
         <v>1400</v>
       </c>
       <c r="G16" s="11">
-        <v>0.126</v>
+        <v>0.125</v>
       </c>
       <c r="H16" s="3">
         <v>1415</v>
       </c>
       <c r="I16" s="11">
-        <v>0.124</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="J16" s="3">
-        <v>1478</v>
+        <v>1443</v>
       </c>
       <c r="K16" s="11">
-        <v>0.13400000000000001</v>
+        <v>0.13300000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1250,28 +1250,28 @@
         <v>15</v>
       </c>
       <c r="D17" s="4">
-        <v>6337</v>
+        <v>6365</v>
       </c>
       <c r="E17" s="11">
-        <v>1.3520000000000001</v>
+        <v>1.2210000000000001</v>
       </c>
       <c r="F17" s="3">
-        <v>6769</v>
+        <v>6812</v>
       </c>
       <c r="G17" s="11">
-        <v>1.3839999999999999</v>
+        <v>1.3959999999999999</v>
       </c>
       <c r="H17" s="3">
-        <v>5922</v>
+        <v>6022</v>
       </c>
       <c r="I17" s="11">
-        <v>1.2889999999999999</v>
+        <v>1.32</v>
       </c>
       <c r="J17" s="3">
-        <v>6371</v>
+        <v>6420</v>
       </c>
       <c r="K17" s="11">
-        <v>1.6359999999999999</v>
+        <v>1.5740000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1291,22 +1291,22 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="F18" s="3">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="G18" s="11">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="H18" s="3">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="I18" s="11">
-        <v>7.1999999999999995E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="J18" s="3">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="K18" s="11">
-        <v>0.121</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1320,28 +1320,28 @@
         <v>30</v>
       </c>
       <c r="D19" s="4">
-        <v>3454</v>
+        <v>3432</v>
       </c>
       <c r="E19" s="11">
-        <v>0.90900000000000003</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="F19" s="3">
-        <v>3682</v>
+        <v>3708</v>
       </c>
       <c r="G19" s="11">
-        <v>0.748</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="H19" s="3">
-        <v>3499</v>
+        <v>3544</v>
       </c>
       <c r="I19" s="11">
-        <v>0.63800000000000001</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="J19" s="3">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="K19" s="11">
-        <v>0.83499999999999996</v>
+        <v>0.77400000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1355,28 +1355,28 @@
         <v>50</v>
       </c>
       <c r="D20" s="4">
-        <v>6945</v>
+        <v>7079</v>
       </c>
       <c r="E20" s="11">
-        <v>1.143</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="F20" s="3">
-        <v>7209</v>
+        <v>6970</v>
       </c>
       <c r="G20" s="11">
-        <v>1.05</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="H20" s="3">
-        <v>99540</v>
+        <v>97917</v>
       </c>
       <c r="I20" s="11">
-        <v>11.587999999999999</v>
+        <v>10.923999999999999</v>
       </c>
       <c r="J20" s="3">
-        <v>99405</v>
+        <v>99106</v>
       </c>
       <c r="K20" s="11">
-        <v>12.962999999999999</v>
+        <v>11.065</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1390,28 +1390,28 @@
         <v>30</v>
       </c>
       <c r="D21" s="4">
-        <v>3513</v>
+        <v>3637</v>
       </c>
       <c r="E21" s="11">
-        <v>0.45800000000000002</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="F21" s="3">
-        <v>4658</v>
+        <v>4600</v>
       </c>
       <c r="G21" s="11">
-        <v>0.63300000000000001</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="H21" s="3">
-        <v>4063</v>
+        <v>4076</v>
       </c>
       <c r="I21" s="11">
-        <v>0.48399999999999999</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="J21" s="3">
-        <v>4027</v>
+        <v>4188</v>
       </c>
       <c r="K21" s="11">
-        <v>0.46400000000000002</v>
+        <v>0.49399999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1425,28 +1425,28 @@
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <v>2318</v>
+        <v>2605</v>
       </c>
       <c r="E22" s="11">
-        <v>3.948</v>
+        <v>6.0039999999999996</v>
       </c>
       <c r="F22" s="3">
-        <v>2318</v>
+        <v>2605</v>
       </c>
       <c r="G22" s="11">
-        <v>3.524</v>
+        <v>6.14</v>
       </c>
       <c r="H22" s="3">
-        <v>2318</v>
+        <v>2605</v>
       </c>
       <c r="I22" s="11">
-        <v>3.536</v>
+        <v>5.9539999999999997</v>
       </c>
       <c r="J22" s="3">
-        <v>2318</v>
+        <v>2605</v>
       </c>
       <c r="K22" s="11">
-        <v>3.6930000000000001</v>
+        <v>6.0519999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1460,28 +1460,28 @@
         <v>15</v>
       </c>
       <c r="D23" s="4">
-        <v>3073</v>
+        <v>3132</v>
       </c>
       <c r="E23" s="11">
-        <v>1.0980000000000001</v>
+        <v>1.0740000000000001</v>
       </c>
       <c r="F23" s="3">
-        <v>3077</v>
+        <v>3111</v>
       </c>
       <c r="G23" s="11">
-        <v>1.1839999999999999</v>
+        <v>1.1830000000000001</v>
       </c>
       <c r="H23" s="3">
-        <v>3723</v>
+        <v>3782</v>
       </c>
       <c r="I23" s="11">
-        <v>1.4259999999999999</v>
+        <v>1.3720000000000001</v>
       </c>
       <c r="J23" s="3">
-        <v>3633</v>
+        <v>3676</v>
       </c>
       <c r="K23" s="11">
-        <v>1.4650000000000001</v>
+        <v>1.5680000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1498,25 +1498,25 @@
         <v>131</v>
       </c>
       <c r="E24" s="11">
-        <v>0.156</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="F24" s="3">
         <v>131</v>
       </c>
       <c r="G24" s="11">
-        <v>0.10299999999999999</v>
+        <v>0.11</v>
       </c>
       <c r="H24" s="3">
         <v>131</v>
       </c>
       <c r="I24" s="11">
-        <v>0.10100000000000001</v>
+        <v>0.107</v>
       </c>
       <c r="J24" s="3">
         <v>131</v>
       </c>
       <c r="K24" s="11">
-        <v>0.105</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1530,28 +1530,28 @@
         <v>30</v>
       </c>
       <c r="D25" s="4">
-        <v>4726</v>
+        <v>4741</v>
       </c>
       <c r="E25" s="11">
-        <v>3.9220000000000002</v>
+        <v>3.391</v>
       </c>
       <c r="F25" s="3">
-        <v>5178</v>
+        <v>5224</v>
       </c>
       <c r="G25" s="11">
-        <v>4.5709999999999997</v>
+        <v>4.2190000000000003</v>
       </c>
       <c r="H25" s="3">
-        <v>4554</v>
+        <v>4567</v>
       </c>
       <c r="I25" s="11">
-        <v>3.82</v>
+        <v>3.7229999999999999</v>
       </c>
       <c r="J25" s="3">
-        <v>5129</v>
+        <v>5136</v>
       </c>
       <c r="K25" s="11">
-        <v>4.4320000000000004</v>
+        <v>4.43</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1565,28 +1565,28 @@
         <v>12</v>
       </c>
       <c r="D26" s="4">
-        <v>13098</v>
+        <v>14378</v>
       </c>
       <c r="E26" s="11">
-        <v>6.81</v>
+        <v>7.3920000000000003</v>
       </c>
       <c r="F26" s="3">
-        <v>11877</v>
+        <v>14691</v>
       </c>
       <c r="G26" s="11">
-        <v>6.4649999999999999</v>
+        <v>8.6159999999999997</v>
       </c>
       <c r="H26" s="3">
-        <v>22049</v>
+        <v>18066</v>
       </c>
       <c r="I26" s="11">
-        <v>11.522</v>
+        <v>9.84</v>
       </c>
       <c r="J26" s="3">
-        <v>22779</v>
+        <v>19938</v>
       </c>
       <c r="K26" s="11">
-        <v>11.706</v>
+        <v>10.523999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1600,28 +1600,28 @@
         <v>20</v>
       </c>
       <c r="D27" s="9">
-        <v>3451</v>
+        <v>3317</v>
       </c>
       <c r="E27" s="11">
-        <v>2.222</v>
+        <v>2.0289999999999999</v>
       </c>
       <c r="F27" s="3">
-        <v>4110</v>
+        <v>4299</v>
       </c>
       <c r="G27" s="11">
-        <v>3.3980000000000001</v>
+        <v>3.899</v>
       </c>
       <c r="H27" s="3">
-        <v>3538</v>
+        <v>3428</v>
       </c>
       <c r="I27" s="11">
-        <v>2.2109999999999999</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="J27" s="3">
-        <v>5557</v>
+        <v>4426</v>
       </c>
       <c r="K27" s="11">
-        <v>6.1289999999999996</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1638,25 +1638,25 @@
         <v>940</v>
       </c>
       <c r="E28" s="11">
-        <v>0.154</v>
+        <v>0.157</v>
       </c>
       <c r="F28" s="3">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="G28" s="11">
-        <v>0.125</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="H28" s="3">
         <v>967</v>
       </c>
       <c r="I28" s="11">
-        <v>0.11700000000000001</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="J28" s="3">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="K28" s="11">
-        <v>0.129</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1673,25 +1673,25 @@
         <v>710</v>
       </c>
       <c r="E29" s="11">
-        <v>0.14099999999999999</v>
+        <v>0.153</v>
       </c>
       <c r="F29" s="3">
         <v>833</v>
       </c>
       <c r="G29" s="11">
-        <v>0.13700000000000001</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="H29" s="3">
         <v>747</v>
       </c>
       <c r="I29" s="11">
-        <v>0.11799999999999999</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="J29" s="3">
-        <v>860</v>
+        <v>850</v>
       </c>
       <c r="K29" s="11">
-        <v>0.16</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1708,25 +1708,25 @@
         <v>10343</v>
       </c>
       <c r="E30" s="11">
-        <v>13.141</v>
+        <v>12.298999999999999</v>
       </c>
       <c r="F30" s="3">
-        <v>12272</v>
+        <v>12202</v>
       </c>
       <c r="G30" s="11">
-        <v>25.661999999999999</v>
+        <v>24.783000000000001</v>
       </c>
       <c r="H30" s="3">
-        <v>11659</v>
+        <v>11671</v>
       </c>
       <c r="I30" s="11">
-        <v>19.334</v>
+        <v>19.189</v>
       </c>
       <c r="J30" s="3">
-        <v>21192</v>
+        <v>13423</v>
       </c>
       <c r="K30" s="11">
-        <v>89.869</v>
+        <v>34.979999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1743,22 +1743,22 @@
         <v>663</v>
       </c>
       <c r="E31" s="11">
-        <v>0.16</v>
+        <v>0.161</v>
       </c>
       <c r="F31" s="3">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="G31" s="11">
-        <v>0.192</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="H31" s="3">
-        <v>660</v>
+        <v>668</v>
       </c>
       <c r="I31" s="11">
-        <v>0.108</v>
+        <v>0.109</v>
       </c>
       <c r="J31" s="3">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="K31" s="11">
         <v>0.19700000000000001</v>
@@ -1778,25 +1778,25 @@
         <v>2422</v>
       </c>
       <c r="E32" s="11">
-        <v>1.268</v>
+        <v>1.296</v>
       </c>
       <c r="F32" s="3">
-        <v>5303</v>
+        <v>5269</v>
       </c>
       <c r="G32" s="11">
-        <v>8.8840000000000003</v>
+        <v>7.92</v>
       </c>
       <c r="H32" s="3">
         <v>2512</v>
       </c>
       <c r="I32" s="11">
-        <v>1.306</v>
+        <v>1.347</v>
       </c>
       <c r="J32" s="3">
-        <v>6180</v>
+        <v>5544</v>
       </c>
       <c r="K32" s="11">
-        <v>12.259</v>
+        <v>9.5009999999999994</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1810,28 +1810,28 @@
         <v>10</v>
       </c>
       <c r="D33" s="4">
-        <v>2635</v>
+        <v>2657</v>
       </c>
       <c r="E33" s="11">
-        <v>0.79</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="F33" s="3">
-        <v>4096</v>
+        <v>4038</v>
       </c>
       <c r="G33" s="11">
-        <v>1.296</v>
+        <v>1.101</v>
       </c>
       <c r="H33" s="3">
-        <v>3029</v>
+        <v>3047</v>
       </c>
       <c r="I33" s="11">
-        <v>0.65700000000000003</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="J33" s="3">
-        <v>4353</v>
+        <v>4400</v>
       </c>
       <c r="K33" s="11">
-        <v>1.2609999999999999</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1845,28 +1845,28 @@
         <v>3</v>
       </c>
       <c r="D34" s="4">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E34" s="11">
-        <v>0.14099999999999999</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="F34" s="3">
-        <v>758</v>
+        <v>745</v>
       </c>
       <c r="G34" s="11">
-        <v>0.39300000000000002</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="H34" s="3">
-        <v>481</v>
+        <v>505</v>
       </c>
       <c r="I34" s="11">
-        <v>0.114</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="J34" s="3">
-        <v>868</v>
+        <v>846</v>
       </c>
       <c r="K34" s="11">
-        <v>0.38200000000000001</v>
+        <v>0.42199999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1883,25 +1883,25 @@
         <v>1667</v>
       </c>
       <c r="E35" s="11">
-        <v>0.29599999999999999</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="F35" s="3">
-        <v>3127</v>
+        <v>3138</v>
       </c>
       <c r="G35" s="11">
-        <v>0.98499999999999999</v>
+        <v>1.125</v>
       </c>
       <c r="H35" s="3">
-        <v>1739</v>
+        <v>1673</v>
       </c>
       <c r="I35" s="11">
-        <v>0.29399999999999998</v>
+        <v>0.251</v>
       </c>
       <c r="J35" s="3">
-        <v>3225</v>
+        <v>3202</v>
       </c>
       <c r="K35" s="11">
-        <v>0.92700000000000005</v>
+        <v>1.0329999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1915,28 +1915,28 @@
         <v>36</v>
       </c>
       <c r="D36" s="4">
-        <v>4473</v>
+        <v>4561</v>
       </c>
       <c r="E36" s="11">
-        <v>0.96899999999999997</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="F36" s="3">
-        <v>6767</v>
+        <v>6856</v>
       </c>
       <c r="G36" s="11">
-        <v>2.17</v>
+        <v>2.3969999999999998</v>
       </c>
       <c r="H36" s="3">
-        <v>4576</v>
+        <v>4552</v>
       </c>
       <c r="I36" s="11">
-        <v>0.93200000000000005</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="J36" s="3">
-        <v>6779</v>
+        <v>6916</v>
       </c>
       <c r="K36" s="11">
-        <v>2.4590000000000001</v>
+        <v>2.496</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1953,25 +1953,25 @@
         <v>5619</v>
       </c>
       <c r="E37" s="11">
-        <v>0.78700000000000003</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="F37" s="3">
-        <v>8361</v>
+        <v>8257</v>
       </c>
       <c r="G37" s="11">
-        <v>2.6819999999999999</v>
+        <v>2.6059999999999999</v>
       </c>
       <c r="H37" s="3">
         <v>5671</v>
       </c>
       <c r="I37" s="11">
-        <v>0.70599999999999996</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="J37" s="3">
-        <v>8452</v>
+        <v>8335</v>
       </c>
       <c r="K37" s="11">
-        <v>3.0310000000000001</v>
+        <v>2.6389999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1988,25 +1988,25 @@
         <v>4175</v>
       </c>
       <c r="E38" s="11">
-        <v>1.1879999999999999</v>
+        <v>1.1459999999999999</v>
       </c>
       <c r="F38" s="3">
-        <v>4632</v>
+        <v>4671</v>
       </c>
       <c r="G38" s="11">
-        <v>1.7529999999999999</v>
+        <v>1.6919999999999999</v>
       </c>
       <c r="H38" s="3">
         <v>4256</v>
       </c>
       <c r="I38" s="11">
-        <v>1.23</v>
+        <v>1.2869999999999999</v>
       </c>
       <c r="J38" s="3">
-        <v>4807</v>
+        <v>4800</v>
       </c>
       <c r="K38" s="11">
-        <v>1.974</v>
+        <v>2.0209999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2020,28 +2020,28 @@
         <v>40</v>
       </c>
       <c r="D39" s="4">
-        <v>4964</v>
+        <v>4912</v>
       </c>
       <c r="E39" s="11">
-        <v>0.64400000000000002</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="F39" s="3">
-        <v>5451</v>
+        <v>5407</v>
       </c>
       <c r="G39" s="11">
-        <v>0.94799999999999995</v>
+        <v>0.871</v>
       </c>
       <c r="H39" s="3">
-        <v>4879</v>
+        <v>4945</v>
       </c>
       <c r="I39" s="11">
-        <v>0.63</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="J39" s="3">
-        <v>5234</v>
+        <v>5196</v>
       </c>
       <c r="K39" s="11">
-        <v>0.81399999999999995</v>
+        <v>0.82299999999999995</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2055,28 +2055,28 @@
         <v>36</v>
       </c>
       <c r="D40" s="4">
-        <v>4175</v>
+        <v>4044</v>
       </c>
       <c r="E40" s="11">
-        <v>1.9450000000000001</v>
+        <v>1.6359999999999999</v>
       </c>
       <c r="F40" s="3">
-        <v>4596</v>
+        <v>4529</v>
       </c>
       <c r="G40" s="11">
-        <v>2.6480000000000001</v>
+        <v>2.7120000000000002</v>
       </c>
       <c r="H40" s="3">
-        <v>4185</v>
+        <v>4143</v>
       </c>
       <c r="I40" s="11">
-        <v>2.181</v>
+        <v>1.899</v>
       </c>
       <c r="J40" s="3">
-        <v>4635</v>
+        <v>4629</v>
       </c>
       <c r="K40" s="11">
-        <v>3.012</v>
+        <v>2.7330000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2093,25 +2093,25 @@
         <v>4601</v>
       </c>
       <c r="E41" s="11">
-        <v>1.361</v>
+        <v>1.387</v>
       </c>
       <c r="F41" s="3">
-        <v>4556</v>
+        <v>4611</v>
       </c>
       <c r="G41" s="11">
-        <v>1.8939999999999999</v>
+        <v>1.9239999999999999</v>
       </c>
       <c r="H41" s="3">
-        <v>4746</v>
+        <v>4745</v>
       </c>
       <c r="I41" s="11">
-        <v>1.7090000000000001</v>
+        <v>1.5880000000000001</v>
       </c>
       <c r="J41" s="3">
-        <v>4615</v>
+        <v>4587</v>
       </c>
       <c r="K41" s="11">
-        <v>2.0249999999999999</v>
+        <v>1.881</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2128,25 +2128,25 @@
         <v>6024</v>
       </c>
       <c r="E42" s="11">
-        <v>0.93600000000000005</v>
+        <v>0.86</v>
       </c>
       <c r="F42" s="3">
-        <v>6475</v>
+        <v>6434</v>
       </c>
       <c r="G42" s="11">
-        <v>1.177</v>
+        <v>1.159</v>
       </c>
       <c r="H42" s="3">
         <v>6388</v>
       </c>
       <c r="I42" s="11">
-        <v>0.96399999999999997</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="J42" s="3">
-        <v>6781</v>
+        <v>6734</v>
       </c>
       <c r="K42" s="11">
-        <v>1.3759999999999999</v>
+        <v>1.1879999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2163,25 +2163,25 @@
         <v>1231</v>
       </c>
       <c r="E43" s="11">
-        <v>0.29899999999999999</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="F43" s="3">
         <v>1385</v>
       </c>
       <c r="G43" s="11">
-        <v>0.5</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="H43" s="3">
         <v>1249</v>
       </c>
       <c r="I43" s="11">
-        <v>0.26100000000000001</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="J43" s="3">
         <v>1503</v>
       </c>
       <c r="K43" s="11">
-        <v>0.45</v>
+        <v>0.49099999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2195,28 +2195,28 @@
         <v>24</v>
       </c>
       <c r="D44" s="4">
-        <v>7839</v>
+        <v>7808</v>
       </c>
       <c r="E44" s="11">
-        <v>4.7089999999999996</v>
+        <v>4.1449999999999996</v>
       </c>
       <c r="F44" s="3">
-        <v>6402</v>
+        <v>6527</v>
       </c>
       <c r="G44" s="11">
-        <v>6.3289999999999997</v>
+        <v>5.8209999999999997</v>
       </c>
       <c r="H44" s="3">
-        <v>8393</v>
+        <v>7920</v>
       </c>
       <c r="I44" s="11">
-        <v>4.9640000000000004</v>
+        <v>4.6989999999999998</v>
       </c>
       <c r="J44" s="3">
-        <v>6653</v>
+        <v>6644</v>
       </c>
       <c r="K44" s="11">
-        <v>6.4619999999999997</v>
+        <v>6.2869999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2230,28 +2230,28 @@
         <v>30</v>
       </c>
       <c r="D45" s="4">
-        <v>4789</v>
+        <v>4923</v>
       </c>
       <c r="E45" s="11">
-        <v>4.7160000000000002</v>
+        <v>5.5469999999999997</v>
       </c>
       <c r="F45" s="3">
-        <v>4789</v>
+        <v>4923</v>
       </c>
       <c r="G45" s="11">
-        <v>4.5110000000000001</v>
+        <v>5.4329999999999998</v>
       </c>
       <c r="H45" s="3">
-        <v>4789</v>
+        <v>4923</v>
       </c>
       <c r="I45" s="11">
-        <v>4.899</v>
+        <v>5.5490000000000004</v>
       </c>
       <c r="J45" s="3">
-        <v>4789</v>
+        <v>4923</v>
       </c>
       <c r="K45" s="11">
-        <v>4.5019999999999998</v>
+        <v>5.5339999999999998</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2265,28 +2265,28 @@
         <v>8.5</v>
       </c>
       <c r="D46" s="4">
-        <v>2565</v>
+        <v>2551</v>
       </c>
       <c r="E46" s="11">
-        <v>18.984000000000002</v>
+        <v>19.486000000000001</v>
       </c>
       <c r="F46" s="3">
-        <v>2565</v>
+        <v>2551</v>
       </c>
       <c r="G46" s="11">
-        <v>19.010999999999999</v>
+        <v>19.513000000000002</v>
       </c>
       <c r="H46" s="3">
-        <v>2565</v>
+        <v>2551</v>
       </c>
       <c r="I46" s="11">
-        <v>18.683</v>
+        <v>18.972999999999999</v>
       </c>
       <c r="J46" s="3">
-        <v>2565</v>
+        <v>2551</v>
       </c>
       <c r="K46" s="11">
-        <v>18.646000000000001</v>
+        <v>18.916</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2300,10 +2300,10 @@
         <v>33.72</v>
       </c>
       <c r="D47" s="4">
-        <v>8673</v>
+        <v>8965</v>
       </c>
       <c r="E47" s="11">
-        <v>4.2709999999999999</v>
+        <v>4.1440000000000001</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>44</v>
@@ -2335,10 +2335,10 @@
         <v>32.19</v>
       </c>
       <c r="D48" s="4">
-        <v>8919</v>
+        <v>8747</v>
       </c>
       <c r="E48" s="11">
-        <v>5.3570000000000002</v>
+        <v>5.4039999999999999</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>44</v>
@@ -2370,10 +2370,10 @@
         <v>59.18</v>
       </c>
       <c r="D49" s="4">
-        <v>15052</v>
+        <v>15010</v>
       </c>
       <c r="E49" s="11">
-        <v>10.231999999999999</v>
+        <v>10.494999999999999</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>44</v>
@@ -2405,10 +2405,10 @@
         <v>39.020000000000003</v>
       </c>
       <c r="D50" s="4">
-        <v>11289</v>
+        <v>11170</v>
       </c>
       <c r="E50" s="11">
-        <v>8.1929999999999996</v>
+        <v>7.5449999999999999</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>44</v>
@@ -2437,13 +2437,13 @@
         <v>48</v>
       </c>
       <c r="C51" s="11">
-        <v>34.659999999999997</v>
+        <v>34.69</v>
       </c>
       <c r="D51" s="4">
-        <v>8973</v>
+        <v>9292</v>
       </c>
       <c r="E51" s="11">
-        <v>5.26</v>
+        <v>5.298</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>44</v>
@@ -2472,13 +2472,13 @@
         <v>49</v>
       </c>
       <c r="C52" s="11">
-        <v>40.82</v>
+        <v>40.86</v>
       </c>
       <c r="D52" s="4">
-        <v>11694</v>
+        <v>11807</v>
       </c>
       <c r="E52" s="11">
-        <v>11.776999999999999</v>
+        <v>10.874000000000001</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>44</v>
@@ -2510,10 +2510,10 @@
         <v>41.28</v>
       </c>
       <c r="D53" s="2">
-        <v>11318</v>
+        <v>11580</v>
       </c>
       <c r="E53" s="11">
-        <v>8.3559999999999999</v>
+        <v>8.1509999999999998</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>44</v>
@@ -2545,10 +2545,10 @@
         <v>45.28</v>
       </c>
       <c r="D54" s="2">
-        <v>12142</v>
+        <v>11898</v>
       </c>
       <c r="E54" s="11">
-        <v>13.596</v>
+        <v>13.010999999999999</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>44</v>
@@ -2580,10 +2580,10 @@
         <v>27.71</v>
       </c>
       <c r="D55" s="2">
-        <v>8758</v>
+        <v>9000</v>
       </c>
       <c r="E55" s="11">
-        <v>9.5679999999999996</v>
+        <v>8.3710000000000004</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>44</v>
@@ -2618,17 +2618,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100525B94EEF47D42499A62120CC90E0AB3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e706cd362d7e41030bb8c72a7c62a9d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c85acdc-a394-4ae0-8c72-fb4a95b3d573" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55e2521e7df4d5c11309cefaa7c01562" ns2:_="">
     <xsd:import namespace="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
@@ -2773,16 +2762,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2828,10 +2819,29 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2853,35 +2863,25 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE6D0D52-57FE-48CB-8E43-11384E6CFEE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630E037-F79E-4175-B540-A23B306F8900}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE6D0D52-57FE-48CB-8E43-11384E6CFEE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Initial commit R2016b.  Version 4.1
</commit_message>
<xml_diff>
--- a/Scripts_Data/CFR_Results.xlsx
+++ b/Scripts_Data/CFR_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R16a\Scripts_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R16b\Scripts_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -213,10 +213,10 @@
     <t>CFL v4.0</t>
   </si>
   <si>
-    <t>9.0.0.341360 (R2016a)</t>
-  </si>
-  <si>
-    <t>09-Mar-2018 10:12:47</t>
+    <t>9.1.0.441655 (R2016b)</t>
+  </si>
+  <si>
+    <t>09-Mar-2018 07:57:04</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,28 +795,28 @@
         <v>6</v>
       </c>
       <c r="D4" s="15">
-        <v>2387</v>
+        <v>2400</v>
       </c>
       <c r="E4" s="14">
-        <v>0.26400000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="F4" s="15">
-        <v>2387</v>
+        <v>2400</v>
       </c>
       <c r="G4" s="14">
-        <v>0.17</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="H4" s="15">
-        <v>2387</v>
+        <v>2400</v>
       </c>
       <c r="I4" s="14">
-        <v>0.18099999999999999</v>
+        <v>0.156</v>
       </c>
       <c r="J4" s="15">
-        <v>2387</v>
+        <v>2400</v>
       </c>
       <c r="K4" s="14">
-        <v>0.17499999999999999</v>
+        <v>0.17100000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -833,25 +833,25 @@
         <v>674</v>
       </c>
       <c r="E5" s="11">
-        <v>9.0999999999999998E-2</v>
+        <v>0.15</v>
       </c>
       <c r="F5" s="4">
         <v>959</v>
       </c>
       <c r="G5" s="11">
-        <v>8.5999999999999993E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="H5" s="4">
         <v>731</v>
       </c>
       <c r="I5" s="11">
-        <v>5.7000000000000002E-2</v>
+        <v>0.06</v>
       </c>
       <c r="J5" s="4">
         <v>1028</v>
       </c>
       <c r="K5" s="11">
-        <v>9.8000000000000004E-2</v>
+        <v>9.4E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -868,25 +868,25 @@
         <v>311</v>
       </c>
       <c r="E6" s="11">
-        <v>0.113</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="F6" s="4">
         <v>366</v>
       </c>
       <c r="G6" s="11">
-        <v>7.5999999999999998E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="H6" s="4">
         <v>317</v>
       </c>
       <c r="I6" s="11">
-        <v>4.9000000000000002E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="J6" s="4">
         <v>397</v>
       </c>
       <c r="K6" s="11">
-        <v>5.8999999999999997E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -900,28 +900,28 @@
         <v>3</v>
       </c>
       <c r="D7" s="4">
-        <v>3822</v>
+        <v>3805</v>
       </c>
       <c r="E7" s="11">
-        <v>2.0859999999999999</v>
+        <v>1.863</v>
       </c>
       <c r="F7" s="4">
-        <v>4763</v>
+        <v>4908</v>
       </c>
       <c r="G7" s="11">
-        <v>2.6480000000000001</v>
+        <v>2.5619999999999998</v>
       </c>
       <c r="H7" s="4">
-        <v>5140</v>
+        <v>4676</v>
       </c>
       <c r="I7" s="11">
-        <v>2.843</v>
+        <v>2.4359999999999999</v>
       </c>
       <c r="J7" s="4">
-        <v>6055</v>
+        <v>6075</v>
       </c>
       <c r="K7" s="11">
-        <v>3.8330000000000002</v>
+        <v>3.4780000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -935,28 +935,28 @@
         <v>5</v>
       </c>
       <c r="D8" s="4">
-        <v>2061</v>
+        <v>2040</v>
       </c>
       <c r="E8" s="11">
-        <v>0.22900000000000001</v>
+        <v>0.307</v>
       </c>
       <c r="F8" s="4">
-        <v>2626</v>
+        <v>2667</v>
       </c>
       <c r="G8" s="11">
-        <v>0.40100000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="H8" s="4">
-        <v>2271</v>
+        <v>2284</v>
       </c>
       <c r="I8" s="11">
-        <v>0.222</v>
+        <v>0.21</v>
       </c>
       <c r="J8" s="4">
-        <v>2981</v>
+        <v>2900</v>
       </c>
       <c r="K8" s="11">
-        <v>0.36699999999999999</v>
+        <v>0.313</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -973,13 +973,13 @@
         <v>616</v>
       </c>
       <c r="E9" s="11">
-        <v>0.17199999999999999</v>
+        <v>0.158</v>
       </c>
       <c r="F9" s="4">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="G9" s="11">
-        <v>9.0999999999999998E-2</v>
+        <v>0.122</v>
       </c>
       <c r="H9" s="4">
         <v>745</v>
@@ -988,10 +988,10 @@
         <v>0.127</v>
       </c>
       <c r="J9" s="4">
-        <v>601</v>
+        <v>616</v>
       </c>
       <c r="K9" s="11">
-        <v>0.121</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1008,25 +1008,25 @@
         <v>200</v>
       </c>
       <c r="E10" s="11">
-        <v>5.7000000000000002E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="F10" s="4">
         <v>207</v>
       </c>
       <c r="G10" s="11">
-        <v>0.03</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="H10" s="4">
         <v>213</v>
       </c>
       <c r="I10" s="11">
-        <v>0.03</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="J10" s="4">
         <v>221</v>
       </c>
       <c r="K10" s="11">
-        <v>4.2000000000000003E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1043,25 +1043,25 @@
         <v>10055</v>
       </c>
       <c r="E11" s="11">
-        <v>2.879</v>
+        <v>3.1349999999999998</v>
       </c>
       <c r="F11" s="4">
-        <v>18811</v>
+        <v>18721</v>
       </c>
       <c r="G11" s="11">
-        <v>7.54</v>
+        <v>6.9119999999999999</v>
       </c>
       <c r="H11" s="4">
         <v>12458</v>
       </c>
       <c r="I11" s="11">
-        <v>5.4349999999999996</v>
+        <v>4.673</v>
       </c>
       <c r="J11" s="4">
-        <v>21397</v>
+        <v>21338</v>
       </c>
       <c r="K11" s="11">
-        <v>8.5030000000000001</v>
+        <v>8.7789999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1078,25 +1078,25 @@
         <v>1211</v>
       </c>
       <c r="E12" s="11">
-        <v>0.107</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="F12" s="4">
         <v>1211</v>
       </c>
       <c r="G12" s="11">
-        <v>6.0999999999999999E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="H12" s="4">
         <v>1211</v>
       </c>
       <c r="I12" s="11">
-        <v>6.0999999999999999E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="J12" s="4">
         <v>1211</v>
       </c>
       <c r="K12" s="11">
-        <v>6.2E-2</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1113,25 +1113,25 @@
         <v>1301</v>
       </c>
       <c r="E13" s="11">
-        <v>0.17299999999999999</v>
+        <v>0.184</v>
       </c>
       <c r="F13" s="3">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="G13" s="11">
-        <v>0.17699999999999999</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="H13" s="4">
         <v>1396</v>
       </c>
       <c r="I13" s="11">
-        <v>0.14599999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="J13" s="4">
-        <v>1487</v>
+        <v>1476</v>
       </c>
       <c r="K13" s="11">
-        <v>0.183</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1145,25 +1145,25 @@
         <v>45</v>
       </c>
       <c r="D14" s="4">
-        <v>5555</v>
+        <v>5538</v>
       </c>
       <c r="E14" s="11">
-        <v>0.38800000000000001</v>
+        <v>0.378</v>
       </c>
       <c r="F14" s="3">
-        <v>5555</v>
+        <v>5538</v>
       </c>
       <c r="G14" s="11">
-        <v>0.25900000000000001</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="H14" s="4">
-        <v>5555</v>
+        <v>5538</v>
       </c>
       <c r="I14" s="11">
-        <v>0.25800000000000001</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="J14" s="4">
-        <v>5555</v>
+        <v>5538</v>
       </c>
       <c r="K14" s="11">
         <v>0.26400000000000001</v>
@@ -1183,25 +1183,25 @@
         <v>732</v>
       </c>
       <c r="E15" s="11">
-        <v>0.121</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="F15" s="3">
         <v>859</v>
       </c>
       <c r="G15" s="11">
-        <v>0.08</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="H15" s="3">
         <v>807</v>
       </c>
       <c r="I15" s="11">
-        <v>7.0000000000000007E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="J15" s="3">
         <v>934</v>
       </c>
       <c r="K15" s="11">
-        <v>8.7999999999999995E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1218,25 +1218,25 @@
         <v>1305</v>
       </c>
       <c r="E16" s="11">
-        <v>0.13900000000000001</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="F16" s="3">
         <v>1400</v>
       </c>
       <c r="G16" s="11">
-        <v>0.125</v>
+        <v>0.126</v>
       </c>
       <c r="H16" s="3">
         <v>1415</v>
       </c>
       <c r="I16" s="11">
-        <v>0.11600000000000001</v>
+        <v>0.121</v>
       </c>
       <c r="J16" s="3">
         <v>1443</v>
       </c>
       <c r="K16" s="11">
-        <v>0.13300000000000001</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1253,25 +1253,25 @@
         <v>6365</v>
       </c>
       <c r="E17" s="11">
-        <v>1.2210000000000001</v>
+        <v>1.204</v>
       </c>
       <c r="F17" s="3">
         <v>6812</v>
       </c>
       <c r="G17" s="11">
-        <v>1.3959999999999999</v>
+        <v>1.4119999999999999</v>
       </c>
       <c r="H17" s="3">
         <v>6022</v>
       </c>
       <c r="I17" s="11">
-        <v>1.32</v>
+        <v>1.3069999999999999</v>
       </c>
       <c r="J17" s="3">
         <v>6420</v>
       </c>
       <c r="K17" s="11">
-        <v>1.5740000000000001</v>
+        <v>1.4750000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1294,19 +1294,19 @@
         <v>307</v>
       </c>
       <c r="G18" s="11">
-        <v>5.8000000000000003E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="H18" s="3">
         <v>314</v>
       </c>
       <c r="I18" s="11">
-        <v>5.7000000000000002E-2</v>
+        <v>0.06</v>
       </c>
       <c r="J18" s="3">
         <v>334</v>
       </c>
       <c r="K18" s="11">
-        <v>6.7000000000000004E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1323,25 +1323,25 @@
         <v>3432</v>
       </c>
       <c r="E19" s="11">
-        <v>0.67900000000000005</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="F19" s="3">
-        <v>3708</v>
+        <v>3672</v>
       </c>
       <c r="G19" s="11">
-        <v>0.71899999999999997</v>
+        <v>0.7</v>
       </c>
       <c r="H19" s="3">
         <v>3544</v>
       </c>
       <c r="I19" s="11">
-        <v>0.63300000000000001</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="J19" s="3">
-        <v>3834</v>
+        <v>3829</v>
       </c>
       <c r="K19" s="11">
-        <v>0.77400000000000002</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1355,28 +1355,28 @@
         <v>50</v>
       </c>
       <c r="D20" s="4">
-        <v>7079</v>
+        <v>6974</v>
       </c>
       <c r="E20" s="11">
-        <v>0.88100000000000001</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="F20" s="3">
-        <v>6970</v>
+        <v>6688</v>
       </c>
       <c r="G20" s="11">
-        <v>0.88400000000000001</v>
+        <v>0.74</v>
       </c>
       <c r="H20" s="3">
-        <v>97917</v>
+        <v>98588</v>
       </c>
       <c r="I20" s="11">
-        <v>10.923999999999999</v>
+        <v>10.592000000000001</v>
       </c>
       <c r="J20" s="3">
-        <v>99106</v>
+        <v>99644</v>
       </c>
       <c r="K20" s="11">
-        <v>11.065</v>
+        <v>10.602</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1393,25 +1393,25 @@
         <v>3637</v>
       </c>
       <c r="E21" s="11">
-        <v>0.66500000000000004</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="F21" s="3">
-        <v>4600</v>
+        <v>4630</v>
       </c>
       <c r="G21" s="11">
-        <v>0.64800000000000002</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="H21" s="3">
         <v>4076</v>
       </c>
       <c r="I21" s="11">
-        <v>0.45500000000000002</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="J21" s="3">
-        <v>4188</v>
+        <v>4180</v>
       </c>
       <c r="K21" s="11">
-        <v>0.49399999999999999</v>
+        <v>0.47799999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1425,28 +1425,28 @@
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <v>2605</v>
+        <v>2138</v>
       </c>
       <c r="E22" s="11">
-        <v>6.0039999999999996</v>
+        <v>4.5529999999999999</v>
       </c>
       <c r="F22" s="3">
-        <v>2605</v>
+        <v>2138</v>
       </c>
       <c r="G22" s="11">
-        <v>6.14</v>
+        <v>4.819</v>
       </c>
       <c r="H22" s="3">
-        <v>2605</v>
+        <v>2138</v>
       </c>
       <c r="I22" s="11">
-        <v>5.9539999999999997</v>
+        <v>4.625</v>
       </c>
       <c r="J22" s="3">
-        <v>2605</v>
+        <v>2138</v>
       </c>
       <c r="K22" s="11">
-        <v>6.0519999999999996</v>
+        <v>4.5789999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1463,13 +1463,13 @@
         <v>3132</v>
       </c>
       <c r="E23" s="11">
-        <v>1.0740000000000001</v>
+        <v>1.298</v>
       </c>
       <c r="F23" s="3">
         <v>3111</v>
       </c>
       <c r="G23" s="11">
-        <v>1.1830000000000001</v>
+        <v>1.1890000000000001</v>
       </c>
       <c r="H23" s="3">
         <v>3782</v>
@@ -1481,7 +1481,7 @@
         <v>3676</v>
       </c>
       <c r="K23" s="11">
-        <v>1.5680000000000001</v>
+        <v>1.3919999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1498,7 +1498,7 @@
         <v>131</v>
       </c>
       <c r="E24" s="11">
-        <v>0.17399999999999999</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="F24" s="3">
         <v>131</v>
@@ -1510,13 +1510,13 @@
         <v>131</v>
       </c>
       <c r="I24" s="11">
-        <v>0.107</v>
+        <v>0.111</v>
       </c>
       <c r="J24" s="3">
         <v>131</v>
       </c>
       <c r="K24" s="11">
-        <v>0.111</v>
+        <v>0.10199999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1533,25 +1533,25 @@
         <v>4741</v>
       </c>
       <c r="E25" s="11">
-        <v>3.391</v>
+        <v>3.5289999999999999</v>
       </c>
       <c r="F25" s="3">
         <v>5224</v>
       </c>
       <c r="G25" s="11">
-        <v>4.2190000000000003</v>
+        <v>4.3760000000000003</v>
       </c>
       <c r="H25" s="3">
         <v>4567</v>
       </c>
       <c r="I25" s="11">
-        <v>3.7229999999999999</v>
+        <v>3.7530000000000001</v>
       </c>
       <c r="J25" s="3">
         <v>5136</v>
       </c>
       <c r="K25" s="11">
-        <v>4.43</v>
+        <v>4.4459999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1565,28 +1565,28 @@
         <v>12</v>
       </c>
       <c r="D26" s="4">
-        <v>14378</v>
+        <v>13792</v>
       </c>
       <c r="E26" s="11">
-        <v>7.3920000000000003</v>
+        <v>7.2080000000000002</v>
       </c>
       <c r="F26" s="3">
-        <v>14691</v>
+        <v>14308</v>
       </c>
       <c r="G26" s="11">
-        <v>8.6159999999999997</v>
+        <v>7.3949999999999996</v>
       </c>
       <c r="H26" s="3">
-        <v>18066</v>
+        <v>19430</v>
       </c>
       <c r="I26" s="11">
-        <v>9.84</v>
+        <v>10.407999999999999</v>
       </c>
       <c r="J26" s="3">
-        <v>19938</v>
+        <v>23305</v>
       </c>
       <c r="K26" s="11">
-        <v>10.523999999999999</v>
+        <v>12.148</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1600,28 +1600,28 @@
         <v>20</v>
       </c>
       <c r="D27" s="9">
-        <v>3317</v>
+        <v>3423</v>
       </c>
       <c r="E27" s="11">
-        <v>2.0289999999999999</v>
+        <v>2.1829999999999998</v>
       </c>
       <c r="F27" s="3">
-        <v>4299</v>
+        <v>4110</v>
       </c>
       <c r="G27" s="11">
-        <v>3.899</v>
+        <v>3.218</v>
       </c>
       <c r="H27" s="3">
-        <v>3428</v>
+        <v>3479</v>
       </c>
       <c r="I27" s="11">
-        <v>2.0499999999999998</v>
+        <v>2.077</v>
       </c>
       <c r="J27" s="3">
-        <v>4426</v>
+        <v>4217</v>
       </c>
       <c r="K27" s="11">
-        <v>3.64</v>
+        <v>3.1760000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1638,25 +1638,25 @@
         <v>940</v>
       </c>
       <c r="E28" s="11">
-        <v>0.157</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="F28" s="3">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="G28" s="11">
-        <v>0.11700000000000001</v>
+        <v>0.124</v>
       </c>
       <c r="H28" s="3">
         <v>967</v>
       </c>
       <c r="I28" s="11">
-        <v>9.8000000000000004E-2</v>
+        <v>0.106</v>
       </c>
       <c r="J28" s="3">
         <v>1060</v>
       </c>
       <c r="K28" s="11">
-        <v>0.13200000000000001</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1673,25 +1673,25 @@
         <v>710</v>
       </c>
       <c r="E29" s="11">
-        <v>0.153</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="F29" s="3">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="G29" s="11">
-        <v>0.14499999999999999</v>
+        <v>0.126</v>
       </c>
       <c r="H29" s="3">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="I29" s="11">
-        <v>0.16600000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="J29" s="3">
-        <v>850</v>
+        <v>856</v>
       </c>
       <c r="K29" s="11">
-        <v>0.156</v>
+        <v>0.16200000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1705,28 +1705,28 @@
         <v>20</v>
       </c>
       <c r="D30" s="4">
-        <v>10343</v>
+        <v>10344</v>
       </c>
       <c r="E30" s="11">
-        <v>12.298999999999999</v>
+        <v>11.092000000000001</v>
       </c>
       <c r="F30" s="3">
-        <v>12202</v>
+        <v>12311</v>
       </c>
       <c r="G30" s="11">
-        <v>24.783000000000001</v>
+        <v>24.744</v>
       </c>
       <c r="H30" s="3">
-        <v>11671</v>
+        <v>11682</v>
       </c>
       <c r="I30" s="11">
-        <v>19.189</v>
+        <v>17.956</v>
       </c>
       <c r="J30" s="3">
-        <v>13423</v>
+        <v>13340</v>
       </c>
       <c r="K30" s="11">
-        <v>34.979999999999997</v>
+        <v>31.748999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1743,25 +1743,25 @@
         <v>663</v>
       </c>
       <c r="E31" s="11">
-        <v>0.161</v>
+        <v>0.157</v>
       </c>
       <c r="F31" s="3">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="G31" s="11">
-        <v>0.18099999999999999</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="H31" s="3">
         <v>668</v>
       </c>
       <c r="I31" s="11">
-        <v>0.109</v>
+        <v>0.114</v>
       </c>
       <c r="J31" s="3">
-        <v>930</v>
+        <v>925</v>
       </c>
       <c r="K31" s="11">
-        <v>0.19700000000000001</v>
+        <v>0.22700000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1778,25 +1778,25 @@
         <v>2422</v>
       </c>
       <c r="E32" s="11">
-        <v>1.296</v>
+        <v>1.2789999999999999</v>
       </c>
       <c r="F32" s="3">
-        <v>5269</v>
+        <v>5169</v>
       </c>
       <c r="G32" s="11">
-        <v>7.92</v>
+        <v>8.1859999999999999</v>
       </c>
       <c r="H32" s="3">
-        <v>2512</v>
+        <v>2515</v>
       </c>
       <c r="I32" s="11">
-        <v>1.347</v>
+        <v>1.3720000000000001</v>
       </c>
       <c r="J32" s="3">
-        <v>5544</v>
+        <v>5457</v>
       </c>
       <c r="K32" s="11">
-        <v>9.5009999999999994</v>
+        <v>8.2889999999999997</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1810,28 +1810,28 @@
         <v>10</v>
       </c>
       <c r="D33" s="4">
-        <v>2657</v>
+        <v>2640</v>
       </c>
       <c r="E33" s="11">
-        <v>0.55900000000000005</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="F33" s="3">
-        <v>4038</v>
+        <v>4082</v>
       </c>
       <c r="G33" s="11">
-        <v>1.101</v>
+        <v>1.232</v>
       </c>
       <c r="H33" s="3">
-        <v>3047</v>
+        <v>3035</v>
       </c>
       <c r="I33" s="11">
-        <v>0.58599999999999997</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="J33" s="3">
-        <v>4400</v>
+        <v>4410</v>
       </c>
       <c r="K33" s="11">
-        <v>1.32</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1848,25 +1848,25 @@
         <v>431</v>
       </c>
       <c r="E34" s="11">
-        <v>0.14599999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="F34" s="3">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="G34" s="11">
-        <v>0.36699999999999999</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="H34" s="3">
         <v>505</v>
       </c>
       <c r="I34" s="11">
-        <v>0.14299999999999999</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="J34" s="3">
-        <v>846</v>
+        <v>828</v>
       </c>
       <c r="K34" s="11">
-        <v>0.42199999999999999</v>
+        <v>0.45200000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1880,28 +1880,28 @@
         <v>11</v>
       </c>
       <c r="D35" s="4">
-        <v>1667</v>
+        <v>1664</v>
       </c>
       <c r="E35" s="11">
-        <v>0.29699999999999999</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="F35" s="3">
-        <v>3138</v>
+        <v>3056</v>
       </c>
       <c r="G35" s="11">
-        <v>1.125</v>
+        <v>1.3560000000000001</v>
       </c>
       <c r="H35" s="3">
-        <v>1673</v>
+        <v>1734</v>
       </c>
       <c r="I35" s="11">
-        <v>0.251</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="J35" s="3">
-        <v>3202</v>
+        <v>3296</v>
       </c>
       <c r="K35" s="11">
-        <v>1.0329999999999999</v>
+        <v>1.3109999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1915,28 +1915,28 @@
         <v>36</v>
       </c>
       <c r="D36" s="4">
-        <v>4561</v>
+        <v>4550</v>
       </c>
       <c r="E36" s="11">
-        <v>0.91900000000000004</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="F36" s="3">
-        <v>6856</v>
+        <v>6830</v>
       </c>
       <c r="G36" s="11">
-        <v>2.3969999999999998</v>
+        <v>2.2370000000000001</v>
       </c>
       <c r="H36" s="3">
-        <v>4552</v>
+        <v>4544</v>
       </c>
       <c r="I36" s="11">
-        <v>0.88500000000000001</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="J36" s="3">
-        <v>6916</v>
+        <v>6909</v>
       </c>
       <c r="K36" s="11">
-        <v>2.496</v>
+        <v>2.2370000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1953,25 +1953,25 @@
         <v>5619</v>
       </c>
       <c r="E37" s="11">
-        <v>0.71699999999999997</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="F37" s="3">
-        <v>8257</v>
+        <v>8339</v>
       </c>
       <c r="G37" s="11">
-        <v>2.6059999999999999</v>
+        <v>2.605</v>
       </c>
       <c r="H37" s="3">
         <v>5671</v>
       </c>
       <c r="I37" s="11">
-        <v>0.68899999999999995</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="J37" s="3">
-        <v>8335</v>
+        <v>8470</v>
       </c>
       <c r="K37" s="11">
-        <v>2.6389999999999998</v>
+        <v>2.5110000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1988,25 +1988,25 @@
         <v>4175</v>
       </c>
       <c r="E38" s="11">
-        <v>1.1459999999999999</v>
+        <v>1.0780000000000001</v>
       </c>
       <c r="F38" s="3">
-        <v>4671</v>
+        <v>4689</v>
       </c>
       <c r="G38" s="11">
-        <v>1.6919999999999999</v>
+        <v>1.714</v>
       </c>
       <c r="H38" s="3">
         <v>4256</v>
       </c>
       <c r="I38" s="11">
-        <v>1.2869999999999999</v>
+        <v>1.2310000000000001</v>
       </c>
       <c r="J38" s="3">
-        <v>4800</v>
+        <v>4785</v>
       </c>
       <c r="K38" s="11">
-        <v>2.0209999999999999</v>
+        <v>1.7989999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2023,25 +2023,25 @@
         <v>4912</v>
       </c>
       <c r="E39" s="11">
-        <v>0.61399999999999999</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="F39" s="3">
-        <v>5407</v>
+        <v>5361</v>
       </c>
       <c r="G39" s="11">
-        <v>0.871</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="H39" s="3">
         <v>4945</v>
       </c>
       <c r="I39" s="11">
-        <v>0.65400000000000003</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="J39" s="3">
-        <v>5196</v>
+        <v>5193</v>
       </c>
       <c r="K39" s="11">
-        <v>0.82299999999999995</v>
+        <v>0.76200000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2055,28 +2055,28 @@
         <v>36</v>
       </c>
       <c r="D40" s="4">
-        <v>4044</v>
+        <v>4204</v>
       </c>
       <c r="E40" s="11">
-        <v>1.6359999999999999</v>
+        <v>1.7210000000000001</v>
       </c>
       <c r="F40" s="3">
-        <v>4529</v>
+        <v>4542</v>
       </c>
       <c r="G40" s="11">
-        <v>2.7120000000000002</v>
+        <v>2.3730000000000002</v>
       </c>
       <c r="H40" s="3">
-        <v>4143</v>
+        <v>4219</v>
       </c>
       <c r="I40" s="11">
-        <v>1.899</v>
+        <v>2.0609999999999999</v>
       </c>
       <c r="J40" s="3">
-        <v>4629</v>
+        <v>4511</v>
       </c>
       <c r="K40" s="11">
-        <v>2.7330000000000001</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2093,25 +2093,25 @@
         <v>4601</v>
       </c>
       <c r="E41" s="11">
-        <v>1.387</v>
+        <v>1.3360000000000001</v>
       </c>
       <c r="F41" s="3">
-        <v>4611</v>
+        <v>4596</v>
       </c>
       <c r="G41" s="11">
-        <v>1.9239999999999999</v>
+        <v>1.774</v>
       </c>
       <c r="H41" s="3">
-        <v>4745</v>
+        <v>4746</v>
       </c>
       <c r="I41" s="11">
-        <v>1.5880000000000001</v>
+        <v>1.5569999999999999</v>
       </c>
       <c r="J41" s="3">
-        <v>4587</v>
+        <v>4534</v>
       </c>
       <c r="K41" s="11">
-        <v>1.881</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2128,25 +2128,25 @@
         <v>6024</v>
       </c>
       <c r="E42" s="11">
-        <v>0.86</v>
+        <v>0.79</v>
       </c>
       <c r="F42" s="3">
-        <v>6434</v>
+        <v>6409</v>
       </c>
       <c r="G42" s="11">
-        <v>1.159</v>
+        <v>1.125</v>
       </c>
       <c r="H42" s="3">
         <v>6388</v>
       </c>
       <c r="I42" s="11">
-        <v>0.92800000000000005</v>
+        <v>0.90400000000000003</v>
       </c>
       <c r="J42" s="3">
-        <v>6734</v>
+        <v>6740</v>
       </c>
       <c r="K42" s="11">
-        <v>1.1879999999999999</v>
+        <v>1.669</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2163,25 +2163,25 @@
         <v>1231</v>
       </c>
       <c r="E43" s="11">
-        <v>0.29399999999999998</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F43" s="3">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="G43" s="11">
-        <v>0.44800000000000001</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="H43" s="3">
         <v>1249</v>
       </c>
       <c r="I43" s="11">
-        <v>0.25600000000000001</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="J43" s="3">
-        <v>1503</v>
+        <v>1525</v>
       </c>
       <c r="K43" s="11">
-        <v>0.49099999999999999</v>
+        <v>0.49399999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2195,28 +2195,28 @@
         <v>24</v>
       </c>
       <c r="D44" s="4">
-        <v>7808</v>
+        <v>7786</v>
       </c>
       <c r="E44" s="11">
-        <v>4.1449999999999996</v>
+        <v>3.9550000000000001</v>
       </c>
       <c r="F44" s="3">
-        <v>6527</v>
+        <v>6530</v>
       </c>
       <c r="G44" s="11">
-        <v>5.8209999999999997</v>
+        <v>5.5190000000000001</v>
       </c>
       <c r="H44" s="3">
-        <v>7920</v>
+        <v>7901</v>
       </c>
       <c r="I44" s="11">
-        <v>4.6989999999999998</v>
+        <v>3.85</v>
       </c>
       <c r="J44" s="3">
-        <v>6644</v>
+        <v>6611</v>
       </c>
       <c r="K44" s="11">
-        <v>6.2869999999999999</v>
+        <v>6.1379999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2230,28 +2230,28 @@
         <v>30</v>
       </c>
       <c r="D45" s="4">
-        <v>4923</v>
+        <v>4891</v>
       </c>
       <c r="E45" s="11">
-        <v>5.5469999999999997</v>
+        <v>6</v>
       </c>
       <c r="F45" s="3">
-        <v>4923</v>
+        <v>4891</v>
       </c>
       <c r="G45" s="11">
-        <v>5.4329999999999998</v>
+        <v>5.54</v>
       </c>
       <c r="H45" s="3">
-        <v>4923</v>
+        <v>4891</v>
       </c>
       <c r="I45" s="11">
-        <v>5.5490000000000004</v>
+        <v>6.202</v>
       </c>
       <c r="J45" s="3">
-        <v>4923</v>
+        <v>4891</v>
       </c>
       <c r="K45" s="11">
-        <v>5.5339999999999998</v>
+        <v>5.9779999999999998</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2265,28 +2265,28 @@
         <v>8.5</v>
       </c>
       <c r="D46" s="4">
-        <v>2551</v>
+        <v>2463</v>
       </c>
       <c r="E46" s="11">
-        <v>19.486000000000001</v>
+        <v>20.654</v>
       </c>
       <c r="F46" s="3">
-        <v>2551</v>
+        <v>2463</v>
       </c>
       <c r="G46" s="11">
-        <v>19.513000000000002</v>
+        <v>20.923999999999999</v>
       </c>
       <c r="H46" s="3">
-        <v>2551</v>
+        <v>2463</v>
       </c>
       <c r="I46" s="11">
-        <v>18.972999999999999</v>
+        <v>22.632000000000001</v>
       </c>
       <c r="J46" s="3">
-        <v>2551</v>
+        <v>2463</v>
       </c>
       <c r="K46" s="11">
-        <v>18.916</v>
+        <v>22.393000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2300,10 +2300,10 @@
         <v>33.72</v>
       </c>
       <c r="D47" s="4">
-        <v>8965</v>
+        <v>8856</v>
       </c>
       <c r="E47" s="11">
-        <v>4.1440000000000001</v>
+        <v>3.8050000000000002</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>44</v>
@@ -2335,10 +2335,10 @@
         <v>32.19</v>
       </c>
       <c r="D48" s="4">
-        <v>8747</v>
+        <v>8467</v>
       </c>
       <c r="E48" s="11">
-        <v>5.4039999999999999</v>
+        <v>5.258</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>44</v>
@@ -2370,10 +2370,10 @@
         <v>59.18</v>
       </c>
       <c r="D49" s="4">
-        <v>15010</v>
+        <v>14844</v>
       </c>
       <c r="E49" s="11">
-        <v>10.494999999999999</v>
+        <v>10.207000000000001</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>44</v>
@@ -2405,10 +2405,10 @@
         <v>39.020000000000003</v>
       </c>
       <c r="D50" s="4">
-        <v>11170</v>
+        <v>11309</v>
       </c>
       <c r="E50" s="11">
-        <v>7.5449999999999999</v>
+        <v>7.6210000000000004</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>44</v>
@@ -2437,13 +2437,13 @@
         <v>48</v>
       </c>
       <c r="C51" s="11">
-        <v>34.69</v>
+        <v>34.68</v>
       </c>
       <c r="D51" s="4">
-        <v>9292</v>
+        <v>9052</v>
       </c>
       <c r="E51" s="11">
-        <v>5.298</v>
+        <v>4.8920000000000003</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>44</v>
@@ -2475,10 +2475,10 @@
         <v>40.86</v>
       </c>
       <c r="D52" s="4">
-        <v>11807</v>
+        <v>12326</v>
       </c>
       <c r="E52" s="11">
-        <v>10.874000000000001</v>
+        <v>11.484</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>44</v>
@@ -2507,13 +2507,13 @@
         <v>50</v>
       </c>
       <c r="C53" s="2">
-        <v>41.28</v>
+        <v>41.27</v>
       </c>
       <c r="D53" s="2">
-        <v>11580</v>
+        <v>11073</v>
       </c>
       <c r="E53" s="11">
-        <v>8.1509999999999998</v>
+        <v>8.2249999999999996</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>44</v>
@@ -2545,10 +2545,10 @@
         <v>45.28</v>
       </c>
       <c r="D54" s="2">
-        <v>11898</v>
+        <v>11677</v>
       </c>
       <c r="E54" s="11">
-        <v>13.010999999999999</v>
+        <v>14.265000000000001</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>44</v>
@@ -2580,10 +2580,10 @@
         <v>27.71</v>
       </c>
       <c r="D55" s="2">
-        <v>9000</v>
+        <v>9011</v>
       </c>
       <c r="E55" s="11">
-        <v>8.3710000000000004</v>
+        <v>8.4209999999999994</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Initial commit R2017a.  Version 4.1
</commit_message>
<xml_diff>
--- a/Scripts_Data/CFR_Results.xlsx
+++ b/Scripts_Data/CFR_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R16b\Scripts_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R17a\Scripts_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -210,13 +210,13 @@
     <t>Frict3D_08_Ball_on_Driven_Tube</t>
   </si>
   <si>
+    <t>9.2.0.538062 (R2017a)</t>
+  </si>
+  <si>
+    <t>09-Mar-2018 01:22:33</t>
+  </si>
+  <si>
     <t>CFL v4.0</t>
-  </si>
-  <si>
-    <t>9.1.0.441655 (R2016b)</t>
-  </si>
-  <si>
-    <t>09-Mar-2018 07:57:04</t>
   </si>
 </sst>
 </file>
@@ -719,16 +719,16 @@
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -798,25 +798,25 @@
         <v>2400</v>
       </c>
       <c r="E4" s="14">
-        <v>0.26</v>
+        <v>0.505</v>
       </c>
       <c r="F4" s="15">
         <v>2400</v>
       </c>
       <c r="G4" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="H4" s="15">
         <v>2400</v>
       </c>
       <c r="I4" s="14">
-        <v>0.156</v>
+        <v>0.224</v>
       </c>
       <c r="J4" s="15">
         <v>2400</v>
       </c>
       <c r="K4" s="14">
-        <v>0.17100000000000001</v>
+        <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -833,25 +833,25 @@
         <v>674</v>
       </c>
       <c r="E5" s="11">
-        <v>0.15</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="F5" s="4">
         <v>959</v>
       </c>
       <c r="G5" s="11">
-        <v>8.2000000000000003E-2</v>
+        <v>0.11</v>
       </c>
       <c r="H5" s="4">
         <v>731</v>
       </c>
       <c r="I5" s="11">
-        <v>0.06</v>
+        <v>0.124</v>
       </c>
       <c r="J5" s="4">
         <v>1028</v>
       </c>
       <c r="K5" s="11">
-        <v>9.4E-2</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -868,25 +868,25 @@
         <v>311</v>
       </c>
       <c r="E6" s="11">
-        <v>0.13400000000000001</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="F6" s="4">
         <v>366</v>
       </c>
       <c r="G6" s="11">
-        <v>6.4000000000000001E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="H6" s="4">
         <v>317</v>
       </c>
       <c r="I6" s="11">
-        <v>5.2999999999999999E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="J6" s="4">
         <v>397</v>
       </c>
       <c r="K6" s="11">
-        <v>6.7000000000000004E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -903,25 +903,25 @@
         <v>3805</v>
       </c>
       <c r="E7" s="11">
-        <v>1.863</v>
+        <v>1.9630000000000001</v>
       </c>
       <c r="F7" s="4">
         <v>4908</v>
       </c>
       <c r="G7" s="11">
-        <v>2.5619999999999998</v>
+        <v>2.7829999999999999</v>
       </c>
       <c r="H7" s="4">
         <v>4676</v>
       </c>
       <c r="I7" s="11">
-        <v>2.4359999999999999</v>
+        <v>2.5830000000000002</v>
       </c>
       <c r="J7" s="4">
         <v>6075</v>
       </c>
       <c r="K7" s="11">
-        <v>3.4780000000000002</v>
+        <v>4.5179999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -938,25 +938,25 @@
         <v>2040</v>
       </c>
       <c r="E8" s="11">
-        <v>0.307</v>
+        <v>0.44</v>
       </c>
       <c r="F8" s="4">
         <v>2667</v>
       </c>
       <c r="G8" s="11">
-        <v>0.4</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="H8" s="4">
         <v>2284</v>
       </c>
       <c r="I8" s="11">
-        <v>0.21</v>
+        <v>0.42</v>
       </c>
       <c r="J8" s="4">
         <v>2900</v>
       </c>
       <c r="K8" s="11">
-        <v>0.313</v>
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -973,25 +973,25 @@
         <v>616</v>
       </c>
       <c r="E9" s="11">
-        <v>0.158</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="F9" s="4">
         <v>600</v>
       </c>
       <c r="G9" s="11">
-        <v>0.122</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="H9" s="4">
         <v>745</v>
       </c>
       <c r="I9" s="11">
-        <v>0.127</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="J9" s="4">
         <v>616</v>
       </c>
       <c r="K9" s="11">
-        <v>0.128</v>
+        <v>0.13900000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1008,13 +1008,13 @@
         <v>200</v>
       </c>
       <c r="E10" s="11">
-        <v>6.0999999999999999E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="F10" s="4">
         <v>207</v>
       </c>
       <c r="G10" s="11">
-        <v>3.2000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="H10" s="4">
         <v>213</v>
@@ -1026,7 +1026,7 @@
         <v>221</v>
       </c>
       <c r="K10" s="11">
-        <v>3.6999999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1043,25 +1043,25 @@
         <v>10055</v>
       </c>
       <c r="E11" s="11">
-        <v>3.1349999999999998</v>
+        <v>3.5720000000000001</v>
       </c>
       <c r="F11" s="4">
         <v>18721</v>
       </c>
       <c r="G11" s="11">
-        <v>6.9119999999999999</v>
+        <v>8.0489999999999995</v>
       </c>
       <c r="H11" s="4">
         <v>12458</v>
       </c>
       <c r="I11" s="11">
-        <v>4.673</v>
+        <v>5.2290000000000001</v>
       </c>
       <c r="J11" s="4">
         <v>21338</v>
       </c>
       <c r="K11" s="11">
-        <v>8.7789999999999999</v>
+        <v>9.423</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1078,25 +1078,25 @@
         <v>1211</v>
       </c>
       <c r="E12" s="11">
-        <v>0.14399999999999999</v>
+        <v>0.107</v>
       </c>
       <c r="F12" s="4">
         <v>1211</v>
       </c>
       <c r="G12" s="11">
-        <v>6.7000000000000004E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="H12" s="4">
         <v>1211</v>
       </c>
       <c r="I12" s="11">
-        <v>6.2E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="J12" s="4">
         <v>1211</v>
       </c>
       <c r="K12" s="11">
-        <v>6.3E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1113,25 +1113,25 @@
         <v>1301</v>
       </c>
       <c r="E13" s="11">
-        <v>0.184</v>
+        <v>0.187</v>
       </c>
       <c r="F13" s="3">
         <v>1411</v>
       </c>
       <c r="G13" s="11">
-        <v>0.17100000000000001</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="H13" s="4">
         <v>1396</v>
       </c>
       <c r="I13" s="11">
-        <v>0.16</v>
+        <v>0.161</v>
       </c>
       <c r="J13" s="4">
         <v>1476</v>
       </c>
       <c r="K13" s="11">
-        <v>0.19</v>
+        <v>0.19800000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1148,25 +1148,25 @@
         <v>5538</v>
       </c>
       <c r="E14" s="11">
-        <v>0.378</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="F14" s="3">
         <v>5538</v>
       </c>
       <c r="G14" s="11">
-        <v>0.27200000000000002</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="H14" s="4">
         <v>5538</v>
       </c>
       <c r="I14" s="11">
-        <v>0.26400000000000001</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="J14" s="4">
         <v>5538</v>
       </c>
       <c r="K14" s="11">
-        <v>0.26400000000000001</v>
+        <v>0.49099999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1183,25 +1183,25 @@
         <v>732</v>
       </c>
       <c r="E15" s="11">
-        <v>0.11899999999999999</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="F15" s="3">
         <v>859</v>
       </c>
       <c r="G15" s="11">
-        <v>9.1999999999999998E-2</v>
+        <v>0.111</v>
       </c>
       <c r="H15" s="3">
         <v>807</v>
       </c>
       <c r="I15" s="11">
-        <v>7.2999999999999995E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="J15" s="3">
         <v>934</v>
       </c>
       <c r="K15" s="11">
-        <v>9.7000000000000003E-2</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1218,25 +1218,25 @@
         <v>1305</v>
       </c>
       <c r="E16" s="11">
-        <v>0.14399999999999999</v>
+        <v>0.19700000000000001</v>
       </c>
       <c r="F16" s="3">
         <v>1400</v>
       </c>
       <c r="G16" s="11">
-        <v>0.126</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="H16" s="3">
         <v>1415</v>
       </c>
       <c r="I16" s="11">
-        <v>0.121</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="J16" s="3">
         <v>1443</v>
       </c>
       <c r="K16" s="11">
-        <v>0.151</v>
+        <v>0.13900000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1253,25 +1253,25 @@
         <v>6365</v>
       </c>
       <c r="E17" s="11">
-        <v>1.204</v>
+        <v>2.0619999999999998</v>
       </c>
       <c r="F17" s="3">
         <v>6812</v>
       </c>
       <c r="G17" s="11">
-        <v>1.4119999999999999</v>
+        <v>1.86</v>
       </c>
       <c r="H17" s="3">
         <v>6022</v>
       </c>
       <c r="I17" s="11">
-        <v>1.3069999999999999</v>
+        <v>1.6859999999999999</v>
       </c>
       <c r="J17" s="3">
         <v>6420</v>
       </c>
       <c r="K17" s="11">
-        <v>1.4750000000000001</v>
+        <v>1.7849999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1288,25 +1288,25 @@
         <v>277</v>
       </c>
       <c r="E18" s="11">
-        <v>0.10100000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="F18" s="3">
         <v>307</v>
       </c>
       <c r="G18" s="11">
-        <v>5.7000000000000002E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="H18" s="3">
         <v>314</v>
       </c>
       <c r="I18" s="11">
-        <v>0.06</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="J18" s="3">
         <v>334</v>
       </c>
       <c r="K18" s="11">
-        <v>6.6000000000000003E-2</v>
+        <v>7.8E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1323,25 +1323,25 @@
         <v>3432</v>
       </c>
       <c r="E19" s="11">
-        <v>0.61899999999999999</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="F19" s="3">
         <v>3672</v>
       </c>
       <c r="G19" s="11">
-        <v>0.7</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="H19" s="3">
         <v>3544</v>
       </c>
       <c r="I19" s="11">
-        <v>0.67100000000000004</v>
+        <v>0.89900000000000002</v>
       </c>
       <c r="J19" s="3">
         <v>3829</v>
       </c>
       <c r="K19" s="11">
-        <v>0.73</v>
+        <v>1.0069999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1358,25 +1358,25 @@
         <v>6974</v>
       </c>
       <c r="E20" s="11">
-        <v>0.86199999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="F20" s="3">
         <v>6688</v>
       </c>
       <c r="G20" s="11">
-        <v>0.74</v>
+        <v>1.4450000000000001</v>
       </c>
       <c r="H20" s="3">
         <v>98588</v>
       </c>
       <c r="I20" s="11">
-        <v>10.592000000000001</v>
+        <v>14.33</v>
       </c>
       <c r="J20" s="3">
         <v>99644</v>
       </c>
       <c r="K20" s="11">
-        <v>10.602</v>
+        <v>12.486000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1393,19 +1393,19 @@
         <v>3637</v>
       </c>
       <c r="E21" s="11">
-        <v>0.59699999999999998</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="F21" s="3">
         <v>4630</v>
       </c>
       <c r="G21" s="11">
-        <v>0.60699999999999998</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="H21" s="3">
         <v>4076</v>
       </c>
       <c r="I21" s="11">
-        <v>0.44700000000000001</v>
+        <v>0.48099999999999998</v>
       </c>
       <c r="J21" s="3">
         <v>4180</v>
@@ -1428,25 +1428,25 @@
         <v>2138</v>
       </c>
       <c r="E22" s="11">
-        <v>4.5529999999999999</v>
+        <v>6.4850000000000003</v>
       </c>
       <c r="F22" s="3">
         <v>2138</v>
       </c>
       <c r="G22" s="11">
-        <v>4.819</v>
+        <v>6.3029999999999999</v>
       </c>
       <c r="H22" s="3">
         <v>2138</v>
       </c>
       <c r="I22" s="11">
-        <v>4.625</v>
+        <v>5.94</v>
       </c>
       <c r="J22" s="3">
         <v>2138</v>
       </c>
       <c r="K22" s="11">
-        <v>4.5789999999999997</v>
+        <v>7.0640000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1460,28 +1460,28 @@
         <v>15</v>
       </c>
       <c r="D23" s="4">
-        <v>3132</v>
+        <v>3145</v>
       </c>
       <c r="E23" s="11">
-        <v>1.298</v>
+        <v>1.5109999999999999</v>
       </c>
       <c r="F23" s="3">
-        <v>3111</v>
+        <v>3164</v>
       </c>
       <c r="G23" s="11">
-        <v>1.1890000000000001</v>
+        <v>1.2909999999999999</v>
       </c>
       <c r="H23" s="3">
-        <v>3782</v>
+        <v>3721</v>
       </c>
       <c r="I23" s="11">
-        <v>1.3720000000000001</v>
+        <v>1.5580000000000001</v>
       </c>
       <c r="J23" s="3">
-        <v>3676</v>
+        <v>3684</v>
       </c>
       <c r="K23" s="11">
-        <v>1.3919999999999999</v>
+        <v>1.4610000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1498,25 +1498,25 @@
         <v>131</v>
       </c>
       <c r="E24" s="11">
-        <v>0.17499999999999999</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="F24" s="3">
         <v>131</v>
       </c>
       <c r="G24" s="11">
-        <v>0.11</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="H24" s="3">
         <v>131</v>
       </c>
       <c r="I24" s="11">
-        <v>0.111</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J24" s="3">
         <v>131</v>
       </c>
       <c r="K24" s="11">
-        <v>0.10199999999999999</v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1533,25 +1533,25 @@
         <v>4741</v>
       </c>
       <c r="E25" s="11">
-        <v>3.5289999999999999</v>
+        <v>4.3620000000000001</v>
       </c>
       <c r="F25" s="3">
         <v>5224</v>
       </c>
       <c r="G25" s="11">
-        <v>4.3760000000000003</v>
+        <v>5.1769999999999996</v>
       </c>
       <c r="H25" s="3">
         <v>4567</v>
       </c>
       <c r="I25" s="11">
-        <v>3.7530000000000001</v>
+        <v>4.5149999999999997</v>
       </c>
       <c r="J25" s="3">
         <v>5136</v>
       </c>
       <c r="K25" s="11">
-        <v>4.4459999999999997</v>
+        <v>5.3010000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1568,25 +1568,25 @@
         <v>13792</v>
       </c>
       <c r="E26" s="11">
-        <v>7.2080000000000002</v>
+        <v>8.0649999999999995</v>
       </c>
       <c r="F26" s="3">
         <v>14308</v>
       </c>
       <c r="G26" s="11">
-        <v>7.3949999999999996</v>
+        <v>8.1969999999999992</v>
       </c>
       <c r="H26" s="3">
         <v>19430</v>
       </c>
       <c r="I26" s="11">
-        <v>10.407999999999999</v>
+        <v>11.334</v>
       </c>
       <c r="J26" s="3">
         <v>23305</v>
       </c>
       <c r="K26" s="11">
-        <v>12.148</v>
+        <v>13.595000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1603,25 +1603,25 @@
         <v>3423</v>
       </c>
       <c r="E27" s="11">
-        <v>2.1829999999999998</v>
+        <v>2.4910000000000001</v>
       </c>
       <c r="F27" s="3">
         <v>4110</v>
       </c>
       <c r="G27" s="11">
-        <v>3.218</v>
+        <v>3.7050000000000001</v>
       </c>
       <c r="H27" s="3">
         <v>3479</v>
       </c>
       <c r="I27" s="11">
-        <v>2.077</v>
+        <v>2.6230000000000002</v>
       </c>
       <c r="J27" s="3">
         <v>4217</v>
       </c>
       <c r="K27" s="11">
-        <v>3.1760000000000002</v>
+        <v>3.8109999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1638,25 +1638,25 @@
         <v>940</v>
       </c>
       <c r="E28" s="11">
-        <v>0.16900000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="F28" s="3">
-        <v>1005</v>
+        <v>1024</v>
       </c>
       <c r="G28" s="11">
-        <v>0.124</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="H28" s="3">
         <v>967</v>
       </c>
       <c r="I28" s="11">
-        <v>0.106</v>
+        <v>0.112</v>
       </c>
       <c r="J28" s="3">
         <v>1060</v>
       </c>
       <c r="K28" s="11">
-        <v>0.156</v>
+        <v>0.17100000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1670,28 +1670,28 @@
         <v>5</v>
       </c>
       <c r="D29" s="4">
-        <v>710</v>
+        <v>756</v>
       </c>
       <c r="E29" s="11">
-        <v>0.14399999999999999</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="F29" s="3">
-        <v>832</v>
+        <v>863</v>
       </c>
       <c r="G29" s="11">
-        <v>0.126</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="H29" s="3">
-        <v>746</v>
+        <v>786</v>
       </c>
       <c r="I29" s="11">
-        <v>0.128</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="J29" s="3">
-        <v>856</v>
+        <v>896</v>
       </c>
       <c r="K29" s="11">
-        <v>0.16200000000000001</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1708,25 +1708,25 @@
         <v>10344</v>
       </c>
       <c r="E30" s="11">
-        <v>11.092000000000001</v>
+        <v>16.177</v>
       </c>
       <c r="F30" s="3">
         <v>12311</v>
       </c>
       <c r="G30" s="11">
-        <v>24.744</v>
+        <v>29.396000000000001</v>
       </c>
       <c r="H30" s="3">
         <v>11682</v>
       </c>
       <c r="I30" s="11">
-        <v>17.956</v>
+        <v>23.045000000000002</v>
       </c>
       <c r="J30" s="3">
         <v>13340</v>
       </c>
       <c r="K30" s="11">
-        <v>31.748999999999999</v>
+        <v>40.973999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1740,28 +1740,28 @@
         <v>5</v>
       </c>
       <c r="D31" s="4">
-        <v>663</v>
+        <v>882</v>
       </c>
       <c r="E31" s="11">
-        <v>0.157</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="F31" s="3">
-        <v>897</v>
+        <v>910</v>
       </c>
       <c r="G31" s="11">
-        <v>0.19900000000000001</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="H31" s="3">
-        <v>668</v>
+        <v>879</v>
       </c>
       <c r="I31" s="11">
-        <v>0.114</v>
+        <v>0.255</v>
       </c>
       <c r="J31" s="3">
-        <v>925</v>
+        <v>949</v>
       </c>
       <c r="K31" s="11">
-        <v>0.22700000000000001</v>
+        <v>0.245</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1775,28 +1775,28 @@
         <v>20</v>
       </c>
       <c r="D32" s="4">
-        <v>2422</v>
+        <v>2429</v>
       </c>
       <c r="E32" s="11">
-        <v>1.2789999999999999</v>
+        <v>1.3360000000000001</v>
       </c>
       <c r="F32" s="3">
-        <v>5169</v>
+        <v>5534</v>
       </c>
       <c r="G32" s="11">
-        <v>8.1859999999999999</v>
+        <v>10.211</v>
       </c>
       <c r="H32" s="3">
-        <v>2515</v>
+        <v>2519</v>
       </c>
       <c r="I32" s="11">
-        <v>1.3720000000000001</v>
+        <v>1.56</v>
       </c>
       <c r="J32" s="3">
-        <v>5457</v>
+        <v>6071</v>
       </c>
       <c r="K32" s="11">
-        <v>8.2889999999999997</v>
+        <v>11.276999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1813,25 +1813,25 @@
         <v>2640</v>
       </c>
       <c r="E33" s="11">
-        <v>0.51900000000000002</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="F33" s="3">
         <v>4082</v>
       </c>
       <c r="G33" s="11">
-        <v>1.232</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H33" s="3">
         <v>3035</v>
       </c>
       <c r="I33" s="11">
-        <v>0.58799999999999997</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="J33" s="3">
         <v>4410</v>
       </c>
       <c r="K33" s="11">
-        <v>0.92500000000000004</v>
+        <v>1.125</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1848,25 +1848,25 @@
         <v>431</v>
       </c>
       <c r="E34" s="11">
-        <v>0.15</v>
+        <v>0.189</v>
       </c>
       <c r="F34" s="3">
         <v>740</v>
       </c>
       <c r="G34" s="11">
-        <v>0.35099999999999998</v>
+        <v>0.43</v>
       </c>
       <c r="H34" s="3">
         <v>505</v>
       </c>
       <c r="I34" s="11">
-        <v>0.13500000000000001</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="J34" s="3">
         <v>828</v>
       </c>
       <c r="K34" s="11">
-        <v>0.45200000000000001</v>
+        <v>0.46800000000000003</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1883,25 +1883,25 @@
         <v>1664</v>
       </c>
       <c r="E35" s="11">
-        <v>0.30099999999999999</v>
+        <v>0.38700000000000001</v>
       </c>
       <c r="F35" s="3">
         <v>3056</v>
       </c>
       <c r="G35" s="11">
-        <v>1.3560000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="H35" s="3">
         <v>1734</v>
       </c>
       <c r="I35" s="11">
-        <v>0.26300000000000001</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="J35" s="3">
         <v>3296</v>
       </c>
       <c r="K35" s="11">
-        <v>1.3109999999999999</v>
+        <v>1.1559999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1918,25 +1918,25 @@
         <v>4550</v>
       </c>
       <c r="E36" s="11">
-        <v>0.89800000000000002</v>
+        <v>0.95</v>
       </c>
       <c r="F36" s="3">
         <v>6830</v>
       </c>
       <c r="G36" s="11">
-        <v>2.2370000000000001</v>
+        <v>2.3690000000000002</v>
       </c>
       <c r="H36" s="3">
         <v>4544</v>
       </c>
       <c r="I36" s="11">
-        <v>0.84499999999999997</v>
+        <v>1.1020000000000001</v>
       </c>
       <c r="J36" s="3">
         <v>6909</v>
       </c>
       <c r="K36" s="11">
-        <v>2.2370000000000001</v>
+        <v>2.286</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1950,28 +1950,28 @@
         <v>48</v>
       </c>
       <c r="D37" s="4">
-        <v>5619</v>
+        <v>5609</v>
       </c>
       <c r="E37" s="11">
-        <v>0.68500000000000005</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="F37" s="3">
-        <v>8339</v>
+        <v>8295</v>
       </c>
       <c r="G37" s="11">
-        <v>2.605</v>
+        <v>2.8929999999999998</v>
       </c>
       <c r="H37" s="3">
-        <v>5671</v>
+        <v>5673</v>
       </c>
       <c r="I37" s="11">
-        <v>0.64600000000000002</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="J37" s="3">
-        <v>8470</v>
+        <v>8346</v>
       </c>
       <c r="K37" s="11">
-        <v>2.5110000000000001</v>
+        <v>3.0489999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1988,25 +1988,25 @@
         <v>4175</v>
       </c>
       <c r="E38" s="11">
-        <v>1.0780000000000001</v>
+        <v>1.2569999999999999</v>
       </c>
       <c r="F38" s="3">
         <v>4689</v>
       </c>
       <c r="G38" s="11">
-        <v>1.714</v>
+        <v>1.8260000000000001</v>
       </c>
       <c r="H38" s="3">
         <v>4256</v>
       </c>
       <c r="I38" s="11">
-        <v>1.2310000000000001</v>
+        <v>1.41</v>
       </c>
       <c r="J38" s="3">
         <v>4785</v>
       </c>
       <c r="K38" s="11">
-        <v>1.7989999999999999</v>
+        <v>1.996</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2023,25 +2023,25 @@
         <v>4912</v>
       </c>
       <c r="E39" s="11">
-        <v>0.60599999999999998</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="F39" s="3">
         <v>5361</v>
       </c>
       <c r="G39" s="11">
-        <v>0.83499999999999996</v>
+        <v>1.0389999999999999</v>
       </c>
       <c r="H39" s="3">
         <v>4945</v>
       </c>
       <c r="I39" s="11">
-        <v>0.61499999999999999</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="J39" s="3">
         <v>5193</v>
       </c>
       <c r="K39" s="11">
-        <v>0.76200000000000001</v>
+        <v>0.91400000000000003</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2058,25 +2058,25 @@
         <v>4204</v>
       </c>
       <c r="E40" s="11">
-        <v>1.7210000000000001</v>
+        <v>2.1320000000000001</v>
       </c>
       <c r="F40" s="3">
         <v>4542</v>
       </c>
       <c r="G40" s="11">
-        <v>2.3730000000000002</v>
+        <v>2.8029999999999999</v>
       </c>
       <c r="H40" s="3">
         <v>4219</v>
       </c>
       <c r="I40" s="11">
-        <v>2.0609999999999999</v>
+        <v>2.133</v>
       </c>
       <c r="J40" s="3">
         <v>4511</v>
       </c>
       <c r="K40" s="11">
-        <v>2.57</v>
+        <v>2.718</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2093,25 +2093,25 @@
         <v>4601</v>
       </c>
       <c r="E41" s="11">
-        <v>1.3360000000000001</v>
+        <v>1.5529999999999999</v>
       </c>
       <c r="F41" s="3">
         <v>4596</v>
       </c>
       <c r="G41" s="11">
-        <v>1.774</v>
+        <v>1.976</v>
       </c>
       <c r="H41" s="3">
         <v>4746</v>
       </c>
       <c r="I41" s="11">
-        <v>1.5569999999999999</v>
+        <v>1.655</v>
       </c>
       <c r="J41" s="3">
         <v>4534</v>
       </c>
       <c r="K41" s="11">
-        <v>1.85</v>
+        <v>1.9550000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2128,25 +2128,25 @@
         <v>6024</v>
       </c>
       <c r="E42" s="11">
-        <v>0.79</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="F42" s="3">
         <v>6409</v>
       </c>
       <c r="G42" s="11">
-        <v>1.125</v>
+        <v>1.361</v>
       </c>
       <c r="H42" s="3">
         <v>6388</v>
       </c>
       <c r="I42" s="11">
-        <v>0.90400000000000003</v>
+        <v>1.0720000000000001</v>
       </c>
       <c r="J42" s="3">
         <v>6740</v>
       </c>
       <c r="K42" s="11">
-        <v>1.669</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2163,25 +2163,25 @@
         <v>1231</v>
       </c>
       <c r="E43" s="11">
-        <v>0.28999999999999998</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="F43" s="3">
         <v>1386</v>
       </c>
       <c r="G43" s="11">
-        <v>0.43099999999999999</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="H43" s="3">
         <v>1249</v>
       </c>
       <c r="I43" s="11">
-        <v>0.25900000000000001</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="J43" s="3">
         <v>1525</v>
       </c>
       <c r="K43" s="11">
-        <v>0.49399999999999999</v>
+        <v>0.79800000000000004</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2195,28 +2195,28 @@
         <v>24</v>
       </c>
       <c r="D44" s="4">
-        <v>7786</v>
+        <v>8147</v>
       </c>
       <c r="E44" s="11">
-        <v>3.9550000000000001</v>
+        <v>5.4169999999999998</v>
       </c>
       <c r="F44" s="3">
-        <v>6530</v>
+        <v>6557</v>
       </c>
       <c r="G44" s="11">
-        <v>5.5190000000000001</v>
+        <v>7.7069999999999999</v>
       </c>
       <c r="H44" s="3">
-        <v>7901</v>
+        <v>8243</v>
       </c>
       <c r="I44" s="11">
-        <v>3.85</v>
+        <v>5.335</v>
       </c>
       <c r="J44" s="3">
-        <v>6611</v>
+        <v>6634</v>
       </c>
       <c r="K44" s="11">
-        <v>6.1379999999999999</v>
+        <v>8.2360000000000007</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2233,25 +2233,25 @@
         <v>4891</v>
       </c>
       <c r="E45" s="11">
-        <v>6</v>
+        <v>6.0960000000000001</v>
       </c>
       <c r="F45" s="3">
         <v>4891</v>
       </c>
       <c r="G45" s="11">
-        <v>5.54</v>
+        <v>6.0869999999999997</v>
       </c>
       <c r="H45" s="3">
         <v>4891</v>
       </c>
       <c r="I45" s="11">
-        <v>6.202</v>
+        <v>6.0830000000000002</v>
       </c>
       <c r="J45" s="3">
         <v>4891</v>
       </c>
       <c r="K45" s="11">
-        <v>5.9779999999999998</v>
+        <v>6.1260000000000003</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2268,25 +2268,25 @@
         <v>2463</v>
       </c>
       <c r="E46" s="11">
-        <v>20.654</v>
+        <v>24.542000000000002</v>
       </c>
       <c r="F46" s="3">
         <v>2463</v>
       </c>
       <c r="G46" s="11">
-        <v>20.923999999999999</v>
+        <v>25.917000000000002</v>
       </c>
       <c r="H46" s="3">
         <v>2463</v>
       </c>
       <c r="I46" s="11">
-        <v>22.632000000000001</v>
+        <v>26.273</v>
       </c>
       <c r="J46" s="3">
         <v>2463</v>
       </c>
       <c r="K46" s="11">
-        <v>22.393000000000001</v>
+        <v>25.462</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2303,7 +2303,7 @@
         <v>8856</v>
       </c>
       <c r="E47" s="11">
-        <v>3.8050000000000002</v>
+        <v>4.5309999999999997</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>44</v>
@@ -2338,7 +2338,7 @@
         <v>8467</v>
       </c>
       <c r="E48" s="11">
-        <v>5.258</v>
+        <v>6.093</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>44</v>
@@ -2373,7 +2373,7 @@
         <v>14844</v>
       </c>
       <c r="E49" s="11">
-        <v>10.207000000000001</v>
+        <v>10.676</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>44</v>
@@ -2408,7 +2408,7 @@
         <v>11309</v>
       </c>
       <c r="E50" s="11">
-        <v>7.6210000000000004</v>
+        <v>8.7360000000000007</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>44</v>
@@ -2443,7 +2443,7 @@
         <v>9052</v>
       </c>
       <c r="E51" s="11">
-        <v>4.8920000000000003</v>
+        <v>5.5179999999999998</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>44</v>
@@ -2478,7 +2478,7 @@
         <v>12326</v>
       </c>
       <c r="E52" s="11">
-        <v>11.484</v>
+        <v>13.411</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>44</v>
@@ -2513,7 +2513,7 @@
         <v>11073</v>
       </c>
       <c r="E53" s="11">
-        <v>8.2249999999999996</v>
+        <v>8.609</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>44</v>
@@ -2545,10 +2545,10 @@
         <v>45.28</v>
       </c>
       <c r="D54" s="2">
-        <v>11677</v>
+        <v>12191</v>
       </c>
       <c r="E54" s="11">
-        <v>14.265000000000001</v>
+        <v>13.792999999999999</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>44</v>
@@ -2583,7 +2583,7 @@
         <v>9011</v>
       </c>
       <c r="E55" s="11">
-        <v>8.4209999999999994</v>
+        <v>9.0809999999999995</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>44</v>
@@ -2618,6 +2618,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100525B94EEF47D42499A62120CC90E0AB3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e706cd362d7e41030bb8c72a7c62a9d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c85acdc-a394-4ae0-8c72-fb4a95b3d573" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55e2521e7df4d5c11309cefaa7c01562" ns2:_="">
     <xsd:import namespace="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
@@ -2762,18 +2773,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2819,29 +2828,10 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2863,25 +2853,35 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630E037-F79E-4175-B540-A23B306F8900}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE6D0D52-57FE-48CB-8E43-11384E6CFEE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630E037-F79E-4175-B540-A23B306F8900}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Initial commit R2017b.  Version 4.1
</commit_message>
<xml_diff>
--- a/Scripts_Data/CFR_Results.xlsx
+++ b/Scripts_Data/CFR_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R17a\Scripts_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R17b\Scripts_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -210,13 +210,13 @@
     <t>Frict3D_08_Ball_on_Driven_Tube</t>
   </si>
   <si>
-    <t>9.2.0.538062 (R2017a)</t>
-  </si>
-  <si>
-    <t>09-Mar-2018 01:22:33</t>
-  </si>
-  <si>
     <t>CFL v4.0</t>
+  </si>
+  <si>
+    <t>9.3.0.701794 (R2017b)</t>
+  </si>
+  <si>
+    <t>10-Mar-2018 01:26:40</t>
   </si>
 </sst>
 </file>
@@ -719,16 +719,16 @@
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -795,28 +795,28 @@
         <v>6</v>
       </c>
       <c r="D4" s="15">
-        <v>2400</v>
+        <v>2388</v>
       </c>
       <c r="E4" s="14">
-        <v>0.505</v>
+        <v>0.81699999999999995</v>
       </c>
       <c r="F4" s="15">
-        <v>2400</v>
+        <v>2388</v>
       </c>
       <c r="G4" s="14">
-        <v>0.25</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="H4" s="15">
-        <v>2400</v>
+        <v>2388</v>
       </c>
       <c r="I4" s="14">
-        <v>0.224</v>
+        <v>0.218</v>
       </c>
       <c r="J4" s="15">
-        <v>2400</v>
+        <v>2388</v>
       </c>
       <c r="K4" s="14">
-        <v>0.20799999999999999</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -833,25 +833,25 @@
         <v>674</v>
       </c>
       <c r="E5" s="11">
-        <v>0.14799999999999999</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F5" s="4">
         <v>959</v>
       </c>
       <c r="G5" s="11">
-        <v>0.11</v>
+        <v>0.113</v>
       </c>
       <c r="H5" s="4">
         <v>731</v>
       </c>
       <c r="I5" s="11">
-        <v>0.124</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="J5" s="4">
         <v>1028</v>
       </c>
       <c r="K5" s="11">
-        <v>0.109</v>
+        <v>0.11700000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -868,25 +868,25 @@
         <v>311</v>
       </c>
       <c r="E6" s="11">
-        <v>0.16300000000000001</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="F6" s="4">
         <v>366</v>
       </c>
       <c r="G6" s="11">
-        <v>8.5000000000000006E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="H6" s="4">
         <v>317</v>
       </c>
       <c r="I6" s="11">
-        <v>7.0999999999999994E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="J6" s="4">
         <v>397</v>
       </c>
       <c r="K6" s="11">
-        <v>7.0999999999999994E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -903,25 +903,25 @@
         <v>3805</v>
       </c>
       <c r="E7" s="11">
-        <v>1.9630000000000001</v>
+        <v>1.7410000000000001</v>
       </c>
       <c r="F7" s="4">
         <v>4908</v>
       </c>
       <c r="G7" s="11">
-        <v>2.7829999999999999</v>
+        <v>2.5369999999999999</v>
       </c>
       <c r="H7" s="4">
         <v>4676</v>
       </c>
       <c r="I7" s="11">
-        <v>2.5830000000000002</v>
+        <v>2.4649999999999999</v>
       </c>
       <c r="J7" s="4">
         <v>6075</v>
       </c>
       <c r="K7" s="11">
-        <v>4.5179999999999998</v>
+        <v>3.585</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -938,25 +938,25 @@
         <v>2040</v>
       </c>
       <c r="E8" s="11">
-        <v>0.44</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="F8" s="4">
         <v>2667</v>
       </c>
       <c r="G8" s="11">
-        <v>0.45700000000000002</v>
+        <v>0.432</v>
       </c>
       <c r="H8" s="4">
         <v>2284</v>
       </c>
       <c r="I8" s="11">
-        <v>0.42</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="J8" s="4">
         <v>2900</v>
       </c>
       <c r="K8" s="11">
-        <v>0.49199999999999999</v>
+        <v>0.45400000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -970,28 +970,28 @@
         <v>1.2</v>
       </c>
       <c r="D9" s="4">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E9" s="11">
-        <v>0.17399999999999999</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="F9" s="4">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="G9" s="11">
-        <v>0.13400000000000001</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="H9" s="4">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="I9" s="11">
-        <v>0.13700000000000001</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="J9" s="4">
-        <v>616</v>
+        <v>587</v>
       </c>
       <c r="K9" s="11">
-        <v>0.13900000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1008,25 +1008,25 @@
         <v>200</v>
       </c>
       <c r="E10" s="11">
-        <v>7.1999999999999995E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F10" s="4">
         <v>207</v>
       </c>
       <c r="G10" s="11">
-        <v>4.9000000000000002E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="H10" s="4">
         <v>213</v>
       </c>
       <c r="I10" s="11">
-        <v>4.2999999999999997E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="J10" s="4">
         <v>221</v>
       </c>
       <c r="K10" s="11">
-        <v>4.2000000000000003E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1043,25 +1043,25 @@
         <v>10055</v>
       </c>
       <c r="E11" s="11">
-        <v>3.5720000000000001</v>
+        <v>2.6930000000000001</v>
       </c>
       <c r="F11" s="4">
         <v>18721</v>
       </c>
       <c r="G11" s="11">
-        <v>8.0489999999999995</v>
+        <v>5.5209999999999999</v>
       </c>
       <c r="H11" s="4">
         <v>12458</v>
       </c>
       <c r="I11" s="11">
-        <v>5.2290000000000001</v>
+        <v>3.8980000000000001</v>
       </c>
       <c r="J11" s="4">
         <v>21338</v>
       </c>
       <c r="K11" s="11">
-        <v>9.423</v>
+        <v>7.165</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1078,7 +1078,7 @@
         <v>1211</v>
       </c>
       <c r="E12" s="11">
-        <v>0.107</v>
+        <v>0.11</v>
       </c>
       <c r="F12" s="4">
         <v>1211</v>
@@ -1090,13 +1090,13 @@
         <v>1211</v>
       </c>
       <c r="I12" s="11">
-        <v>6.5000000000000002E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="J12" s="4">
         <v>1211</v>
       </c>
       <c r="K12" s="11">
-        <v>6.9000000000000006E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1113,25 +1113,25 @@
         <v>1301</v>
       </c>
       <c r="E13" s="11">
-        <v>0.187</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="F13" s="3">
         <v>1411</v>
       </c>
       <c r="G13" s="11">
-        <v>0.20899999999999999</v>
+        <v>0.189</v>
       </c>
       <c r="H13" s="4">
         <v>1396</v>
       </c>
       <c r="I13" s="11">
-        <v>0.161</v>
+        <v>0.17</v>
       </c>
       <c r="J13" s="4">
         <v>1476</v>
       </c>
       <c r="K13" s="11">
-        <v>0.19800000000000001</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1148,25 +1148,25 @@
         <v>5538</v>
       </c>
       <c r="E14" s="11">
-        <v>0.61799999999999999</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="F14" s="3">
         <v>5538</v>
       </c>
       <c r="G14" s="11">
-        <v>0.44800000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="H14" s="4">
         <v>5538</v>
       </c>
       <c r="I14" s="11">
-        <v>0.45100000000000001</v>
+        <v>0.435</v>
       </c>
       <c r="J14" s="4">
         <v>5538</v>
       </c>
       <c r="K14" s="11">
-        <v>0.49099999999999999</v>
+        <v>0.41699999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1189,19 +1189,19 @@
         <v>859</v>
       </c>
       <c r="G15" s="11">
-        <v>0.111</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="H15" s="3">
         <v>807</v>
       </c>
       <c r="I15" s="11">
-        <v>9.2999999999999999E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="J15" s="3">
         <v>934</v>
       </c>
       <c r="K15" s="11">
-        <v>0.107</v>
+        <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1218,25 +1218,25 @@
         <v>1305</v>
       </c>
       <c r="E16" s="11">
-        <v>0.19700000000000001</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="F16" s="3">
         <v>1400</v>
       </c>
       <c r="G16" s="11">
-        <v>0.17899999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="H16" s="3">
         <v>1415</v>
       </c>
       <c r="I16" s="11">
-        <v>0.14599999999999999</v>
+        <v>0.128</v>
       </c>
       <c r="J16" s="3">
         <v>1443</v>
       </c>
       <c r="K16" s="11">
-        <v>0.13900000000000001</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1253,25 +1253,25 @@
         <v>6365</v>
       </c>
       <c r="E17" s="11">
-        <v>2.0619999999999998</v>
+        <v>1.133</v>
       </c>
       <c r="F17" s="3">
         <v>6812</v>
       </c>
       <c r="G17" s="11">
-        <v>1.86</v>
+        <v>1.25</v>
       </c>
       <c r="H17" s="3">
         <v>6022</v>
       </c>
       <c r="I17" s="11">
-        <v>1.6859999999999999</v>
+        <v>1.4079999999999999</v>
       </c>
       <c r="J17" s="3">
         <v>6420</v>
       </c>
       <c r="K17" s="11">
-        <v>1.7849999999999999</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1288,7 +1288,7 @@
         <v>277</v>
       </c>
       <c r="E18" s="11">
-        <v>0.14199999999999999</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F18" s="3">
         <v>307</v>
@@ -1300,13 +1300,13 @@
         <v>314</v>
       </c>
       <c r="I18" s="11">
-        <v>7.4999999999999997E-2</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="J18" s="3">
         <v>334</v>
       </c>
       <c r="K18" s="11">
-        <v>7.8E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1323,25 +1323,25 @@
         <v>3432</v>
       </c>
       <c r="E19" s="11">
-        <v>0.78200000000000003</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="F19" s="3">
         <v>3672</v>
       </c>
       <c r="G19" s="11">
-        <v>0.93400000000000005</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="H19" s="3">
         <v>3544</v>
       </c>
       <c r="I19" s="11">
-        <v>0.89900000000000002</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="J19" s="3">
         <v>3829</v>
       </c>
       <c r="K19" s="11">
-        <v>1.0069999999999999</v>
+        <v>0.82699999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1358,25 +1358,25 @@
         <v>6974</v>
       </c>
       <c r="E20" s="11">
-        <v>1.24</v>
+        <v>0.85299999999999998</v>
       </c>
       <c r="F20" s="3">
         <v>6688</v>
       </c>
       <c r="G20" s="11">
-        <v>1.4450000000000001</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="H20" s="3">
         <v>98588</v>
       </c>
       <c r="I20" s="11">
-        <v>14.33</v>
+        <v>12.75</v>
       </c>
       <c r="J20" s="3">
         <v>99644</v>
       </c>
       <c r="K20" s="11">
-        <v>12.486000000000001</v>
+        <v>16.699000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1393,25 +1393,25 @@
         <v>3637</v>
       </c>
       <c r="E21" s="11">
-        <v>0.54300000000000004</v>
+        <v>0.747</v>
       </c>
       <c r="F21" s="3">
         <v>4630</v>
       </c>
       <c r="G21" s="11">
-        <v>0.70299999999999996</v>
+        <v>1.0209999999999999</v>
       </c>
       <c r="H21" s="3">
         <v>4076</v>
       </c>
       <c r="I21" s="11">
-        <v>0.48099999999999998</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="J21" s="3">
         <v>4180</v>
       </c>
       <c r="K21" s="11">
-        <v>0.47799999999999998</v>
+        <v>0.51200000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1425,28 +1425,28 @@
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <v>2138</v>
+        <v>2054</v>
       </c>
       <c r="E22" s="11">
-        <v>6.4850000000000003</v>
+        <v>4.22</v>
       </c>
       <c r="F22" s="3">
-        <v>2138</v>
+        <v>2054</v>
       </c>
       <c r="G22" s="11">
-        <v>6.3029999999999999</v>
+        <v>4.16</v>
       </c>
       <c r="H22" s="3">
-        <v>2138</v>
+        <v>2054</v>
       </c>
       <c r="I22" s="11">
-        <v>5.94</v>
+        <v>4.8650000000000002</v>
       </c>
       <c r="J22" s="3">
-        <v>2138</v>
+        <v>2054</v>
       </c>
       <c r="K22" s="11">
-        <v>7.0640000000000001</v>
+        <v>5.6779999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1463,25 +1463,25 @@
         <v>3145</v>
       </c>
       <c r="E23" s="11">
-        <v>1.5109999999999999</v>
+        <v>1.1859999999999999</v>
       </c>
       <c r="F23" s="3">
         <v>3164</v>
       </c>
       <c r="G23" s="11">
-        <v>1.2909999999999999</v>
+        <v>1.2450000000000001</v>
       </c>
       <c r="H23" s="3">
         <v>3721</v>
       </c>
       <c r="I23" s="11">
-        <v>1.5580000000000001</v>
+        <v>1.4690000000000001</v>
       </c>
       <c r="J23" s="3">
         <v>3684</v>
       </c>
       <c r="K23" s="11">
-        <v>1.4610000000000001</v>
+        <v>1.804</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1498,25 +1498,25 @@
         <v>131</v>
       </c>
       <c r="E24" s="11">
-        <v>0.13900000000000001</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="F24" s="3">
         <v>131</v>
       </c>
       <c r="G24" s="11">
-        <v>5.1999999999999998E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="H24" s="3">
         <v>131</v>
       </c>
       <c r="I24" s="11">
-        <v>5.0999999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="J24" s="3">
         <v>131</v>
       </c>
       <c r="K24" s="11">
-        <v>4.9000000000000002E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1533,25 +1533,25 @@
         <v>4741</v>
       </c>
       <c r="E25" s="11">
-        <v>4.3620000000000001</v>
+        <v>3.4550000000000001</v>
       </c>
       <c r="F25" s="3">
         <v>5224</v>
       </c>
       <c r="G25" s="11">
-        <v>5.1769999999999996</v>
+        <v>3.8879999999999999</v>
       </c>
       <c r="H25" s="3">
         <v>4567</v>
       </c>
       <c r="I25" s="11">
-        <v>4.5149999999999997</v>
+        <v>3.6640000000000001</v>
       </c>
       <c r="J25" s="3">
         <v>5136</v>
       </c>
       <c r="K25" s="11">
-        <v>5.3010000000000002</v>
+        <v>4.1959999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1568,25 +1568,25 @@
         <v>13792</v>
       </c>
       <c r="E26" s="11">
-        <v>8.0649999999999995</v>
+        <v>5.9790000000000001</v>
       </c>
       <c r="F26" s="3">
         <v>14308</v>
       </c>
       <c r="G26" s="11">
-        <v>8.1969999999999992</v>
+        <v>7.7969999999999997</v>
       </c>
       <c r="H26" s="3">
         <v>19430</v>
       </c>
       <c r="I26" s="11">
-        <v>11.334</v>
+        <v>14.406000000000001</v>
       </c>
       <c r="J26" s="3">
         <v>23305</v>
       </c>
       <c r="K26" s="11">
-        <v>13.595000000000001</v>
+        <v>11.862</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1603,25 +1603,25 @@
         <v>3423</v>
       </c>
       <c r="E27" s="11">
-        <v>2.4910000000000001</v>
+        <v>2.8260000000000001</v>
       </c>
       <c r="F27" s="3">
         <v>4110</v>
       </c>
       <c r="G27" s="11">
-        <v>3.7050000000000001</v>
+        <v>4.2590000000000003</v>
       </c>
       <c r="H27" s="3">
         <v>3479</v>
       </c>
       <c r="I27" s="11">
-        <v>2.6230000000000002</v>
+        <v>2.0910000000000002</v>
       </c>
       <c r="J27" s="3">
         <v>4217</v>
       </c>
       <c r="K27" s="11">
-        <v>3.8109999999999999</v>
+        <v>3.3010000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1638,25 +1638,25 @@
         <v>940</v>
       </c>
       <c r="E28" s="11">
-        <v>0.17</v>
+        <v>0.151</v>
       </c>
       <c r="F28" s="3">
         <v>1024</v>
       </c>
       <c r="G28" s="11">
-        <v>0.14299999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H28" s="3">
         <v>967</v>
       </c>
       <c r="I28" s="11">
-        <v>0.112</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="J28" s="3">
         <v>1060</v>
       </c>
       <c r="K28" s="11">
-        <v>0.17100000000000001</v>
+        <v>0.17399999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1673,25 +1673,25 @@
         <v>756</v>
       </c>
       <c r="E29" s="11">
-        <v>0.16500000000000001</v>
+        <v>0.152</v>
       </c>
       <c r="F29" s="3">
         <v>863</v>
       </c>
       <c r="G29" s="11">
-        <v>0.16400000000000001</v>
+        <v>0.151</v>
       </c>
       <c r="H29" s="3">
         <v>786</v>
       </c>
       <c r="I29" s="11">
-        <v>0.20499999999999999</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="J29" s="3">
         <v>896</v>
       </c>
       <c r="K29" s="11">
-        <v>0.17</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1708,25 +1708,25 @@
         <v>10344</v>
       </c>
       <c r="E30" s="11">
-        <v>16.177</v>
+        <v>12.112</v>
       </c>
       <c r="F30" s="3">
         <v>12311</v>
       </c>
       <c r="G30" s="11">
-        <v>29.396000000000001</v>
+        <v>22.838000000000001</v>
       </c>
       <c r="H30" s="3">
         <v>11682</v>
       </c>
       <c r="I30" s="11">
-        <v>23.045000000000002</v>
+        <v>18.12</v>
       </c>
       <c r="J30" s="3">
         <v>13340</v>
       </c>
       <c r="K30" s="11">
-        <v>40.973999999999997</v>
+        <v>28.736999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1743,25 +1743,25 @@
         <v>882</v>
       </c>
       <c r="E31" s="11">
-        <v>0.28199999999999997</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="F31" s="3">
         <v>910</v>
       </c>
       <c r="G31" s="11">
-        <v>0.24299999999999999</v>
+        <v>0.219</v>
       </c>
       <c r="H31" s="3">
         <v>879</v>
       </c>
       <c r="I31" s="11">
-        <v>0.255</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="J31" s="3">
         <v>949</v>
       </c>
       <c r="K31" s="11">
-        <v>0.245</v>
+        <v>0.22500000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1778,25 +1778,25 @@
         <v>2429</v>
       </c>
       <c r="E32" s="11">
-        <v>1.3360000000000001</v>
+        <v>1.39</v>
       </c>
       <c r="F32" s="3">
         <v>5534</v>
       </c>
       <c r="G32" s="11">
-        <v>10.211</v>
+        <v>8.7729999999999997</v>
       </c>
       <c r="H32" s="3">
         <v>2519</v>
       </c>
       <c r="I32" s="11">
-        <v>1.56</v>
+        <v>1.36</v>
       </c>
       <c r="J32" s="3">
         <v>6071</v>
       </c>
       <c r="K32" s="11">
-        <v>11.276999999999999</v>
+        <v>11.234</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1813,25 +1813,25 @@
         <v>2640</v>
       </c>
       <c r="E33" s="11">
-        <v>0.55100000000000005</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="F33" s="3">
         <v>4082</v>
       </c>
       <c r="G33" s="11">
-        <v>1.1200000000000001</v>
+        <v>1.302</v>
       </c>
       <c r="H33" s="3">
         <v>3035</v>
       </c>
       <c r="I33" s="11">
-        <v>0.64100000000000001</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="J33" s="3">
         <v>4410</v>
       </c>
       <c r="K33" s="11">
-        <v>1.125</v>
+        <v>1.3149999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1848,25 +1848,25 @@
         <v>431</v>
       </c>
       <c r="E34" s="11">
-        <v>0.189</v>
+        <v>0.27</v>
       </c>
       <c r="F34" s="3">
         <v>740</v>
       </c>
       <c r="G34" s="11">
-        <v>0.43</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="H34" s="3">
         <v>505</v>
       </c>
       <c r="I34" s="11">
-        <v>0.14799999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="J34" s="3">
         <v>828</v>
       </c>
       <c r="K34" s="11">
-        <v>0.46800000000000003</v>
+        <v>0.57199999999999995</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1883,25 +1883,25 @@
         <v>1664</v>
       </c>
       <c r="E35" s="11">
-        <v>0.38700000000000001</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="F35" s="3">
         <v>3056</v>
       </c>
       <c r="G35" s="11">
-        <v>1.02</v>
+        <v>1.482</v>
       </c>
       <c r="H35" s="3">
         <v>1734</v>
       </c>
       <c r="I35" s="11">
-        <v>0.35499999999999998</v>
+        <v>0.52700000000000002</v>
       </c>
       <c r="J35" s="3">
         <v>3296</v>
       </c>
       <c r="K35" s="11">
-        <v>1.1559999999999999</v>
+        <v>1.5980000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1918,25 +1918,25 @@
         <v>4550</v>
       </c>
       <c r="E36" s="11">
-        <v>0.95</v>
+        <v>1.5660000000000001</v>
       </c>
       <c r="F36" s="3">
         <v>6830</v>
       </c>
       <c r="G36" s="11">
-        <v>2.3690000000000002</v>
+        <v>3.7970000000000002</v>
       </c>
       <c r="H36" s="3">
         <v>4544</v>
       </c>
       <c r="I36" s="11">
-        <v>1.1020000000000001</v>
+        <v>1.3140000000000001</v>
       </c>
       <c r="J36" s="3">
         <v>6909</v>
       </c>
       <c r="K36" s="11">
-        <v>2.286</v>
+        <v>3.5619999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1953,25 +1953,25 @@
         <v>5609</v>
       </c>
       <c r="E37" s="11">
-        <v>0.76400000000000001</v>
+        <v>1.0449999999999999</v>
       </c>
       <c r="F37" s="3">
         <v>8295</v>
       </c>
       <c r="G37" s="11">
-        <v>2.8929999999999998</v>
+        <v>3.6859999999999999</v>
       </c>
       <c r="H37" s="3">
         <v>5673</v>
       </c>
       <c r="I37" s="11">
-        <v>0.83099999999999996</v>
+        <v>1.1140000000000001</v>
       </c>
       <c r="J37" s="3">
         <v>8346</v>
       </c>
       <c r="K37" s="11">
-        <v>3.0489999999999999</v>
+        <v>3.5840000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1988,25 +1988,25 @@
         <v>4175</v>
       </c>
       <c r="E38" s="11">
-        <v>1.2569999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F38" s="3">
         <v>4689</v>
       </c>
       <c r="G38" s="11">
-        <v>1.8260000000000001</v>
+        <v>1.7430000000000001</v>
       </c>
       <c r="H38" s="3">
         <v>4256</v>
       </c>
       <c r="I38" s="11">
-        <v>1.41</v>
+        <v>1.43</v>
       </c>
       <c r="J38" s="3">
         <v>4785</v>
       </c>
       <c r="K38" s="11">
-        <v>1.996</v>
+        <v>2.0430000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2023,25 +2023,25 @@
         <v>4912</v>
       </c>
       <c r="E39" s="11">
-        <v>0.64800000000000002</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="F39" s="3">
         <v>5361</v>
       </c>
       <c r="G39" s="11">
-        <v>1.0389999999999999</v>
+        <v>1.042</v>
       </c>
       <c r="H39" s="3">
         <v>4945</v>
       </c>
       <c r="I39" s="11">
-        <v>0.72499999999999998</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="J39" s="3">
         <v>5193</v>
       </c>
       <c r="K39" s="11">
-        <v>0.91400000000000003</v>
+        <v>0.84699999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2058,25 +2058,25 @@
         <v>4204</v>
       </c>
       <c r="E40" s="11">
-        <v>2.1320000000000001</v>
+        <v>1.8939999999999999</v>
       </c>
       <c r="F40" s="3">
         <v>4542</v>
       </c>
       <c r="G40" s="11">
-        <v>2.8029999999999999</v>
+        <v>2.6259999999999999</v>
       </c>
       <c r="H40" s="3">
         <v>4219</v>
       </c>
       <c r="I40" s="11">
-        <v>2.133</v>
+        <v>2.077</v>
       </c>
       <c r="J40" s="3">
         <v>4511</v>
       </c>
       <c r="K40" s="11">
-        <v>2.718</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2093,25 +2093,25 @@
         <v>4601</v>
       </c>
       <c r="E41" s="11">
-        <v>1.5529999999999999</v>
+        <v>1.5880000000000001</v>
       </c>
       <c r="F41" s="3">
         <v>4596</v>
       </c>
       <c r="G41" s="11">
-        <v>1.976</v>
+        <v>1.9379999999999999</v>
       </c>
       <c r="H41" s="3">
         <v>4746</v>
       </c>
       <c r="I41" s="11">
-        <v>1.655</v>
+        <v>1.659</v>
       </c>
       <c r="J41" s="3">
         <v>4534</v>
       </c>
       <c r="K41" s="11">
-        <v>1.9550000000000001</v>
+        <v>1.9490000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2128,25 +2128,25 @@
         <v>6024</v>
       </c>
       <c r="E42" s="11">
-        <v>0.99099999999999999</v>
+        <v>1.044</v>
       </c>
       <c r="F42" s="3">
         <v>6409</v>
       </c>
       <c r="G42" s="11">
-        <v>1.361</v>
+        <v>1.373</v>
       </c>
       <c r="H42" s="3">
         <v>6388</v>
       </c>
       <c r="I42" s="11">
-        <v>1.0720000000000001</v>
+        <v>1.17</v>
       </c>
       <c r="J42" s="3">
         <v>6740</v>
       </c>
       <c r="K42" s="11">
-        <v>1.46</v>
+        <v>1.3340000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2163,25 +2163,25 @@
         <v>1231</v>
       </c>
       <c r="E43" s="11">
-        <v>0.45200000000000001</v>
+        <v>0.51</v>
       </c>
       <c r="F43" s="3">
         <v>1386</v>
       </c>
       <c r="G43" s="11">
-        <v>0.54300000000000004</v>
+        <v>0.63100000000000001</v>
       </c>
       <c r="H43" s="3">
         <v>1249</v>
       </c>
       <c r="I43" s="11">
-        <v>0.45400000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="J43" s="3">
         <v>1525</v>
       </c>
       <c r="K43" s="11">
-        <v>0.79800000000000004</v>
+        <v>0.58699999999999997</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2195,28 +2195,28 @@
         <v>24</v>
       </c>
       <c r="D44" s="4">
-        <v>8147</v>
+        <v>8079</v>
       </c>
       <c r="E44" s="11">
-        <v>5.4169999999999998</v>
+        <v>4.0830000000000002</v>
       </c>
       <c r="F44" s="3">
-        <v>6557</v>
+        <v>6536</v>
       </c>
       <c r="G44" s="11">
-        <v>7.7069999999999999</v>
+        <v>6.5670000000000002</v>
       </c>
       <c r="H44" s="3">
-        <v>8243</v>
+        <v>8134</v>
       </c>
       <c r="I44" s="11">
-        <v>5.335</v>
+        <v>4.5940000000000003</v>
       </c>
       <c r="J44" s="3">
-        <v>6634</v>
+        <v>6691</v>
       </c>
       <c r="K44" s="11">
-        <v>8.2360000000000007</v>
+        <v>6.5279999999999996</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2233,25 +2233,25 @@
         <v>4891</v>
       </c>
       <c r="E45" s="11">
-        <v>6.0960000000000001</v>
+        <v>5.2539999999999996</v>
       </c>
       <c r="F45" s="3">
         <v>4891</v>
       </c>
       <c r="G45" s="11">
-        <v>6.0869999999999997</v>
+        <v>4.9960000000000004</v>
       </c>
       <c r="H45" s="3">
         <v>4891</v>
       </c>
       <c r="I45" s="11">
-        <v>6.0830000000000002</v>
+        <v>5.2389999999999999</v>
       </c>
       <c r="J45" s="3">
         <v>4891</v>
       </c>
       <c r="K45" s="11">
-        <v>6.1260000000000003</v>
+        <v>5.3620000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2268,25 +2268,25 @@
         <v>2463</v>
       </c>
       <c r="E46" s="11">
-        <v>24.542000000000002</v>
+        <v>20.614000000000001</v>
       </c>
       <c r="F46" s="3">
         <v>2463</v>
       </c>
       <c r="G46" s="11">
-        <v>25.917000000000002</v>
+        <v>20.388999999999999</v>
       </c>
       <c r="H46" s="3">
         <v>2463</v>
       </c>
       <c r="I46" s="11">
-        <v>26.273</v>
+        <v>21.419</v>
       </c>
       <c r="J46" s="3">
         <v>2463</v>
       </c>
       <c r="K46" s="11">
-        <v>25.462</v>
+        <v>21.561</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2303,7 +2303,7 @@
         <v>8856</v>
       </c>
       <c r="E47" s="11">
-        <v>4.5309999999999997</v>
+        <v>4.0780000000000003</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>44</v>
@@ -2338,7 +2338,7 @@
         <v>8467</v>
       </c>
       <c r="E48" s="11">
-        <v>6.093</v>
+        <v>4.8129999999999997</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>44</v>
@@ -2373,7 +2373,7 @@
         <v>14844</v>
       </c>
       <c r="E49" s="11">
-        <v>10.676</v>
+        <v>9.0589999999999993</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>44</v>
@@ -2408,7 +2408,7 @@
         <v>11309</v>
       </c>
       <c r="E50" s="11">
-        <v>8.7360000000000007</v>
+        <v>7.335</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>44</v>
@@ -2443,7 +2443,7 @@
         <v>9052</v>
       </c>
       <c r="E51" s="11">
-        <v>5.5179999999999998</v>
+        <v>4.6360000000000001</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>44</v>
@@ -2478,7 +2478,7 @@
         <v>12326</v>
       </c>
       <c r="E52" s="11">
-        <v>13.411</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>44</v>
@@ -2513,7 +2513,7 @@
         <v>11073</v>
       </c>
       <c r="E53" s="11">
-        <v>8.609</v>
+        <v>7.3840000000000003</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>44</v>
@@ -2548,7 +2548,7 @@
         <v>12191</v>
       </c>
       <c r="E54" s="11">
-        <v>13.792999999999999</v>
+        <v>12.08</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>44</v>
@@ -2583,7 +2583,7 @@
         <v>9011</v>
       </c>
       <c r="E55" s="11">
-        <v>9.0809999999999995</v>
+        <v>8.0820000000000007</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>44</v>
@@ -2618,17 +2618,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100525B94EEF47D42499A62120CC90E0AB3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e706cd362d7e41030bb8c72a7c62a9d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c85acdc-a394-4ae0-8c72-fb4a95b3d573" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55e2521e7df4d5c11309cefaa7c01562" ns2:_="">
     <xsd:import namespace="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
@@ -2773,16 +2762,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2828,10 +2819,29 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2853,35 +2863,25 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE6D0D52-57FE-48CB-8E43-11384E6CFEE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630E037-F79E-4175-B540-A23B306F8900}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE6D0D52-57FE-48CB-8E43-11384E6CFEE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Initial commit R2018a.  Version 4.1
</commit_message>
<xml_diff>
--- a/Scripts_Data/CFR_Results.xlsx
+++ b/Scripts_Data/CFR_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R17b\Scripts_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R18a\Scripts_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -210,13 +210,13 @@
     <t>Frict3D_08_Ball_on_Driven_Tube</t>
   </si>
   <si>
+    <t>9.4.0.813654 (R2018a)</t>
+  </si>
+  <si>
     <t>CFL v4.0</t>
   </si>
   <si>
-    <t>9.3.0.701794 (R2017b)</t>
-  </si>
-  <si>
-    <t>10-Mar-2018 01:26:40</t>
+    <t>09-Mar-2018 23:51:33</t>
   </si>
 </sst>
 </file>
@@ -700,7 +700,7 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3:K55"/>
@@ -719,7 +719,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -728,7 +728,7 @@
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -798,25 +798,25 @@
         <v>2388</v>
       </c>
       <c r="E4" s="14">
-        <v>0.81699999999999995</v>
+        <v>2.9830000000000001</v>
       </c>
       <c r="F4" s="15">
         <v>2388</v>
       </c>
       <c r="G4" s="14">
-        <v>0.20200000000000001</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="H4" s="15">
         <v>2388</v>
       </c>
       <c r="I4" s="14">
-        <v>0.218</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="J4" s="15">
         <v>2388</v>
       </c>
       <c r="K4" s="14">
-        <v>0.188</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -830,28 +830,28 @@
         <v>4</v>
       </c>
       <c r="D5" s="4">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="E5" s="11">
-        <v>0.56999999999999995</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="F5" s="4">
-        <v>959</v>
+        <v>929</v>
       </c>
       <c r="G5" s="11">
-        <v>0.113</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="H5" s="4">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="I5" s="11">
-        <v>0.10299999999999999</v>
+        <v>0.123</v>
       </c>
       <c r="J5" s="4">
-        <v>1028</v>
+        <v>1020</v>
       </c>
       <c r="K5" s="11">
-        <v>0.11700000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -865,28 +865,28 @@
         <v>1.5</v>
       </c>
       <c r="D6" s="4">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="E6" s="11">
-        <v>0.21099999999999999</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="F6" s="4">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="G6" s="11">
-        <v>7.1999999999999995E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="H6" s="4">
         <v>317</v>
       </c>
       <c r="I6" s="11">
-        <v>6.5000000000000002E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="J6" s="4">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="K6" s="11">
-        <v>8.2000000000000003E-2</v>
+        <v>0.11600000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -900,28 +900,28 @@
         <v>3</v>
       </c>
       <c r="D7" s="4">
-        <v>3805</v>
+        <v>3726</v>
       </c>
       <c r="E7" s="11">
-        <v>1.7410000000000001</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="F7" s="4">
-        <v>4908</v>
+        <v>4928</v>
       </c>
       <c r="G7" s="11">
-        <v>2.5369999999999999</v>
+        <v>3.048</v>
       </c>
       <c r="H7" s="4">
-        <v>4676</v>
+        <v>5039</v>
       </c>
       <c r="I7" s="11">
-        <v>2.4649999999999999</v>
+        <v>3.5009999999999999</v>
       </c>
       <c r="J7" s="4">
-        <v>6075</v>
+        <v>6295</v>
       </c>
       <c r="K7" s="11">
-        <v>3.585</v>
+        <v>4.8639999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -935,28 +935,28 @@
         <v>5</v>
       </c>
       <c r="D8" s="4">
-        <v>2040</v>
+        <v>2096</v>
       </c>
       <c r="E8" s="11">
-        <v>0.36399999999999999</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="F8" s="4">
-        <v>2667</v>
+        <v>2794</v>
       </c>
       <c r="G8" s="11">
-        <v>0.432</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="H8" s="4">
-        <v>2284</v>
+        <v>2425</v>
       </c>
       <c r="I8" s="11">
-        <v>0.39600000000000002</v>
+        <v>0.48299999999999998</v>
       </c>
       <c r="J8" s="4">
-        <v>2900</v>
+        <v>3210</v>
       </c>
       <c r="K8" s="11">
-        <v>0.45400000000000001</v>
+        <v>0.69699999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -970,28 +970,28 @@
         <v>1.2</v>
       </c>
       <c r="D9" s="4">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E9" s="11">
-        <v>0.17499999999999999</v>
+        <v>0.26</v>
       </c>
       <c r="F9" s="4">
-        <v>603</v>
+        <v>579</v>
       </c>
       <c r="G9" s="11">
-        <v>0.14699999999999999</v>
+        <v>0.154</v>
       </c>
       <c r="H9" s="4">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="I9" s="11">
-        <v>0.13600000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="J9" s="4">
-        <v>587</v>
+        <v>602</v>
       </c>
       <c r="K9" s="11">
-        <v>0.13</v>
+        <v>0.17799999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1005,28 +1005,28 @@
         <v>1.5</v>
       </c>
       <c r="D10" s="4">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="E10" s="11">
-        <v>6.5000000000000002E-2</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="F10" s="4">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="G10" s="11">
-        <v>4.4999999999999998E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="H10" s="4">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="I10" s="11">
-        <v>4.2000000000000003E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="J10" s="4">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="K10" s="11">
-        <v>4.4999999999999998E-2</v>
+        <v>0.28199999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1040,28 +1040,28 @@
         <v>5</v>
       </c>
       <c r="D11" s="4">
-        <v>10055</v>
+        <v>9225</v>
       </c>
       <c r="E11" s="11">
-        <v>2.6930000000000001</v>
+        <v>4.7</v>
       </c>
       <c r="F11" s="4">
-        <v>18721</v>
+        <v>17963</v>
       </c>
       <c r="G11" s="11">
-        <v>5.5209999999999999</v>
+        <v>13.412000000000001</v>
       </c>
       <c r="H11" s="4">
-        <v>12458</v>
+        <v>10816</v>
       </c>
       <c r="I11" s="11">
-        <v>3.8980000000000001</v>
+        <v>5.4139999999999997</v>
       </c>
       <c r="J11" s="4">
-        <v>21338</v>
+        <v>21376</v>
       </c>
       <c r="K11" s="11">
-        <v>7.165</v>
+        <v>11.554</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1078,25 +1078,25 @@
         <v>1211</v>
       </c>
       <c r="E12" s="11">
-        <v>0.11</v>
+        <v>0.115</v>
       </c>
       <c r="F12" s="4">
         <v>1211</v>
       </c>
       <c r="G12" s="11">
-        <v>6.8000000000000005E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="H12" s="4">
         <v>1211</v>
       </c>
       <c r="I12" s="11">
-        <v>6.9000000000000006E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="J12" s="4">
         <v>1211</v>
       </c>
       <c r="K12" s="11">
-        <v>6.7000000000000004E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1110,28 +1110,28 @@
         <v>10</v>
       </c>
       <c r="D13" s="4">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="E13" s="11">
-        <v>0.16700000000000001</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="F13" s="3">
-        <v>1411</v>
+        <v>1444</v>
       </c>
       <c r="G13" s="11">
-        <v>0.189</v>
+        <v>0.215</v>
       </c>
       <c r="H13" s="4">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="I13" s="11">
-        <v>0.17</v>
+        <v>0.184</v>
       </c>
       <c r="J13" s="4">
-        <v>1476</v>
+        <v>1516</v>
       </c>
       <c r="K13" s="11">
-        <v>0.214</v>
+        <v>0.245</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1145,28 +1145,28 @@
         <v>45</v>
       </c>
       <c r="D14" s="4">
-        <v>5538</v>
+        <v>5568</v>
       </c>
       <c r="E14" s="11">
-        <v>0.42599999999999999</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="F14" s="3">
-        <v>5538</v>
+        <v>5568</v>
       </c>
       <c r="G14" s="11">
-        <v>0.4</v>
+        <v>0.62</v>
       </c>
       <c r="H14" s="4">
-        <v>5538</v>
+        <v>5568</v>
       </c>
       <c r="I14" s="11">
-        <v>0.435</v>
+        <v>0.51100000000000001</v>
       </c>
       <c r="J14" s="4">
-        <v>5538</v>
+        <v>5568</v>
       </c>
       <c r="K14" s="11">
-        <v>0.41699999999999998</v>
+        <v>0.51800000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1180,28 +1180,28 @@
         <v>4</v>
       </c>
       <c r="D15" s="4">
-        <v>732</v>
+        <v>721</v>
       </c>
       <c r="E15" s="11">
-        <v>0.13400000000000001</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="F15" s="3">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="G15" s="11">
-        <v>9.1999999999999998E-2</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="H15" s="3">
-        <v>807</v>
+        <v>800</v>
       </c>
       <c r="I15" s="11">
-        <v>8.1000000000000003E-2</v>
+        <v>0.109</v>
       </c>
       <c r="J15" s="3">
-        <v>934</v>
+        <v>941</v>
       </c>
       <c r="K15" s="11">
-        <v>9.7000000000000003E-2</v>
+        <v>0.13800000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1215,28 +1215,28 @@
         <v>10</v>
       </c>
       <c r="D16" s="4">
-        <v>1305</v>
+        <v>1314</v>
       </c>
       <c r="E16" s="11">
-        <v>0.13500000000000001</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="F16" s="3">
-        <v>1400</v>
+        <v>1404</v>
       </c>
       <c r="G16" s="11">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1396</v>
+      </c>
+      <c r="I16" s="11">
         <v>0.13300000000000001</v>
       </c>
-      <c r="H16" s="3">
-        <v>1415</v>
-      </c>
-      <c r="I16" s="11">
-        <v>0.128</v>
-      </c>
       <c r="J16" s="3">
-        <v>1443</v>
+        <v>1456</v>
       </c>
       <c r="K16" s="11">
-        <v>0.13200000000000001</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1250,28 +1250,28 @@
         <v>15</v>
       </c>
       <c r="D17" s="4">
-        <v>6365</v>
+        <v>6367</v>
       </c>
       <c r="E17" s="11">
-        <v>1.133</v>
+        <v>1.7849999999999999</v>
       </c>
       <c r="F17" s="3">
-        <v>6812</v>
+        <v>6644</v>
       </c>
       <c r="G17" s="11">
-        <v>1.25</v>
+        <v>1.825</v>
       </c>
       <c r="H17" s="3">
-        <v>6022</v>
+        <v>6035</v>
       </c>
       <c r="I17" s="11">
-        <v>1.4079999999999999</v>
+        <v>1.73</v>
       </c>
       <c r="J17" s="3">
-        <v>6420</v>
+        <v>6527</v>
       </c>
       <c r="K17" s="11">
-        <v>1.47</v>
+        <v>2.4590000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1285,25 +1285,25 @@
         <v>2</v>
       </c>
       <c r="D18" s="4">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="E18" s="11">
-        <v>0.10100000000000001</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="F18" s="3">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G18" s="11">
-        <v>6.9000000000000006E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="H18" s="3">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I18" s="11">
-        <v>0.13100000000000001</v>
+        <v>0.104</v>
       </c>
       <c r="J18" s="3">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="K18" s="11">
         <v>9.8000000000000004E-2</v>
@@ -1320,28 +1320,28 @@
         <v>30</v>
       </c>
       <c r="D19" s="4">
-        <v>3432</v>
+        <v>3439</v>
       </c>
       <c r="E19" s="11">
-        <v>0.59199999999999997</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="F19" s="3">
-        <v>3672</v>
+        <v>3749</v>
       </c>
       <c r="G19" s="11">
-        <v>0.73499999999999999</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="H19" s="3">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="I19" s="11">
-        <v>0.76900000000000002</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="J19" s="3">
-        <v>3829</v>
+        <v>3754</v>
       </c>
       <c r="K19" s="11">
-        <v>0.82699999999999996</v>
+        <v>1.008</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1355,28 +1355,28 @@
         <v>50</v>
       </c>
       <c r="D20" s="4">
-        <v>6974</v>
+        <v>7116</v>
       </c>
       <c r="E20" s="11">
-        <v>0.85299999999999998</v>
+        <v>1.2230000000000001</v>
       </c>
       <c r="F20" s="3">
-        <v>6688</v>
+        <v>7227</v>
       </c>
       <c r="G20" s="11">
-        <v>0.85899999999999999</v>
+        <v>1.208</v>
       </c>
       <c r="H20" s="3">
-        <v>98588</v>
+        <v>99561</v>
       </c>
       <c r="I20" s="11">
-        <v>12.75</v>
+        <v>12.928000000000001</v>
       </c>
       <c r="J20" s="3">
-        <v>99644</v>
+        <v>206549</v>
       </c>
       <c r="K20" s="11">
-        <v>16.699000000000002</v>
+        <v>32.481000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1390,28 +1390,28 @@
         <v>30</v>
       </c>
       <c r="D21" s="4">
-        <v>3637</v>
+        <v>3715</v>
       </c>
       <c r="E21" s="11">
-        <v>0.747</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="F21" s="3">
-        <v>4630</v>
+        <v>4719</v>
       </c>
       <c r="G21" s="11">
-        <v>1.0209999999999999</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="H21" s="3">
-        <v>4076</v>
+        <v>3988</v>
       </c>
       <c r="I21" s="11">
-        <v>0.64300000000000002</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="J21" s="3">
-        <v>4180</v>
+        <v>3942</v>
       </c>
       <c r="K21" s="11">
-        <v>0.51200000000000001</v>
+        <v>0.63500000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1425,28 +1425,28 @@
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <v>2054</v>
+        <v>2511</v>
       </c>
       <c r="E22" s="11">
-        <v>4.22</v>
+        <v>7.1980000000000004</v>
       </c>
       <c r="F22" s="3">
-        <v>2054</v>
+        <v>2511</v>
       </c>
       <c r="G22" s="11">
-        <v>4.16</v>
+        <v>6.6710000000000003</v>
       </c>
       <c r="H22" s="3">
-        <v>2054</v>
+        <v>2511</v>
       </c>
       <c r="I22" s="11">
-        <v>4.8650000000000002</v>
+        <v>6.9390000000000001</v>
       </c>
       <c r="J22" s="3">
-        <v>2054</v>
+        <v>2511</v>
       </c>
       <c r="K22" s="11">
-        <v>5.6779999999999999</v>
+        <v>6.6619999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1460,28 +1460,28 @@
         <v>15</v>
       </c>
       <c r="D23" s="4">
-        <v>3145</v>
+        <v>3105</v>
       </c>
       <c r="E23" s="11">
-        <v>1.1859999999999999</v>
+        <v>1.748</v>
       </c>
       <c r="F23" s="3">
-        <v>3164</v>
+        <v>2987</v>
       </c>
       <c r="G23" s="11">
-        <v>1.2450000000000001</v>
+        <v>1.3879999999999999</v>
       </c>
       <c r="H23" s="3">
-        <v>3721</v>
+        <v>3783</v>
       </c>
       <c r="I23" s="11">
-        <v>1.4690000000000001</v>
+        <v>1.8560000000000001</v>
       </c>
       <c r="J23" s="3">
-        <v>3684</v>
+        <v>3676</v>
       </c>
       <c r="K23" s="11">
-        <v>1.804</v>
+        <v>1.845</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1498,25 +1498,25 @@
         <v>131</v>
       </c>
       <c r="E24" s="11">
-        <v>0.14499999999999999</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="F24" s="3">
         <v>131</v>
       </c>
       <c r="G24" s="11">
-        <v>5.7000000000000002E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="H24" s="3">
         <v>131</v>
       </c>
       <c r="I24" s="11">
-        <v>5.8000000000000003E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="J24" s="3">
         <v>131</v>
       </c>
       <c r="K24" s="11">
-        <v>5.1999999999999998E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1530,28 +1530,28 @@
         <v>30</v>
       </c>
       <c r="D25" s="4">
-        <v>4741</v>
+        <v>4739</v>
       </c>
       <c r="E25" s="11">
-        <v>3.4550000000000001</v>
+        <v>4.5739999999999998</v>
       </c>
       <c r="F25" s="3">
-        <v>5224</v>
+        <v>5195</v>
       </c>
       <c r="G25" s="11">
-        <v>3.8879999999999999</v>
+        <v>5.0220000000000002</v>
       </c>
       <c r="H25" s="3">
-        <v>4567</v>
+        <v>4547</v>
       </c>
       <c r="I25" s="11">
-        <v>3.6640000000000001</v>
+        <v>4.5960000000000001</v>
       </c>
       <c r="J25" s="3">
-        <v>5136</v>
+        <v>5128</v>
       </c>
       <c r="K25" s="11">
-        <v>4.1959999999999997</v>
+        <v>5.3920000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1565,28 +1565,28 @@
         <v>12</v>
       </c>
       <c r="D26" s="4">
-        <v>13792</v>
+        <v>13132</v>
       </c>
       <c r="E26" s="11">
-        <v>5.9790000000000001</v>
+        <v>7.1529999999999996</v>
       </c>
       <c r="F26" s="3">
-        <v>14308</v>
+        <v>14228</v>
       </c>
       <c r="G26" s="11">
-        <v>7.7969999999999997</v>
+        <v>8.41</v>
       </c>
       <c r="H26" s="3">
-        <v>19430</v>
+        <v>18990</v>
       </c>
       <c r="I26" s="11">
-        <v>14.406000000000001</v>
+        <v>10.222</v>
       </c>
       <c r="J26" s="3">
-        <v>23305</v>
+        <v>18458</v>
       </c>
       <c r="K26" s="11">
-        <v>11.862</v>
+        <v>9.923</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1600,28 +1600,28 @@
         <v>20</v>
       </c>
       <c r="D27" s="9">
-        <v>3423</v>
+        <v>3433</v>
       </c>
       <c r="E27" s="11">
-        <v>2.8260000000000001</v>
+        <v>2.4710000000000001</v>
       </c>
       <c r="F27" s="3">
-        <v>4110</v>
+        <v>4404</v>
       </c>
       <c r="G27" s="11">
-        <v>4.2590000000000003</v>
+        <v>4.2169999999999996</v>
       </c>
       <c r="H27" s="3">
-        <v>3479</v>
+        <v>3534</v>
       </c>
       <c r="I27" s="11">
-        <v>2.0910000000000002</v>
+        <v>2.5720000000000001</v>
       </c>
       <c r="J27" s="3">
-        <v>4217</v>
+        <v>4409</v>
       </c>
       <c r="K27" s="11">
-        <v>3.3010000000000002</v>
+        <v>3.915</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1635,28 +1635,28 @@
         <v>7.5</v>
       </c>
       <c r="D28" s="4">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="E28" s="11">
-        <v>0.151</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F28" s="3">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="G28" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.152</v>
       </c>
       <c r="H28" s="3">
         <v>967</v>
       </c>
       <c r="I28" s="11">
-        <v>0.16500000000000001</v>
+        <v>0.121</v>
       </c>
       <c r="J28" s="3">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="K28" s="11">
-        <v>0.17399999999999999</v>
+        <v>0.16400000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1673,25 +1673,25 @@
         <v>756</v>
       </c>
       <c r="E29" s="11">
-        <v>0.152</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="F29" s="3">
-        <v>863</v>
+        <v>848</v>
       </c>
       <c r="G29" s="11">
-        <v>0.151</v>
+        <v>0.159</v>
       </c>
       <c r="H29" s="3">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="I29" s="11">
-        <v>0.20699999999999999</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="J29" s="3">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c r="K29" s="11">
-        <v>0.192</v>
+        <v>0.26900000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1705,28 +1705,28 @@
         <v>20</v>
       </c>
       <c r="D30" s="4">
-        <v>10344</v>
+        <v>10378</v>
       </c>
       <c r="E30" s="11">
-        <v>12.112</v>
+        <v>13.558999999999999</v>
       </c>
       <c r="F30" s="3">
-        <v>12311</v>
+        <v>12300</v>
       </c>
       <c r="G30" s="11">
-        <v>22.838000000000001</v>
+        <v>26.756</v>
       </c>
       <c r="H30" s="3">
-        <v>11682</v>
+        <v>11935</v>
       </c>
       <c r="I30" s="11">
-        <v>18.12</v>
+        <v>19.782</v>
       </c>
       <c r="J30" s="3">
-        <v>13340</v>
+        <v>13347</v>
       </c>
       <c r="K30" s="11">
-        <v>28.736999999999998</v>
+        <v>34.249000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1740,28 +1740,28 @@
         <v>5</v>
       </c>
       <c r="D31" s="4">
-        <v>882</v>
+        <v>891</v>
       </c>
       <c r="E31" s="11">
-        <v>0.26500000000000001</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="F31" s="3">
-        <v>910</v>
+        <v>919</v>
       </c>
       <c r="G31" s="11">
-        <v>0.219</v>
+        <v>0.24</v>
       </c>
       <c r="H31" s="3">
-        <v>879</v>
+        <v>838</v>
       </c>
       <c r="I31" s="11">
-        <v>0.20599999999999999</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="J31" s="3">
-        <v>949</v>
+        <v>938</v>
       </c>
       <c r="K31" s="11">
-        <v>0.22500000000000001</v>
+        <v>0.26800000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1775,28 +1775,28 @@
         <v>20</v>
       </c>
       <c r="D32" s="4">
-        <v>2429</v>
+        <v>2439</v>
       </c>
       <c r="E32" s="11">
-        <v>1.39</v>
+        <v>1.5209999999999999</v>
       </c>
       <c r="F32" s="3">
-        <v>5534</v>
+        <v>5539</v>
       </c>
       <c r="G32" s="11">
-        <v>8.7729999999999997</v>
+        <v>9.1110000000000007</v>
       </c>
       <c r="H32" s="3">
-        <v>2519</v>
+        <v>2517</v>
       </c>
       <c r="I32" s="11">
-        <v>1.36</v>
+        <v>1.4419999999999999</v>
       </c>
       <c r="J32" s="3">
-        <v>6071</v>
+        <v>6007</v>
       </c>
       <c r="K32" s="11">
-        <v>11.234</v>
+        <v>10.215</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1810,28 +1810,28 @@
         <v>10</v>
       </c>
       <c r="D33" s="4">
-        <v>2640</v>
+        <v>2706</v>
       </c>
       <c r="E33" s="11">
-        <v>0.58599999999999997</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="F33" s="3">
-        <v>4082</v>
+        <v>4132</v>
       </c>
       <c r="G33" s="11">
-        <v>1.302</v>
+        <v>1.2450000000000001</v>
       </c>
       <c r="H33" s="3">
-        <v>3035</v>
+        <v>3099</v>
       </c>
       <c r="I33" s="11">
-        <v>0.70299999999999996</v>
+        <v>0.69</v>
       </c>
       <c r="J33" s="3">
-        <v>4410</v>
+        <v>4432</v>
       </c>
       <c r="K33" s="11">
-        <v>1.3149999999999999</v>
+        <v>1.4790000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1845,28 +1845,28 @@
         <v>3</v>
       </c>
       <c r="D34" s="4">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E34" s="11">
-        <v>0.27</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="F34" s="3">
-        <v>740</v>
+        <v>804</v>
       </c>
       <c r="G34" s="11">
-        <v>0.48499999999999999</v>
+        <v>0.502</v>
       </c>
       <c r="H34" s="3">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I34" s="11">
-        <v>0.17</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="J34" s="3">
-        <v>828</v>
+        <v>864</v>
       </c>
       <c r="K34" s="11">
-        <v>0.57199999999999995</v>
+        <v>0.50800000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1880,28 +1880,28 @@
         <v>11</v>
       </c>
       <c r="D35" s="4">
-        <v>1664</v>
+        <v>1631</v>
       </c>
       <c r="E35" s="11">
-        <v>0.55400000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="F35" s="3">
-        <v>3056</v>
+        <v>3107</v>
       </c>
       <c r="G35" s="11">
-        <v>1.482</v>
+        <v>1.252</v>
       </c>
       <c r="H35" s="3">
-        <v>1734</v>
+        <v>1673</v>
       </c>
       <c r="I35" s="11">
-        <v>0.52700000000000002</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="J35" s="3">
-        <v>3296</v>
+        <v>3193</v>
       </c>
       <c r="K35" s="11">
-        <v>1.5980000000000001</v>
+        <v>1.2470000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1915,28 +1915,28 @@
         <v>36</v>
       </c>
       <c r="D36" s="4">
-        <v>4550</v>
+        <v>4486</v>
       </c>
       <c r="E36" s="11">
-        <v>1.5660000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="F36" s="3">
-        <v>6830</v>
+        <v>6801</v>
       </c>
       <c r="G36" s="11">
-        <v>3.7970000000000002</v>
+        <v>2.4420000000000002</v>
       </c>
       <c r="H36" s="3">
-        <v>4544</v>
+        <v>4520</v>
       </c>
       <c r="I36" s="11">
-        <v>1.3140000000000001</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="J36" s="3">
-        <v>6909</v>
+        <v>6944</v>
       </c>
       <c r="K36" s="11">
-        <v>3.5619999999999998</v>
+        <v>2.5009999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1950,28 +1950,28 @@
         <v>48</v>
       </c>
       <c r="D37" s="4">
-        <v>5609</v>
+        <v>5610</v>
       </c>
       <c r="E37" s="11">
-        <v>1.0449999999999999</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="F37" s="3">
-        <v>8295</v>
+        <v>8361</v>
       </c>
       <c r="G37" s="11">
-        <v>3.6859999999999999</v>
+        <v>3.125</v>
       </c>
       <c r="H37" s="3">
-        <v>5673</v>
+        <v>5672</v>
       </c>
       <c r="I37" s="11">
-        <v>1.1140000000000001</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="J37" s="3">
-        <v>8346</v>
+        <v>8368</v>
       </c>
       <c r="K37" s="11">
-        <v>3.5840000000000001</v>
+        <v>3.2530000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1985,28 +1985,28 @@
         <v>36</v>
       </c>
       <c r="D38" s="4">
-        <v>4175</v>
+        <v>4176</v>
       </c>
       <c r="E38" s="11">
-        <v>1.1599999999999999</v>
+        <v>1.385</v>
       </c>
       <c r="F38" s="3">
-        <v>4689</v>
+        <v>4658</v>
       </c>
       <c r="G38" s="11">
-        <v>1.7430000000000001</v>
+        <v>1.8069999999999999</v>
       </c>
       <c r="H38" s="3">
-        <v>4256</v>
+        <v>4246</v>
       </c>
       <c r="I38" s="11">
-        <v>1.43</v>
+        <v>1.363</v>
       </c>
       <c r="J38" s="3">
-        <v>4785</v>
+        <v>4753</v>
       </c>
       <c r="K38" s="11">
-        <v>2.0430000000000001</v>
+        <v>2.117</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2020,28 +2020,28 @@
         <v>40</v>
       </c>
       <c r="D39" s="4">
-        <v>4912</v>
+        <v>4897</v>
       </c>
       <c r="E39" s="11">
-        <v>0.66100000000000003</v>
+        <v>0.81799999999999995</v>
       </c>
       <c r="F39" s="3">
-        <v>5361</v>
+        <v>5271</v>
       </c>
       <c r="G39" s="11">
-        <v>1.042</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="H39" s="3">
-        <v>4945</v>
+        <v>4914</v>
       </c>
       <c r="I39" s="11">
-        <v>0.70099999999999996</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="J39" s="3">
-        <v>5193</v>
+        <v>5126</v>
       </c>
       <c r="K39" s="11">
-        <v>0.84699999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2055,28 +2055,28 @@
         <v>36</v>
       </c>
       <c r="D40" s="4">
-        <v>4204</v>
+        <v>4202</v>
       </c>
       <c r="E40" s="11">
-        <v>1.8939999999999999</v>
+        <v>2.6019999999999999</v>
       </c>
       <c r="F40" s="3">
-        <v>4542</v>
+        <v>4670</v>
       </c>
       <c r="G40" s="11">
-        <v>2.6259999999999999</v>
+        <v>3.032</v>
       </c>
       <c r="H40" s="3">
-        <v>4219</v>
+        <v>4213</v>
       </c>
       <c r="I40" s="11">
-        <v>2.077</v>
+        <v>2.72</v>
       </c>
       <c r="J40" s="3">
-        <v>4511</v>
+        <v>4589</v>
       </c>
       <c r="K40" s="11">
-        <v>2.82</v>
+        <v>2.9710000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2090,28 +2090,28 @@
         <v>36</v>
       </c>
       <c r="D41" s="4">
-        <v>4601</v>
+        <v>4580</v>
       </c>
       <c r="E41" s="11">
-        <v>1.5880000000000001</v>
+        <v>1.9650000000000001</v>
       </c>
       <c r="F41" s="3">
-        <v>4596</v>
+        <v>4548</v>
       </c>
       <c r="G41" s="11">
-        <v>1.9379999999999999</v>
+        <v>1.9330000000000001</v>
       </c>
       <c r="H41" s="3">
-        <v>4746</v>
+        <v>4745</v>
       </c>
       <c r="I41" s="11">
-        <v>1.659</v>
+        <v>1.76</v>
       </c>
       <c r="J41" s="3">
-        <v>4534</v>
+        <v>4605</v>
       </c>
       <c r="K41" s="11">
-        <v>1.9490000000000001</v>
+        <v>2.2240000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2125,28 +2125,28 @@
         <v>40</v>
       </c>
       <c r="D42" s="4">
-        <v>6024</v>
+        <v>6000</v>
       </c>
       <c r="E42" s="11">
-        <v>1.044</v>
+        <v>1.151</v>
       </c>
       <c r="F42" s="3">
-        <v>6409</v>
+        <v>6408</v>
       </c>
       <c r="G42" s="11">
-        <v>1.373</v>
+        <v>1.478</v>
       </c>
       <c r="H42" s="3">
-        <v>6388</v>
+        <v>6419</v>
       </c>
       <c r="I42" s="11">
-        <v>1.17</v>
+        <v>1.194</v>
       </c>
       <c r="J42" s="3">
-        <v>6740</v>
+        <v>6765</v>
       </c>
       <c r="K42" s="11">
-        <v>1.3340000000000001</v>
+        <v>1.4370000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2160,28 +2160,28 @@
         <v>10</v>
       </c>
       <c r="D43" s="4">
-        <v>1231</v>
+        <v>1208</v>
       </c>
       <c r="E43" s="11">
-        <v>0.51</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="F43" s="3">
-        <v>1386</v>
+        <v>1421</v>
       </c>
       <c r="G43" s="11">
-        <v>0.63100000000000001</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="H43" s="3">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="I43" s="11">
-        <v>0.45</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="J43" s="3">
-        <v>1525</v>
+        <v>1501</v>
       </c>
       <c r="K43" s="11">
-        <v>0.58699999999999997</v>
+        <v>0.64400000000000002</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2195,28 +2195,28 @@
         <v>24</v>
       </c>
       <c r="D44" s="4">
-        <v>8079</v>
+        <v>8220</v>
       </c>
       <c r="E44" s="11">
-        <v>4.0830000000000002</v>
+        <v>4.8970000000000002</v>
       </c>
       <c r="F44" s="3">
-        <v>6536</v>
+        <v>6651</v>
       </c>
       <c r="G44" s="11">
-        <v>6.5670000000000002</v>
+        <v>6.8029999999999999</v>
       </c>
       <c r="H44" s="3">
-        <v>8134</v>
+        <v>8193</v>
       </c>
       <c r="I44" s="11">
-        <v>4.5940000000000003</v>
+        <v>5.218</v>
       </c>
       <c r="J44" s="3">
-        <v>6691</v>
+        <v>6729</v>
       </c>
       <c r="K44" s="11">
-        <v>6.5279999999999996</v>
+        <v>7.2960000000000003</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2230,28 +2230,28 @@
         <v>30</v>
       </c>
       <c r="D45" s="4">
-        <v>4891</v>
+        <v>4779</v>
       </c>
       <c r="E45" s="11">
-        <v>5.2539999999999996</v>
+        <v>5.508</v>
       </c>
       <c r="F45" s="3">
-        <v>4891</v>
+        <v>4779</v>
       </c>
       <c r="G45" s="11">
-        <v>4.9960000000000004</v>
+        <v>5.3979999999999997</v>
       </c>
       <c r="H45" s="3">
-        <v>4891</v>
+        <v>4779</v>
       </c>
       <c r="I45" s="11">
-        <v>5.2389999999999999</v>
+        <v>6.0819999999999999</v>
       </c>
       <c r="J45" s="3">
-        <v>4891</v>
+        <v>4779</v>
       </c>
       <c r="K45" s="11">
-        <v>5.3620000000000001</v>
+        <v>5.5640000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2265,28 +2265,28 @@
         <v>8.5</v>
       </c>
       <c r="D46" s="4">
-        <v>2463</v>
+        <v>2480</v>
       </c>
       <c r="E46" s="11">
-        <v>20.614000000000001</v>
+        <v>28.033999999999999</v>
       </c>
       <c r="F46" s="3">
-        <v>2463</v>
+        <v>2480</v>
       </c>
       <c r="G46" s="11">
-        <v>20.388999999999999</v>
+        <v>22.266999999999999</v>
       </c>
       <c r="H46" s="3">
-        <v>2463</v>
+        <v>2480</v>
       </c>
       <c r="I46" s="11">
-        <v>21.419</v>
+        <v>22.661000000000001</v>
       </c>
       <c r="J46" s="3">
-        <v>2463</v>
+        <v>2480</v>
       </c>
       <c r="K46" s="11">
-        <v>21.561</v>
+        <v>21.899000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2300,10 +2300,10 @@
         <v>33.72</v>
       </c>
       <c r="D47" s="4">
-        <v>8856</v>
+        <v>8738</v>
       </c>
       <c r="E47" s="11">
-        <v>4.0780000000000003</v>
+        <v>5.01</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>44</v>
@@ -2335,10 +2335,10 @@
         <v>32.19</v>
       </c>
       <c r="D48" s="4">
-        <v>8467</v>
+        <v>8588</v>
       </c>
       <c r="E48" s="11">
-        <v>4.8129999999999997</v>
+        <v>5.2160000000000002</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>44</v>
@@ -2370,10 +2370,10 @@
         <v>59.18</v>
       </c>
       <c r="D49" s="4">
-        <v>14844</v>
+        <v>15259</v>
       </c>
       <c r="E49" s="11">
-        <v>9.0589999999999993</v>
+        <v>10.555</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>44</v>
@@ -2402,13 +2402,13 @@
         <v>47</v>
       </c>
       <c r="C50" s="11">
-        <v>39.020000000000003</v>
+        <v>39.01</v>
       </c>
       <c r="D50" s="4">
-        <v>11309</v>
+        <v>11323</v>
       </c>
       <c r="E50" s="11">
-        <v>7.335</v>
+        <v>7.8949999999999996</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>44</v>
@@ -2437,13 +2437,13 @@
         <v>48</v>
       </c>
       <c r="C51" s="11">
-        <v>34.68</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="D51" s="4">
-        <v>9052</v>
+        <v>9224</v>
       </c>
       <c r="E51" s="11">
-        <v>4.6360000000000001</v>
+        <v>5.4429999999999996</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>44</v>
@@ -2472,13 +2472,13 @@
         <v>49</v>
       </c>
       <c r="C52" s="11">
-        <v>40.86</v>
+        <v>40.82</v>
       </c>
       <c r="D52" s="4">
-        <v>12326</v>
+        <v>11986</v>
       </c>
       <c r="E52" s="11">
-        <v>10.675000000000001</v>
+        <v>11.449</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>44</v>
@@ -2510,10 +2510,10 @@
         <v>41.27</v>
       </c>
       <c r="D53" s="2">
-        <v>11073</v>
+        <v>11451</v>
       </c>
       <c r="E53" s="11">
-        <v>7.3840000000000003</v>
+        <v>8.5050000000000008</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>44</v>
@@ -2545,10 +2545,10 @@
         <v>45.28</v>
       </c>
       <c r="D54" s="2">
-        <v>12191</v>
+        <v>12026</v>
       </c>
       <c r="E54" s="11">
-        <v>12.08</v>
+        <v>13.331</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>44</v>
@@ -2580,10 +2580,10 @@
         <v>27.71</v>
       </c>
       <c r="D55" s="2">
-        <v>9011</v>
+        <v>8687</v>
       </c>
       <c r="E55" s="11">
-        <v>8.0820000000000007</v>
+        <v>8.6210000000000004</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Initial commit R2018b.  Version 4.1
</commit_message>
<xml_diff>
--- a/Scripts_Data/CFR_Results.xlsx
+++ b/Scripts_Data/CFR_Results.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA_CForces\Contact_Forces_R18a\Scripts_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SMILLER\TMW\Simscape\zECLArch\zR18b\Demos\sscMbody\Contact_Forces\Scripts_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC7FFFBC-405F-45B5-BC50-C4BF669CB094}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
   <si>
     <t>#</t>
   </si>
@@ -210,19 +211,16 @@
     <t>Frict3D_08_Ball_on_Driven_Tube</t>
   </si>
   <si>
-    <t>9.4.0.813654 (R2018a)</t>
-  </si>
-  <si>
-    <t>CFL v4.0</t>
-  </si>
-  <si>
-    <t>09-Mar-2018 23:51:33</t>
+    <t>CFL v4.1</t>
+  </si>
+  <si>
+    <t>9.5.0.944444 (R2018b)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3:K55"/>
@@ -719,16 +717,16 @@
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="21" t="s">
-        <v>65</v>
+      <c r="F1" s="21">
+        <v>43354.271284722221</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -798,25 +796,25 @@
         <v>2388</v>
       </c>
       <c r="E4" s="14">
-        <v>2.9830000000000001</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="F4" s="15">
         <v>2388</v>
       </c>
       <c r="G4" s="14">
-        <v>0.23799999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="H4" s="15">
         <v>2388</v>
       </c>
       <c r="I4" s="14">
-        <v>0.23200000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="J4" s="15">
         <v>2388</v>
       </c>
       <c r="K4" s="14">
-        <v>0.192</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -833,25 +831,25 @@
         <v>669</v>
       </c>
       <c r="E5" s="11">
-        <v>0.71199999999999997</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="F5" s="4">
-        <v>929</v>
+        <v>935</v>
       </c>
       <c r="G5" s="11">
-        <v>0.13900000000000001</v>
+        <v>0.107</v>
       </c>
       <c r="H5" s="4">
         <v>718</v>
       </c>
       <c r="I5" s="11">
-        <v>0.123</v>
+        <v>0.124</v>
       </c>
       <c r="J5" s="4">
         <v>1020</v>
       </c>
       <c r="K5" s="11">
-        <v>0.16600000000000001</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -868,25 +866,25 @@
         <v>298</v>
       </c>
       <c r="E6" s="11">
-        <v>0.33500000000000002</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="F6" s="4">
         <v>370</v>
       </c>
       <c r="G6" s="11">
-        <v>9.7000000000000003E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="H6" s="4">
         <v>317</v>
       </c>
       <c r="I6" s="11">
-        <v>7.9000000000000001E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="J6" s="4">
         <v>398</v>
       </c>
       <c r="K6" s="11">
-        <v>0.11600000000000001</v>
+        <v>8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -903,25 +901,25 @@
         <v>3726</v>
       </c>
       <c r="E7" s="11">
-        <v>2.4700000000000002</v>
+        <v>1.871</v>
       </c>
       <c r="F7" s="4">
         <v>4928</v>
       </c>
       <c r="G7" s="11">
-        <v>3.048</v>
+        <v>2.57</v>
       </c>
       <c r="H7" s="4">
         <v>5039</v>
       </c>
       <c r="I7" s="11">
-        <v>3.5009999999999999</v>
+        <v>2.5569999999999999</v>
       </c>
       <c r="J7" s="4">
         <v>6295</v>
       </c>
       <c r="K7" s="11">
-        <v>4.8639999999999999</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -935,28 +933,28 @@
         <v>5</v>
       </c>
       <c r="D8" s="4">
-        <v>2096</v>
+        <v>2071</v>
       </c>
       <c r="E8" s="11">
-        <v>0.36299999999999999</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="F8" s="4">
-        <v>2794</v>
+        <v>2660</v>
       </c>
       <c r="G8" s="11">
-        <v>0.68200000000000005</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="H8" s="4">
-        <v>2425</v>
+        <v>2276</v>
       </c>
       <c r="I8" s="11">
-        <v>0.48299999999999998</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="J8" s="4">
-        <v>3210</v>
+        <v>2954</v>
       </c>
       <c r="K8" s="11">
-        <v>0.69699999999999995</v>
+        <v>0.33200000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -973,25 +971,25 @@
         <v>612</v>
       </c>
       <c r="E9" s="11">
-        <v>0.26</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="F9" s="4">
         <v>579</v>
       </c>
       <c r="G9" s="11">
-        <v>0.154</v>
+        <v>0.12</v>
       </c>
       <c r="H9" s="4">
         <v>747</v>
       </c>
       <c r="I9" s="11">
-        <v>0.16600000000000001</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="J9" s="4">
         <v>602</v>
       </c>
       <c r="K9" s="11">
-        <v>0.17799999999999999</v>
+        <v>0.14199999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1008,25 +1006,25 @@
         <v>210</v>
       </c>
       <c r="E10" s="11">
-        <v>0.13700000000000001</v>
+        <v>0.159</v>
       </c>
       <c r="F10" s="4">
         <v>213</v>
       </c>
       <c r="G10" s="11">
-        <v>6.9000000000000006E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="H10" s="4">
         <v>221</v>
       </c>
       <c r="I10" s="11">
-        <v>6.7000000000000004E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J10" s="4">
         <v>223</v>
       </c>
       <c r="K10" s="11">
-        <v>0.28199999999999997</v>
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1043,25 +1041,25 @@
         <v>9225</v>
       </c>
       <c r="E11" s="11">
-        <v>4.7</v>
+        <v>2.633</v>
       </c>
       <c r="F11" s="4">
         <v>17963</v>
       </c>
       <c r="G11" s="11">
-        <v>13.412000000000001</v>
+        <v>5.1280000000000001</v>
       </c>
       <c r="H11" s="4">
         <v>10816</v>
       </c>
       <c r="I11" s="11">
-        <v>5.4139999999999997</v>
+        <v>3.343</v>
       </c>
       <c r="J11" s="4">
         <v>21376</v>
       </c>
       <c r="K11" s="11">
-        <v>11.554</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1078,25 +1076,25 @@
         <v>1211</v>
       </c>
       <c r="E12" s="11">
-        <v>0.115</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="F12" s="4">
         <v>1211</v>
       </c>
       <c r="G12" s="11">
-        <v>7.4999999999999997E-2</v>
+        <v>0.115</v>
       </c>
       <c r="H12" s="4">
         <v>1211</v>
       </c>
       <c r="I12" s="11">
-        <v>7.4999999999999997E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="J12" s="4">
         <v>1211</v>
       </c>
       <c r="K12" s="11">
-        <v>7.2999999999999995E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1113,25 +1111,25 @@
         <v>1303</v>
       </c>
       <c r="E13" s="11">
-        <v>0.24099999999999999</v>
+        <v>0.255</v>
       </c>
       <c r="F13" s="3">
         <v>1444</v>
       </c>
       <c r="G13" s="11">
-        <v>0.215</v>
+        <v>0.19</v>
       </c>
       <c r="H13" s="4">
         <v>1397</v>
       </c>
       <c r="I13" s="11">
-        <v>0.184</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="J13" s="4">
         <v>1516</v>
       </c>
       <c r="K13" s="11">
-        <v>0.245</v>
+        <v>0.26300000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1148,25 +1146,25 @@
         <v>5568</v>
       </c>
       <c r="E14" s="11">
-        <v>0.64100000000000001</v>
+        <v>0.308</v>
       </c>
       <c r="F14" s="3">
         <v>5568</v>
       </c>
       <c r="G14" s="11">
-        <v>0.62</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="H14" s="4">
         <v>5568</v>
       </c>
       <c r="I14" s="11">
-        <v>0.51100000000000001</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="J14" s="4">
         <v>5568</v>
       </c>
       <c r="K14" s="11">
-        <v>0.51800000000000002</v>
+        <v>0.377</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1183,25 +1181,25 @@
         <v>721</v>
       </c>
       <c r="E15" s="11">
-        <v>0.20499999999999999</v>
+        <v>0.184</v>
       </c>
       <c r="F15" s="3">
         <v>860</v>
       </c>
       <c r="G15" s="11">
-        <v>0.11899999999999999</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="H15" s="3">
         <v>800</v>
       </c>
       <c r="I15" s="11">
-        <v>0.109</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="J15" s="3">
-        <v>941</v>
+        <v>989</v>
       </c>
       <c r="K15" s="11">
-        <v>0.13800000000000001</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1218,25 +1216,25 @@
         <v>1314</v>
       </c>
       <c r="E16" s="11">
-        <v>0.22700000000000001</v>
+        <v>0.185</v>
       </c>
       <c r="F16" s="3">
         <v>1404</v>
       </c>
       <c r="G16" s="11">
-        <v>0.14099999999999999</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="H16" s="3">
         <v>1396</v>
       </c>
       <c r="I16" s="11">
-        <v>0.13300000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="J16" s="3">
         <v>1456</v>
       </c>
       <c r="K16" s="11">
-        <v>0.152</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1253,25 +1251,25 @@
         <v>6367</v>
       </c>
       <c r="E17" s="11">
-        <v>1.7849999999999999</v>
+        <v>1.2929999999999999</v>
       </c>
       <c r="F17" s="3">
         <v>6644</v>
       </c>
       <c r="G17" s="11">
-        <v>1.825</v>
+        <v>1.135</v>
       </c>
       <c r="H17" s="3">
         <v>6035</v>
       </c>
       <c r="I17" s="11">
-        <v>1.73</v>
+        <v>1.079</v>
       </c>
       <c r="J17" s="3">
         <v>6527</v>
       </c>
       <c r="K17" s="11">
-        <v>2.4590000000000001</v>
+        <v>1.2789999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1288,25 +1286,25 @@
         <v>289</v>
       </c>
       <c r="E18" s="11">
-        <v>0.16900000000000001</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="F18" s="3">
         <v>301</v>
       </c>
       <c r="G18" s="11">
-        <v>7.1999999999999995E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="H18" s="3">
         <v>313</v>
       </c>
       <c r="I18" s="11">
-        <v>0.104</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="J18" s="3">
         <v>346</v>
       </c>
       <c r="K18" s="11">
-        <v>9.8000000000000004E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1320,28 +1318,28 @@
         <v>30</v>
       </c>
       <c r="D19" s="4">
-        <v>3439</v>
+        <v>3443</v>
       </c>
       <c r="E19" s="11">
-        <v>1.1399999999999999</v>
+        <v>0.747</v>
       </c>
       <c r="F19" s="3">
-        <v>3749</v>
+        <v>3675</v>
       </c>
       <c r="G19" s="11">
-        <v>1.0900000000000001</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="H19" s="3">
-        <v>3543</v>
+        <v>3496</v>
       </c>
       <c r="I19" s="11">
-        <v>0.97299999999999998</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="J19" s="3">
-        <v>3754</v>
+        <v>3803</v>
       </c>
       <c r="K19" s="11">
-        <v>1.008</v>
+        <v>0.68799999999999994</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1355,28 +1353,28 @@
         <v>50</v>
       </c>
       <c r="D20" s="4">
-        <v>7116</v>
+        <v>6874</v>
       </c>
       <c r="E20" s="11">
-        <v>1.2230000000000001</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="F20" s="3">
-        <v>7227</v>
+        <v>7094</v>
       </c>
       <c r="G20" s="11">
-        <v>1.208</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="H20" s="3">
-        <v>99561</v>
+        <v>98871</v>
       </c>
       <c r="I20" s="11">
-        <v>12.928000000000001</v>
+        <v>9.9429999999999996</v>
       </c>
       <c r="J20" s="3">
-        <v>206549</v>
+        <v>99867</v>
       </c>
       <c r="K20" s="11">
-        <v>32.481000000000002</v>
+        <v>11.047000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1390,28 +1388,28 @@
         <v>30</v>
       </c>
       <c r="D21" s="4">
-        <v>3715</v>
+        <v>3697</v>
       </c>
       <c r="E21" s="11">
-        <v>0.94199999999999995</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="F21" s="3">
-        <v>4719</v>
+        <v>4605</v>
       </c>
       <c r="G21" s="11">
-        <v>0.83499999999999996</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="H21" s="3">
-        <v>3988</v>
+        <v>3969</v>
       </c>
       <c r="I21" s="11">
-        <v>0.64500000000000002</v>
+        <v>0.375</v>
       </c>
       <c r="J21" s="3">
-        <v>3942</v>
+        <v>3933</v>
       </c>
       <c r="K21" s="11">
-        <v>0.63500000000000001</v>
+        <v>0.38400000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1425,28 +1423,28 @@
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <v>2511</v>
+        <v>2229</v>
       </c>
       <c r="E22" s="11">
-        <v>7.1980000000000004</v>
+        <v>4.8159999999999998</v>
       </c>
       <c r="F22" s="3">
-        <v>2511</v>
+        <v>2229</v>
       </c>
       <c r="G22" s="11">
-        <v>6.6710000000000003</v>
+        <v>4.3360000000000003</v>
       </c>
       <c r="H22" s="3">
-        <v>2511</v>
+        <v>2229</v>
       </c>
       <c r="I22" s="11">
-        <v>6.9390000000000001</v>
+        <v>4.242</v>
       </c>
       <c r="J22" s="3">
-        <v>2511</v>
+        <v>2229</v>
       </c>
       <c r="K22" s="11">
-        <v>6.6619999999999999</v>
+        <v>4.2729999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1463,25 +1461,25 @@
         <v>3105</v>
       </c>
       <c r="E23" s="11">
-        <v>1.748</v>
+        <v>1.262</v>
       </c>
       <c r="F23" s="3">
         <v>2987</v>
       </c>
       <c r="G23" s="11">
-        <v>1.3879999999999999</v>
+        <v>1.256</v>
       </c>
       <c r="H23" s="3">
         <v>3783</v>
       </c>
       <c r="I23" s="11">
-        <v>1.8560000000000001</v>
+        <v>1.2869999999999999</v>
       </c>
       <c r="J23" s="3">
         <v>3676</v>
       </c>
       <c r="K23" s="11">
-        <v>1.845</v>
+        <v>1.2529999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1498,25 +1496,25 @@
         <v>131</v>
       </c>
       <c r="E24" s="11">
-        <v>0.17699999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="F24" s="3">
         <v>131</v>
       </c>
       <c r="G24" s="11">
-        <v>5.6000000000000001E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="H24" s="3">
         <v>131</v>
       </c>
       <c r="I24" s="11">
-        <v>5.2999999999999999E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="J24" s="3">
         <v>131</v>
       </c>
       <c r="K24" s="11">
-        <v>5.3999999999999999E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1533,25 +1531,25 @@
         <v>4739</v>
       </c>
       <c r="E25" s="11">
-        <v>4.5739999999999998</v>
+        <v>3.8479999999999999</v>
       </c>
       <c r="F25" s="3">
         <v>5195</v>
       </c>
       <c r="G25" s="11">
-        <v>5.0220000000000002</v>
+        <v>4.2699999999999996</v>
       </c>
       <c r="H25" s="3">
         <v>4547</v>
       </c>
       <c r="I25" s="11">
-        <v>4.5960000000000001</v>
+        <v>3.871</v>
       </c>
       <c r="J25" s="3">
         <v>5128</v>
       </c>
       <c r="K25" s="11">
-        <v>5.3920000000000003</v>
+        <v>4.5529999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1565,28 +1563,28 @@
         <v>12</v>
       </c>
       <c r="D26" s="4">
-        <v>13132</v>
+        <v>14171</v>
       </c>
       <c r="E26" s="11">
-        <v>7.1529999999999996</v>
+        <v>6.2629999999999999</v>
       </c>
       <c r="F26" s="3">
-        <v>14228</v>
+        <v>14108</v>
       </c>
       <c r="G26" s="11">
-        <v>8.41</v>
+        <v>6.0140000000000002</v>
       </c>
       <c r="H26" s="3">
-        <v>18990</v>
+        <v>20521</v>
       </c>
       <c r="I26" s="11">
-        <v>10.222</v>
+        <v>8.7970000000000006</v>
       </c>
       <c r="J26" s="3">
-        <v>18458</v>
+        <v>19890</v>
       </c>
       <c r="K26" s="11">
-        <v>9.923</v>
+        <v>8.6489999999999991</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1603,25 +1601,25 @@
         <v>3433</v>
       </c>
       <c r="E27" s="11">
-        <v>2.4710000000000001</v>
+        <v>2.2690000000000001</v>
       </c>
       <c r="F27" s="3">
         <v>4404</v>
       </c>
       <c r="G27" s="11">
-        <v>4.2169999999999996</v>
+        <v>3.4060000000000001</v>
       </c>
       <c r="H27" s="3">
         <v>3534</v>
       </c>
       <c r="I27" s="11">
-        <v>2.5720000000000001</v>
+        <v>2.1539999999999999</v>
       </c>
       <c r="J27" s="3">
         <v>4409</v>
       </c>
       <c r="K27" s="11">
-        <v>3.915</v>
+        <v>3.4159999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1638,25 +1636,25 @@
         <v>941</v>
       </c>
       <c r="E28" s="11">
-        <v>0.22900000000000001</v>
+        <v>0.249</v>
       </c>
       <c r="F28" s="3">
         <v>1022</v>
       </c>
       <c r="G28" s="11">
-        <v>0.152</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="H28" s="3">
         <v>967</v>
       </c>
       <c r="I28" s="11">
-        <v>0.121</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="J28" s="3">
         <v>1061</v>
       </c>
       <c r="K28" s="11">
-        <v>0.16400000000000001</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1673,7 +1671,7 @@
         <v>756</v>
       </c>
       <c r="E29" s="11">
-        <v>0.23499999999999999</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="F29" s="3">
         <v>848</v>
@@ -1685,13 +1683,13 @@
         <v>785</v>
       </c>
       <c r="I29" s="11">
-        <v>0.21099999999999999</v>
+        <v>0.221</v>
       </c>
       <c r="J29" s="3">
         <v>899</v>
       </c>
       <c r="K29" s="11">
-        <v>0.26900000000000002</v>
+        <v>0.216</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1708,25 +1706,25 @@
         <v>10378</v>
       </c>
       <c r="E30" s="11">
-        <v>13.558999999999999</v>
+        <v>12.255000000000001</v>
       </c>
       <c r="F30" s="3">
         <v>12300</v>
       </c>
       <c r="G30" s="11">
-        <v>26.756</v>
+        <v>24.074000000000002</v>
       </c>
       <c r="H30" s="3">
         <v>11935</v>
       </c>
       <c r="I30" s="11">
-        <v>19.782</v>
+        <v>18.384</v>
       </c>
       <c r="J30" s="3">
         <v>13347</v>
       </c>
       <c r="K30" s="11">
-        <v>34.249000000000002</v>
+        <v>31.193000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1743,25 +1741,25 @@
         <v>891</v>
       </c>
       <c r="E31" s="11">
-        <v>0.36199999999999999</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="F31" s="3">
         <v>919</v>
       </c>
       <c r="G31" s="11">
-        <v>0.24</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="H31" s="3">
         <v>838</v>
       </c>
       <c r="I31" s="11">
-        <v>0.23300000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="J31" s="3">
         <v>938</v>
       </c>
       <c r="K31" s="11">
-        <v>0.26800000000000002</v>
+        <v>0.27800000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1778,25 +1776,25 @@
         <v>2439</v>
       </c>
       <c r="E32" s="11">
-        <v>1.5209999999999999</v>
+        <v>1.9339999999999999</v>
       </c>
       <c r="F32" s="3">
         <v>5539</v>
       </c>
       <c r="G32" s="11">
-        <v>9.1110000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="H32" s="3">
         <v>2517</v>
       </c>
       <c r="I32" s="11">
-        <v>1.4419999999999999</v>
+        <v>1.3360000000000001</v>
       </c>
       <c r="J32" s="3">
         <v>6007</v>
       </c>
       <c r="K32" s="11">
-        <v>10.215</v>
+        <v>9.2289999999999992</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1813,25 +1811,25 @@
         <v>2706</v>
       </c>
       <c r="E33" s="11">
-        <v>0.77200000000000002</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="F33" s="3">
         <v>4132</v>
       </c>
       <c r="G33" s="11">
-        <v>1.2450000000000001</v>
+        <v>0.85299999999999998</v>
       </c>
       <c r="H33" s="3">
         <v>3099</v>
       </c>
       <c r="I33" s="11">
-        <v>0.69</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="J33" s="3">
         <v>4432</v>
       </c>
       <c r="K33" s="11">
-        <v>1.4790000000000001</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1848,25 +1846,25 @@
         <v>429</v>
       </c>
       <c r="E34" s="11">
-        <v>0.25700000000000001</v>
+        <v>0.221</v>
       </c>
       <c r="F34" s="3">
         <v>804</v>
       </c>
       <c r="G34" s="11">
-        <v>0.502</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="H34" s="3">
         <v>504</v>
       </c>
       <c r="I34" s="11">
-        <v>0.16500000000000001</v>
+        <v>0.127</v>
       </c>
       <c r="J34" s="3">
         <v>864</v>
       </c>
       <c r="K34" s="11">
-        <v>0.50800000000000001</v>
+        <v>0.41299999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1883,25 +1881,25 @@
         <v>1631</v>
       </c>
       <c r="E35" s="11">
-        <v>0.5</v>
+        <v>0.318</v>
       </c>
       <c r="F35" s="3">
         <v>3107</v>
       </c>
       <c r="G35" s="11">
-        <v>1.252</v>
+        <v>0.872</v>
       </c>
       <c r="H35" s="3">
         <v>1673</v>
       </c>
       <c r="I35" s="11">
-        <v>0.33800000000000002</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="J35" s="3">
         <v>3193</v>
       </c>
       <c r="K35" s="11">
-        <v>1.2470000000000001</v>
+        <v>0.876</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1918,25 +1916,25 @@
         <v>4486</v>
       </c>
       <c r="E36" s="11">
-        <v>1.07</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="F36" s="3">
         <v>6801</v>
       </c>
       <c r="G36" s="11">
-        <v>2.4420000000000002</v>
+        <v>2.0049999999999999</v>
       </c>
       <c r="H36" s="3">
         <v>4520</v>
       </c>
       <c r="I36" s="11">
-        <v>0.95099999999999996</v>
+        <v>0.749</v>
       </c>
       <c r="J36" s="3">
         <v>6944</v>
       </c>
       <c r="K36" s="11">
-        <v>2.5009999999999999</v>
+        <v>2.2719999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1953,25 +1951,25 @@
         <v>5610</v>
       </c>
       <c r="E37" s="11">
-        <v>0.92900000000000005</v>
+        <v>0.85199999999999998</v>
       </c>
       <c r="F37" s="3">
         <v>8361</v>
       </c>
       <c r="G37" s="11">
-        <v>3.125</v>
+        <v>2.2879999999999998</v>
       </c>
       <c r="H37" s="3">
         <v>5672</v>
       </c>
       <c r="I37" s="11">
-        <v>0.93100000000000005</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="J37" s="3">
         <v>8368</v>
       </c>
       <c r="K37" s="11">
-        <v>3.2530000000000001</v>
+        <v>2.444</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1988,25 +1986,25 @@
         <v>4176</v>
       </c>
       <c r="E38" s="11">
-        <v>1.385</v>
+        <v>1.071</v>
       </c>
       <c r="F38" s="3">
         <v>4658</v>
       </c>
       <c r="G38" s="11">
-        <v>1.8069999999999999</v>
+        <v>1.42</v>
       </c>
       <c r="H38" s="3">
         <v>4246</v>
       </c>
       <c r="I38" s="11">
-        <v>1.363</v>
+        <v>1.044</v>
       </c>
       <c r="J38" s="3">
         <v>4753</v>
       </c>
       <c r="K38" s="11">
-        <v>2.117</v>
+        <v>1.4219999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2023,25 +2021,25 @@
         <v>4897</v>
       </c>
       <c r="E39" s="11">
-        <v>0.81799999999999995</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="F39" s="3">
         <v>5271</v>
       </c>
       <c r="G39" s="11">
-        <v>0.95199999999999996</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="H39" s="3">
         <v>4914</v>
       </c>
       <c r="I39" s="11">
-        <v>0.73899999999999999</v>
+        <v>0.54</v>
       </c>
       <c r="J39" s="3">
         <v>5126</v>
       </c>
       <c r="K39" s="11">
-        <v>0.98499999999999999</v>
+        <v>0.67700000000000005</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2058,25 +2056,25 @@
         <v>4202</v>
       </c>
       <c r="E40" s="11">
-        <v>2.6019999999999999</v>
+        <v>1.677</v>
       </c>
       <c r="F40" s="3">
         <v>4670</v>
       </c>
       <c r="G40" s="11">
-        <v>3.032</v>
+        <v>2.0859999999999999</v>
       </c>
       <c r="H40" s="3">
         <v>4213</v>
       </c>
       <c r="I40" s="11">
-        <v>2.72</v>
+        <v>1.6439999999999999</v>
       </c>
       <c r="J40" s="3">
         <v>4589</v>
       </c>
       <c r="K40" s="11">
-        <v>2.9710000000000001</v>
+        <v>2.0009999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2093,25 +2091,25 @@
         <v>4580</v>
       </c>
       <c r="E41" s="11">
-        <v>1.9650000000000001</v>
+        <v>1.373</v>
       </c>
       <c r="F41" s="3">
         <v>4548</v>
       </c>
       <c r="G41" s="11">
-        <v>1.9330000000000001</v>
+        <v>1.407</v>
       </c>
       <c r="H41" s="3">
         <v>4745</v>
       </c>
       <c r="I41" s="11">
-        <v>1.76</v>
+        <v>1.3280000000000001</v>
       </c>
       <c r="J41" s="3">
         <v>4605</v>
       </c>
       <c r="K41" s="11">
-        <v>2.2240000000000002</v>
+        <v>1.5640000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2128,25 +2126,25 @@
         <v>6000</v>
       </c>
       <c r="E42" s="11">
-        <v>1.151</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="F42" s="3">
         <v>6408</v>
       </c>
       <c r="G42" s="11">
-        <v>1.478</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="H42" s="3">
         <v>6419</v>
       </c>
       <c r="I42" s="11">
-        <v>1.194</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="J42" s="3">
         <v>6765</v>
       </c>
       <c r="K42" s="11">
-        <v>1.4370000000000001</v>
+        <v>0.93500000000000005</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2163,25 +2161,25 @@
         <v>1208</v>
       </c>
       <c r="E43" s="11">
-        <v>0.59799999999999998</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="F43" s="3">
         <v>1421</v>
       </c>
       <c r="G43" s="11">
-        <v>0.48399999999999999</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="H43" s="3">
         <v>1246</v>
       </c>
       <c r="I43" s="11">
-        <v>0.39400000000000002</v>
+        <v>0.27</v>
       </c>
       <c r="J43" s="3">
         <v>1501</v>
       </c>
       <c r="K43" s="11">
-        <v>0.64400000000000002</v>
+        <v>0.42599999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2198,25 +2196,25 @@
         <v>8220</v>
       </c>
       <c r="E44" s="11">
-        <v>4.8970000000000002</v>
+        <v>4.0890000000000004</v>
       </c>
       <c r="F44" s="3">
         <v>6651</v>
       </c>
       <c r="G44" s="11">
-        <v>6.8029999999999999</v>
+        <v>5.3159999999999998</v>
       </c>
       <c r="H44" s="3">
         <v>8193</v>
       </c>
       <c r="I44" s="11">
-        <v>5.218</v>
+        <v>3.81</v>
       </c>
       <c r="J44" s="3">
         <v>6729</v>
       </c>
       <c r="K44" s="11">
-        <v>7.2960000000000003</v>
+        <v>5.3440000000000003</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2230,28 +2228,28 @@
         <v>30</v>
       </c>
       <c r="D45" s="4">
-        <v>4779</v>
+        <v>4242</v>
       </c>
       <c r="E45" s="11">
-        <v>5.508</v>
+        <v>2.9809999999999999</v>
       </c>
       <c r="F45" s="3">
-        <v>4779</v>
+        <v>4242</v>
       </c>
       <c r="G45" s="11">
-        <v>5.3979999999999997</v>
+        <v>2.5579999999999998</v>
       </c>
       <c r="H45" s="3">
-        <v>4779</v>
+        <v>4242</v>
       </c>
       <c r="I45" s="11">
-        <v>6.0819999999999999</v>
+        <v>2.9809999999999999</v>
       </c>
       <c r="J45" s="3">
-        <v>4779</v>
+        <v>4242</v>
       </c>
       <c r="K45" s="11">
-        <v>5.5640000000000001</v>
+        <v>2.5710000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2262,31 +2260,31 @@
         <v>61</v>
       </c>
       <c r="C46" s="11">
-        <v>8.5</v>
+        <v>50</v>
       </c>
       <c r="D46" s="4">
-        <v>2480</v>
+        <v>5515</v>
       </c>
       <c r="E46" s="11">
-        <v>28.033999999999999</v>
+        <v>3.7170000000000001</v>
       </c>
       <c r="F46" s="3">
-        <v>2480</v>
+        <v>9462</v>
       </c>
       <c r="G46" s="11">
-        <v>22.266999999999999</v>
+        <v>6.9489999999999998</v>
       </c>
       <c r="H46" s="3">
-        <v>2480</v>
+        <v>5558</v>
       </c>
       <c r="I46" s="11">
-        <v>22.661000000000001</v>
+        <v>3.22</v>
       </c>
       <c r="J46" s="3">
-        <v>2480</v>
+        <v>9667</v>
       </c>
       <c r="K46" s="11">
-        <v>21.899000000000001</v>
+        <v>7.3250000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2300,10 +2298,10 @@
         <v>33.72</v>
       </c>
       <c r="D47" s="4">
-        <v>8738</v>
+        <v>9375</v>
       </c>
       <c r="E47" s="11">
-        <v>5.01</v>
+        <v>5.2859999999999996</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>44</v>
@@ -2335,10 +2333,10 @@
         <v>32.19</v>
       </c>
       <c r="D48" s="4">
-        <v>8588</v>
+        <v>8828</v>
       </c>
       <c r="E48" s="11">
-        <v>5.2160000000000002</v>
+        <v>5.0209999999999999</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>44</v>
@@ -2370,10 +2368,10 @@
         <v>59.18</v>
       </c>
       <c r="D49" s="4">
-        <v>15259</v>
+        <v>15140</v>
       </c>
       <c r="E49" s="11">
-        <v>10.555</v>
+        <v>11.003</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>44</v>
@@ -2402,13 +2400,13 @@
         <v>47</v>
       </c>
       <c r="C50" s="11">
-        <v>39.01</v>
+        <v>39.020000000000003</v>
       </c>
       <c r="D50" s="4">
-        <v>11323</v>
+        <v>11499</v>
       </c>
       <c r="E50" s="11">
-        <v>7.8949999999999996</v>
+        <v>7.7409999999999997</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>44</v>
@@ -2437,13 +2435,13 @@
         <v>48</v>
       </c>
       <c r="C51" s="11">
-        <v>34.700000000000003</v>
+        <v>34.68</v>
       </c>
       <c r="D51" s="4">
-        <v>9224</v>
+        <v>9443</v>
       </c>
       <c r="E51" s="11">
-        <v>5.4429999999999996</v>
+        <v>5.1580000000000004</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>44</v>
@@ -2475,10 +2473,10 @@
         <v>40.82</v>
       </c>
       <c r="D52" s="4">
-        <v>11986</v>
+        <v>11825</v>
       </c>
       <c r="E52" s="11">
-        <v>11.449</v>
+        <v>11.680999999999999</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>44</v>
@@ -2507,13 +2505,13 @@
         <v>50</v>
       </c>
       <c r="C53" s="2">
-        <v>41.27</v>
+        <v>41.28</v>
       </c>
       <c r="D53" s="2">
-        <v>11451</v>
+        <v>11517</v>
       </c>
       <c r="E53" s="11">
-        <v>8.5050000000000008</v>
+        <v>10.426</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>44</v>
@@ -2542,13 +2540,13 @@
         <v>51</v>
       </c>
       <c r="C54" s="2">
-        <v>45.28</v>
+        <v>45.27</v>
       </c>
       <c r="D54" s="2">
-        <v>12026</v>
+        <v>12245</v>
       </c>
       <c r="E54" s="11">
-        <v>13.331</v>
+        <v>14.163</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>44</v>
@@ -2580,10 +2578,10 @@
         <v>27.71</v>
       </c>
       <c r="D55" s="2">
-        <v>8687</v>
+        <v>8945</v>
       </c>
       <c r="E55" s="11">
-        <v>8.6210000000000004</v>
+        <v>8.5510000000000002</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>44</v>
@@ -2618,6 +2616,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100525B94EEF47D42499A62120CC90E0AB3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e706cd362d7e41030bb8c72a7c62a9d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c85acdc-a394-4ae0-8c72-fb4a95b3d573" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55e2521e7df4d5c11309cefaa7c01562" ns2:_="">
     <xsd:import namespace="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
@@ -2762,18 +2771,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2819,29 +2826,10 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2863,25 +2851,35 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039CDCF7-1F8F-4E25-A268-76852380612B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97465A2D-9EAF-44EA-B51B-9ABE6C271840}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630E037-F79E-4175-B540-A23B306F8900}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE6D0D52-57FE-48CB-8E43-11384E6CFEE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630E037-F79E-4175-B540-A23B306F8900}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Initial commit R2019a.  Version 4.1
</commit_message>
<xml_diff>
--- a/Scripts_Data/CFR_Results.xlsx
+++ b/Scripts_Data/CFR_Results.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SMILLER\TMW\Simscape\zECLArch\zR18b\Demos\sscMbody\Contact_Forces\Scripts_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SMILLER\TMW\Simscape\zECLArch\zR19a\Demos\sscMbody\Contact_Forces\Scripts_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC7FFFBC-405F-45B5-BC50-C4BF669CB094}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C62749C-C011-4EF4-A6B8-AA78F673A18F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>#</t>
   </si>
@@ -28,88 +35,142 @@
     <t>Model</t>
   </si>
   <si>
+    <t># Steps</t>
+  </si>
+  <si>
+    <t>Stop Time</t>
+  </si>
+  <si>
+    <t>Sim Time</t>
+  </si>
+  <si>
+    <t>Contact Forces Tests</t>
+  </si>
+  <si>
+    <t>Linear, No Friction</t>
+  </si>
+  <si>
+    <t>Linear, Stick-Slip C</t>
+  </si>
+  <si>
+    <t>Nonlin., No Friction</t>
+  </si>
+  <si>
+    <t>Nonlin., Stick-Slip C</t>
+  </si>
+  <si>
+    <t>Mini Golf Hole 1</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Mini Golf Hole 2</t>
+  </si>
+  <si>
+    <t>Mini Golf Hole 3</t>
+  </si>
+  <si>
+    <t>Mini Golf Hole 4</t>
+  </si>
+  <si>
+    <t>Mini Golf Hole 5</t>
+  </si>
+  <si>
+    <t>Mini Golf Hole 6</t>
+  </si>
+  <si>
+    <t>Mini Golf Hole 7</t>
+  </si>
+  <si>
+    <t>Mini Golf Hole 8</t>
+  </si>
+  <si>
+    <t>Mini Golf Hole 9</t>
+  </si>
+  <si>
+    <t>Gripper_2Belts</t>
+  </si>
+  <si>
+    <t>sm_tread_drive</t>
+  </si>
+  <si>
+    <t>CFL v4.1</t>
+  </si>
+  <si>
+    <t>Caster_4_Whl</t>
+  </si>
+  <si>
+    <t>Collision_01_Ball_Infinite_Plane</t>
+  </si>
+  <si>
+    <t>Collision_02_Disk_Finite_Plane_Fixed</t>
+  </si>
+  <si>
+    <t>Collision_03_Disk_Finite_Plane_Spin</t>
+  </si>
+  <si>
+    <t>Collision_04_Disks_in_Box</t>
+  </si>
+  <si>
+    <t>Collision_05_Disk_in_Ring</t>
+  </si>
+  <si>
+    <t>Collision_06_Catapult</t>
+  </si>
+  <si>
+    <t>Collision_07_Ball_Finite_Plane_Float</t>
+  </si>
+  <si>
+    <t>Collision_08_Compare_Forces</t>
+  </si>
+  <si>
+    <t>Friction_01_Box_on_Ramp_Constraint</t>
+  </si>
+  <si>
+    <t>Friction_02_Box_on_Ramp</t>
+  </si>
+  <si>
+    <t>Friction_03_Double_Pendulum_Constraint</t>
+  </si>
+  <si>
+    <t>Friction_04_Disk_Rolling_on_Ramp</t>
+  </si>
+  <si>
+    <t>Friction_05_Beam_on_Wheel</t>
+  </si>
+  <si>
+    <t>Friction_06_Disk_on_Disk</t>
+  </si>
+  <si>
+    <t>Friction_07_Floating_Disks</t>
+  </si>
+  <si>
+    <t>Friction_08_Disks_and_Ring</t>
+  </si>
+  <si>
+    <t>Friction_09_Ring_on_Disk_Float</t>
+  </si>
+  <si>
+    <t>Friction_10_Ball_on_Wheel</t>
+  </si>
+  <si>
+    <t>sm_ball_bearing_testrig</t>
+  </si>
+  <si>
     <t>Cam_Follower</t>
   </si>
   <si>
+    <t>Cam_Follower_Constraint</t>
+  </si>
+  <si>
     <t>Geneva_Drive</t>
   </si>
   <si>
-    <t># Steps</t>
-  </si>
-  <si>
-    <t>Stop Time</t>
-  </si>
-  <si>
-    <t>Sim Time</t>
-  </si>
-  <si>
-    <t>Contact Forces Tests</t>
-  </si>
-  <si>
     <t>Spinning_Boxes</t>
   </si>
   <si>
-    <t>Linear, No Friction</t>
-  </si>
-  <si>
-    <t>Linear, Stick-Slip C</t>
-  </si>
-  <si>
-    <t>Nonlin., No Friction</t>
-  </si>
-  <si>
-    <t>Nonlin., Stick-Slip C</t>
-  </si>
-  <si>
-    <t>Collision_01_Ball_Infinite_Plane</t>
-  </si>
-  <si>
-    <t>Collision_04_Disks_in_Box</t>
-  </si>
-  <si>
-    <t>Collision_05_Disk_in_Ring</t>
-  </si>
-  <si>
-    <t>Collision_06_Catapult</t>
-  </si>
-  <si>
-    <t>Collision_07_Ball_Finite_Plane_Float</t>
-  </si>
-  <si>
-    <t>Collision_08_Compare_Forces</t>
-  </si>
-  <si>
-    <t>Collision_02_Disk_Finite_Plane_Fixed</t>
-  </si>
-  <si>
-    <t>Collision_03_Disk_Finite_Plane_Spin</t>
-  </si>
-  <si>
-    <t>Friction_01_Box_on_Ramp_Constraint</t>
-  </si>
-  <si>
-    <t>Friction_02_Box_on_Ramp</t>
-  </si>
-  <si>
-    <t>Friction_03_Double_Pendulum_Constraint</t>
-  </si>
-  <si>
-    <t>Friction_04_Disk_Rolling_on_Ramp</t>
-  </si>
-  <si>
-    <t>Friction_05_Beam_on_Wheel</t>
-  </si>
-  <si>
-    <t>Friction_06_Disk_on_Disk</t>
-  </si>
-  <si>
-    <t>Friction_07_Floating_Disks</t>
-  </si>
-  <si>
-    <t>Friction_08_Disks_and_Ring</t>
-  </si>
-  <si>
-    <t>Friction_09_Ring_on_Disk_Float</t>
+    <t>Belts_01_Two_Belts</t>
   </si>
   <si>
     <t>Coll3D_01_Ball_Plane_Fixed</t>
@@ -130,6 +191,12 @@
     <t>Coll3D_06_Ball_in_Ball</t>
   </si>
   <si>
+    <t>Coll3D_07_Balls_and_Sliding_Tube</t>
+  </si>
+  <si>
+    <t>Coll3D_08_Ball_in_Spinning_Cone</t>
+  </si>
+  <si>
     <t>Frict3D_01_Box_on_Table</t>
   </si>
   <si>
@@ -151,70 +218,16 @@
     <t>Frict3D_07_Ball_in_Ball</t>
   </si>
   <si>
-    <t>Mini Golf Hole 1</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Mini Golf Hole 2</t>
-  </si>
-  <si>
-    <t>Mini Golf Hole 3</t>
-  </si>
-  <si>
-    <t>Mini Golf Hole 4</t>
-  </si>
-  <si>
-    <t>Mini Golf Hole 5</t>
-  </si>
-  <si>
-    <t>Mini Golf Hole 6</t>
-  </si>
-  <si>
-    <t>Mini Golf Hole 7</t>
-  </si>
-  <si>
-    <t>Mini Golf Hole 8</t>
-  </si>
-  <si>
-    <t>Mini Golf Hole 9</t>
-  </si>
-  <si>
-    <t>Belts_01_Two_Belts</t>
+    <t>Frict3D_08_Ball_on_Driven_Tube</t>
   </si>
   <si>
     <t>Robot_2_Whl</t>
   </si>
   <si>
-    <t>Gripper_2Belts</t>
-  </si>
-  <si>
-    <t>Friction_10_Ball_on_Wheel</t>
-  </si>
-  <si>
-    <t>Coll3D_07_Balls_and_Sliding_Tube</t>
-  </si>
-  <si>
-    <t>Coll3D_08_Ball_in_Spinning_Cone</t>
-  </si>
-  <si>
-    <t>Cam_Follower_Constraint</t>
-  </si>
-  <si>
-    <t>sm_ball_bearing_testrig</t>
-  </si>
-  <si>
-    <t>sm_tread_drive</t>
-  </si>
-  <si>
-    <t>Frict3D_08_Ball_on_Driven_Tube</t>
-  </si>
-  <si>
-    <t>CFL v4.1</t>
-  </si>
-  <si>
-    <t>9.5.0.944444 (R2018b)</t>
+    <t>9.6.0.1072779 (R2019a)</t>
+  </si>
+  <si>
+    <t>19-Mar-2019 07:07:34</t>
   </si>
 </sst>
 </file>
@@ -695,13 +708,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:K55"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,36 +727,36 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="21">
-        <v>43354.271284722221</v>
+      <c r="F1" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="7" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D2" s="18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I2" s="19"/>
       <c r="J2" s="18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K2" s="19"/>
     </row>
@@ -755,31 +768,31 @@
         <v>1</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>6</v>
-      </c>
       <c r="F3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>6</v>
-      </c>
       <c r="H3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="16" t="s">
-        <v>6</v>
-      </c>
       <c r="J3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>4</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -787,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C4" s="14">
         <v>6</v>
@@ -796,25 +809,25 @@
         <v>2388</v>
       </c>
       <c r="E4" s="14">
-        <v>0.98899999999999999</v>
+        <v>1.1779999999999999</v>
       </c>
       <c r="F4" s="15">
         <v>2388</v>
       </c>
       <c r="G4" s="14">
-        <v>0.16</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="H4" s="15">
         <v>2388</v>
       </c>
       <c r="I4" s="14">
-        <v>0.13800000000000001</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="J4" s="15">
         <v>2388</v>
       </c>
       <c r="K4" s="14">
-        <v>0.155</v>
+        <v>0.32900000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -822,7 +835,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C5" s="11">
         <v>4</v>
@@ -831,25 +844,25 @@
         <v>669</v>
       </c>
       <c r="E5" s="11">
-        <v>0.63600000000000001</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="F5" s="4">
         <v>935</v>
       </c>
       <c r="G5" s="11">
-        <v>0.107</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="H5" s="4">
         <v>718</v>
       </c>
       <c r="I5" s="11">
-        <v>0.124</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="J5" s="4">
         <v>1020</v>
       </c>
       <c r="K5" s="11">
-        <v>0.107</v>
+        <v>0.159</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -857,7 +870,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C6" s="11">
         <v>1.5</v>
@@ -866,13 +879,13 @@
         <v>298</v>
       </c>
       <c r="E6" s="11">
-        <v>0.23499999999999999</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="F6" s="4">
         <v>370</v>
       </c>
       <c r="G6" s="11">
-        <v>7.6999999999999999E-2</v>
+        <v>0.106</v>
       </c>
       <c r="H6" s="4">
         <v>317</v>
@@ -884,7 +897,7 @@
         <v>398</v>
       </c>
       <c r="K6" s="11">
-        <v>8.7999999999999995E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -892,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C7" s="11">
         <v>3</v>
@@ -901,25 +914,25 @@
         <v>3726</v>
       </c>
       <c r="E7" s="11">
-        <v>1.871</v>
+        <v>4.08</v>
       </c>
       <c r="F7" s="4">
         <v>4928</v>
       </c>
       <c r="G7" s="11">
-        <v>2.57</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H7" s="4">
         <v>5039</v>
       </c>
       <c r="I7" s="11">
-        <v>2.5569999999999999</v>
+        <v>3.1070000000000002</v>
       </c>
       <c r="J7" s="4">
         <v>6295</v>
       </c>
       <c r="K7" s="11">
-        <v>3.52</v>
+        <v>4.0529999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -927,7 +940,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C8" s="11">
         <v>5</v>
@@ -936,25 +949,25 @@
         <v>2071</v>
       </c>
       <c r="E8" s="11">
-        <v>0.29199999999999998</v>
+        <v>0.37</v>
       </c>
       <c r="F8" s="4">
         <v>2660</v>
       </c>
       <c r="G8" s="11">
-        <v>0.33800000000000002</v>
+        <v>0.77300000000000002</v>
       </c>
       <c r="H8" s="4">
         <v>2276</v>
       </c>
       <c r="I8" s="11">
-        <v>0.23799999999999999</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="J8" s="4">
         <v>2954</v>
       </c>
       <c r="K8" s="11">
-        <v>0.33200000000000002</v>
+        <v>0.65300000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -962,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C9" s="11">
         <v>1.2</v>
@@ -971,25 +984,25 @@
         <v>612</v>
       </c>
       <c r="E9" s="11">
-        <v>0.22600000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="F9" s="4">
         <v>579</v>
       </c>
       <c r="G9" s="11">
-        <v>0.12</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="H9" s="4">
         <v>747</v>
       </c>
       <c r="I9" s="11">
-        <v>0.13300000000000001</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="J9" s="4">
         <v>602</v>
       </c>
       <c r="K9" s="11">
-        <v>0.14199999999999999</v>
+        <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -997,7 +1010,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C10" s="11">
         <v>1.5</v>
@@ -1006,25 +1019,25 @@
         <v>210</v>
       </c>
       <c r="E10" s="11">
-        <v>0.159</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="F10" s="4">
         <v>213</v>
       </c>
       <c r="G10" s="11">
-        <v>5.1999999999999998E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="H10" s="4">
         <v>221</v>
       </c>
       <c r="I10" s="11">
-        <v>5.0999999999999997E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="J10" s="4">
         <v>223</v>
       </c>
       <c r="K10" s="11">
-        <v>5.0999999999999997E-2</v>
+        <v>4.7E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1032,7 +1045,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C11" s="11">
         <v>5</v>
@@ -1041,25 +1054,25 @@
         <v>9225</v>
       </c>
       <c r="E11" s="11">
-        <v>2.633</v>
+        <v>5.3250000000000002</v>
       </c>
       <c r="F11" s="4">
         <v>17963</v>
       </c>
       <c r="G11" s="11">
-        <v>5.1280000000000001</v>
+        <v>6.9080000000000004</v>
       </c>
       <c r="H11" s="4">
         <v>10816</v>
       </c>
       <c r="I11" s="11">
-        <v>3.343</v>
+        <v>3.7970000000000002</v>
       </c>
       <c r="J11" s="4">
         <v>21376</v>
       </c>
       <c r="K11" s="11">
-        <v>6.5</v>
+        <v>10.728</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1067,34 +1080,34 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C12" s="11">
         <v>10</v>
       </c>
       <c r="D12" s="4">
-        <v>1211</v>
+        <v>1137</v>
       </c>
       <c r="E12" s="11">
-        <v>0.10199999999999999</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="F12" s="4">
-        <v>1211</v>
+        <v>1137</v>
       </c>
       <c r="G12" s="11">
-        <v>0.115</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="H12" s="4">
-        <v>1211</v>
+        <v>1137</v>
       </c>
       <c r="I12" s="11">
-        <v>6.3E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="J12" s="4">
-        <v>1211</v>
+        <v>1137</v>
       </c>
       <c r="K12" s="11">
-        <v>7.4999999999999997E-2</v>
+        <v>0.10100000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1102,34 +1115,34 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C13" s="11">
         <v>10</v>
       </c>
       <c r="D13" s="4">
-        <v>1303</v>
+        <v>1312</v>
       </c>
       <c r="E13" s="11">
-        <v>0.255</v>
+        <v>0.187</v>
       </c>
       <c r="F13" s="3">
-        <v>1444</v>
+        <v>1420</v>
       </c>
       <c r="G13" s="11">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="H13" s="4">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="I13" s="11">
         <v>0.16900000000000001</v>
       </c>
       <c r="J13" s="4">
-        <v>1516</v>
+        <v>1544</v>
       </c>
       <c r="K13" s="11">
-        <v>0.26300000000000001</v>
+        <v>0.24199999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1137,34 +1150,34 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C14" s="11">
         <v>45</v>
       </c>
       <c r="D14" s="4">
-        <v>5568</v>
+        <v>5530</v>
       </c>
       <c r="E14" s="11">
-        <v>0.308</v>
+        <v>1.0429999999999999</v>
       </c>
       <c r="F14" s="3">
-        <v>5568</v>
+        <v>5530</v>
       </c>
       <c r="G14" s="11">
-        <v>0.41899999999999998</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="H14" s="4">
-        <v>5568</v>
+        <v>5530</v>
       </c>
       <c r="I14" s="11">
-        <v>0.35699999999999998</v>
+        <v>0.59899999999999998</v>
       </c>
       <c r="J14" s="4">
-        <v>5568</v>
+        <v>5530</v>
       </c>
       <c r="K14" s="11">
-        <v>0.377</v>
+        <v>0.54500000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1172,7 +1185,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C15" s="11">
         <v>4</v>
@@ -1181,25 +1194,25 @@
         <v>721</v>
       </c>
       <c r="E15" s="11">
-        <v>0.184</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="F15" s="3">
         <v>860</v>
       </c>
       <c r="G15" s="11">
-        <v>8.5000000000000006E-2</v>
+        <v>0.122</v>
       </c>
       <c r="H15" s="3">
         <v>800</v>
       </c>
       <c r="I15" s="11">
-        <v>8.2000000000000003E-2</v>
+        <v>0.113</v>
       </c>
       <c r="J15" s="3">
         <v>989</v>
       </c>
       <c r="K15" s="11">
-        <v>0.105</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1207,34 +1220,34 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C16" s="11">
         <v>10</v>
       </c>
       <c r="D16" s="4">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="E16" s="11">
-        <v>0.185</v>
+        <v>0.188</v>
       </c>
       <c r="F16" s="3">
-        <v>1404</v>
+        <v>1395</v>
       </c>
       <c r="G16" s="11">
-        <v>0.17199999999999999</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="H16" s="3">
-        <v>1396</v>
+        <v>1420</v>
       </c>
       <c r="I16" s="11">
-        <v>0.111</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="J16" s="3">
-        <v>1456</v>
+        <v>1483</v>
       </c>
       <c r="K16" s="11">
-        <v>0.151</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1242,34 +1255,34 @@
         <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C17" s="11">
         <v>15</v>
       </c>
       <c r="D17" s="4">
-        <v>6367</v>
+        <v>6548</v>
       </c>
       <c r="E17" s="11">
-        <v>1.2929999999999999</v>
+        <v>2.6379999999999999</v>
       </c>
       <c r="F17" s="3">
-        <v>6644</v>
+        <v>6766</v>
       </c>
       <c r="G17" s="11">
-        <v>1.135</v>
+        <v>2.7170000000000001</v>
       </c>
       <c r="H17" s="3">
-        <v>6035</v>
+        <v>5890</v>
       </c>
       <c r="I17" s="11">
-        <v>1.079</v>
+        <v>1.0669999999999999</v>
       </c>
       <c r="J17" s="3">
-        <v>6527</v>
+        <v>6423</v>
       </c>
       <c r="K17" s="11">
-        <v>1.2789999999999999</v>
+        <v>1.248</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1277,7 +1290,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C18" s="11">
         <v>2</v>
@@ -1286,25 +1299,25 @@
         <v>289</v>
       </c>
       <c r="E18" s="11">
-        <v>0.13900000000000001</v>
+        <v>0.126</v>
       </c>
       <c r="F18" s="3">
         <v>301</v>
       </c>
       <c r="G18" s="11">
-        <v>6.6000000000000003E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="H18" s="3">
         <v>313</v>
       </c>
       <c r="I18" s="11">
-        <v>7.0999999999999994E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="J18" s="3">
         <v>346</v>
       </c>
       <c r="K18" s="11">
-        <v>6.9000000000000006E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1312,34 +1325,34 @@
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C19" s="11">
         <v>30</v>
       </c>
       <c r="D19" s="4">
-        <v>3443</v>
+        <v>3480</v>
       </c>
       <c r="E19" s="11">
-        <v>0.747</v>
+        <v>1.286</v>
       </c>
       <c r="F19" s="3">
-        <v>3675</v>
+        <v>3658</v>
       </c>
       <c r="G19" s="11">
-        <v>0.63900000000000001</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="H19" s="3">
-        <v>3496</v>
+        <v>3551</v>
       </c>
       <c r="I19" s="11">
-        <v>0.52800000000000002</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="J19" s="3">
-        <v>3803</v>
+        <v>3800</v>
       </c>
       <c r="K19" s="11">
-        <v>0.68799999999999994</v>
+        <v>0.79700000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1347,34 +1360,34 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C20" s="11">
         <v>50</v>
       </c>
       <c r="D20" s="4">
-        <v>6874</v>
+        <v>7278</v>
       </c>
       <c r="E20" s="11">
-        <v>0.83399999999999996</v>
+        <v>1.1930000000000001</v>
       </c>
       <c r="F20" s="3">
-        <v>7094</v>
+        <v>7037</v>
       </c>
       <c r="G20" s="11">
-        <v>0.88300000000000001</v>
+        <v>1.0649999999999999</v>
       </c>
       <c r="H20" s="3">
-        <v>98871</v>
+        <v>98449</v>
       </c>
       <c r="I20" s="11">
-        <v>9.9429999999999996</v>
+        <v>9.2309999999999999</v>
       </c>
       <c r="J20" s="3">
-        <v>99867</v>
+        <v>99644</v>
       </c>
       <c r="K20" s="11">
-        <v>11.047000000000001</v>
+        <v>10.656000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1382,7 +1395,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C21" s="11">
         <v>30</v>
@@ -1391,25 +1404,25 @@
         <v>3697</v>
       </c>
       <c r="E21" s="11">
-        <v>0.63400000000000001</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="F21" s="3">
         <v>4605</v>
       </c>
       <c r="G21" s="11">
-        <v>0.53900000000000003</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="H21" s="3">
         <v>3969</v>
       </c>
       <c r="I21" s="11">
-        <v>0.375</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="J21" s="3">
         <v>3933</v>
       </c>
       <c r="K21" s="11">
-        <v>0.38400000000000001</v>
+        <v>0.44600000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1417,34 +1430,34 @@
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C22" s="11">
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <v>2229</v>
+        <v>1680</v>
       </c>
       <c r="E22" s="11">
-        <v>4.8159999999999998</v>
+        <v>3.7629999999999999</v>
       </c>
       <c r="F22" s="3">
-        <v>2229</v>
+        <v>1680</v>
       </c>
       <c r="G22" s="11">
-        <v>4.3360000000000003</v>
+        <v>2.4039999999999999</v>
       </c>
       <c r="H22" s="3">
-        <v>2229</v>
+        <v>1680</v>
       </c>
       <c r="I22" s="11">
-        <v>4.242</v>
+        <v>2.4119999999999999</v>
       </c>
       <c r="J22" s="3">
-        <v>2229</v>
+        <v>1680</v>
       </c>
       <c r="K22" s="11">
-        <v>4.2729999999999997</v>
+        <v>2.8330000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1452,34 +1465,34 @@
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="C23" s="11">
         <v>15</v>
       </c>
       <c r="D23" s="4">
-        <v>3105</v>
+        <v>3281</v>
       </c>
       <c r="E23" s="11">
-        <v>1.262</v>
+        <v>1.93</v>
       </c>
       <c r="F23" s="3">
-        <v>2987</v>
+        <v>3192</v>
       </c>
       <c r="G23" s="11">
-        <v>1.256</v>
+        <v>1.546</v>
       </c>
       <c r="H23" s="3">
-        <v>3783</v>
+        <v>3683</v>
       </c>
       <c r="I23" s="11">
-        <v>1.2869999999999999</v>
+        <v>1.212</v>
       </c>
       <c r="J23" s="3">
-        <v>3676</v>
+        <v>3716</v>
       </c>
       <c r="K23" s="11">
-        <v>1.2529999999999999</v>
+        <v>1.2430000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1487,34 +1500,34 @@
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C24" s="11">
         <v>4</v>
       </c>
       <c r="D24" s="4">
-        <v>131</v>
+        <v>252</v>
       </c>
       <c r="E24" s="11">
-        <v>0.14299999999999999</v>
+        <v>0.127</v>
       </c>
       <c r="F24" s="3">
-        <v>131</v>
+        <v>252</v>
       </c>
       <c r="G24" s="11">
-        <v>5.2999999999999999E-2</v>
+        <v>0.08</v>
       </c>
       <c r="H24" s="3">
-        <v>131</v>
+        <v>252</v>
       </c>
       <c r="I24" s="11">
-        <v>5.6000000000000001E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="J24" s="3">
-        <v>131</v>
+        <v>252</v>
       </c>
       <c r="K24" s="11">
-        <v>5.8999999999999997E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1522,34 +1535,34 @@
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C25" s="11">
         <v>30</v>
       </c>
       <c r="D25" s="4">
-        <v>4739</v>
+        <v>4728</v>
       </c>
       <c r="E25" s="11">
-        <v>3.8479999999999999</v>
+        <v>6.71</v>
       </c>
       <c r="F25" s="3">
-        <v>5195</v>
+        <v>5206</v>
       </c>
       <c r="G25" s="11">
-        <v>4.2699999999999996</v>
+        <v>4.657</v>
       </c>
       <c r="H25" s="3">
-        <v>4547</v>
+        <v>4578</v>
       </c>
       <c r="I25" s="11">
-        <v>3.871</v>
+        <v>3.7160000000000002</v>
       </c>
       <c r="J25" s="3">
-        <v>5128</v>
+        <v>5138</v>
       </c>
       <c r="K25" s="11">
-        <v>4.5529999999999999</v>
+        <v>4.7919999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1557,34 +1570,34 @@
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="C26" s="11">
         <v>12</v>
       </c>
       <c r="D26" s="4">
-        <v>14171</v>
+        <v>13314</v>
       </c>
       <c r="E26" s="11">
-        <v>6.2629999999999999</v>
+        <v>7.2830000000000004</v>
       </c>
       <c r="F26" s="3">
-        <v>14108</v>
+        <v>13020</v>
       </c>
       <c r="G26" s="11">
-        <v>6.0140000000000002</v>
+        <v>5.6420000000000003</v>
       </c>
       <c r="H26" s="3">
-        <v>20521</v>
+        <v>20877</v>
       </c>
       <c r="I26" s="11">
-        <v>8.7970000000000006</v>
+        <v>9.6059999999999999</v>
       </c>
       <c r="J26" s="3">
-        <v>19890</v>
+        <v>20428</v>
       </c>
       <c r="K26" s="11">
-        <v>8.6489999999999991</v>
+        <v>9.2189999999999994</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1592,34 +1605,34 @@
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C27" s="11">
         <v>20</v>
       </c>
       <c r="D27" s="9">
-        <v>3433</v>
+        <v>3367</v>
       </c>
       <c r="E27" s="11">
-        <v>2.2690000000000001</v>
+        <v>2.895</v>
       </c>
       <c r="F27" s="3">
-        <v>4404</v>
+        <v>4459</v>
       </c>
       <c r="G27" s="11">
-        <v>3.4060000000000001</v>
+        <v>3.6219999999999999</v>
       </c>
       <c r="H27" s="3">
-        <v>3534</v>
+        <v>3476</v>
       </c>
       <c r="I27" s="11">
-        <v>2.1539999999999999</v>
+        <v>2.06</v>
       </c>
       <c r="J27" s="3">
-        <v>4409</v>
+        <v>5659</v>
       </c>
       <c r="K27" s="11">
-        <v>3.4159999999999999</v>
+        <v>5.1970000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1627,7 +1640,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C28" s="11">
         <v>7.5</v>
@@ -1636,7 +1649,7 @@
         <v>941</v>
       </c>
       <c r="E28" s="11">
-        <v>0.249</v>
+        <v>0.151</v>
       </c>
       <c r="F28" s="3">
         <v>1022</v>
@@ -1648,13 +1661,13 @@
         <v>967</v>
       </c>
       <c r="I28" s="11">
-        <v>0.13100000000000001</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="J28" s="3">
         <v>1061</v>
       </c>
       <c r="K28" s="11">
-        <v>0.156</v>
+        <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1662,7 +1675,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C29" s="11">
         <v>5</v>
@@ -1671,25 +1684,25 @@
         <v>756</v>
       </c>
       <c r="E29" s="11">
-        <v>0.21299999999999999</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="F29" s="3">
         <v>848</v>
       </c>
       <c r="G29" s="11">
-        <v>0.159</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="H29" s="3">
         <v>785</v>
       </c>
       <c r="I29" s="11">
-        <v>0.221</v>
+        <v>0.18</v>
       </c>
       <c r="J29" s="3">
         <v>899</v>
       </c>
       <c r="K29" s="11">
-        <v>0.216</v>
+        <v>0.16300000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1697,7 +1710,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C30" s="11">
         <v>20</v>
@@ -1706,25 +1719,25 @@
         <v>10378</v>
       </c>
       <c r="E30" s="11">
-        <v>12.255000000000001</v>
+        <v>14.446999999999999</v>
       </c>
       <c r="F30" s="3">
         <v>12300</v>
       </c>
       <c r="G30" s="11">
-        <v>24.074000000000002</v>
+        <v>21.109000000000002</v>
       </c>
       <c r="H30" s="3">
         <v>11935</v>
       </c>
       <c r="I30" s="11">
-        <v>18.384</v>
+        <v>18.190999999999999</v>
       </c>
       <c r="J30" s="3">
         <v>13347</v>
       </c>
       <c r="K30" s="11">
-        <v>31.193000000000001</v>
+        <v>28.872</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1732,7 +1745,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C31" s="11">
         <v>5</v>
@@ -1741,25 +1754,25 @@
         <v>891</v>
       </c>
       <c r="E31" s="11">
-        <v>0.41599999999999998</v>
+        <v>0.307</v>
       </c>
       <c r="F31" s="3">
         <v>919</v>
       </c>
       <c r="G31" s="11">
-        <v>0.33600000000000002</v>
+        <v>0.497</v>
       </c>
       <c r="H31" s="3">
         <v>838</v>
       </c>
       <c r="I31" s="11">
-        <v>0.25</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="J31" s="3">
         <v>938</v>
       </c>
       <c r="K31" s="11">
-        <v>0.27800000000000002</v>
+        <v>0.34399999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1767,34 +1780,34 @@
         <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C32" s="11">
         <v>20</v>
       </c>
       <c r="D32" s="4">
-        <v>2439</v>
+        <v>2443</v>
       </c>
       <c r="E32" s="11">
-        <v>1.9339999999999999</v>
+        <v>2.177</v>
       </c>
       <c r="F32" s="3">
-        <v>5539</v>
+        <v>5628</v>
       </c>
       <c r="G32" s="11">
-        <v>8.1999999999999993</v>
+        <v>10.552</v>
       </c>
       <c r="H32" s="3">
-        <v>2517</v>
+        <v>2519</v>
       </c>
       <c r="I32" s="11">
-        <v>1.3360000000000001</v>
+        <v>1.5620000000000001</v>
       </c>
       <c r="J32" s="3">
-        <v>6007</v>
+        <v>6233</v>
       </c>
       <c r="K32" s="11">
-        <v>9.2289999999999992</v>
+        <v>9.5719999999999992</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1802,7 +1815,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C33" s="11">
         <v>10</v>
@@ -1811,25 +1824,25 @@
         <v>2706</v>
       </c>
       <c r="E33" s="11">
-        <v>0.58599999999999997</v>
+        <v>0.8</v>
       </c>
       <c r="F33" s="3">
         <v>4132</v>
       </c>
       <c r="G33" s="11">
-        <v>0.85299999999999998</v>
+        <v>1.4119999999999999</v>
       </c>
       <c r="H33" s="3">
         <v>3099</v>
       </c>
       <c r="I33" s="11">
-        <v>0.49399999999999999</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="J33" s="3">
         <v>4432</v>
       </c>
       <c r="K33" s="11">
-        <v>0.88</v>
+        <v>1.2110000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -1837,7 +1850,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C34" s="11">
         <v>3</v>
@@ -1846,25 +1859,25 @@
         <v>429</v>
       </c>
       <c r="E34" s="11">
-        <v>0.221</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="F34" s="3">
         <v>804</v>
       </c>
       <c r="G34" s="11">
-        <v>0.40799999999999997</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="H34" s="3">
         <v>504</v>
       </c>
       <c r="I34" s="11">
-        <v>0.127</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J34" s="3">
         <v>864</v>
       </c>
       <c r="K34" s="11">
-        <v>0.41299999999999998</v>
+        <v>0.53900000000000003</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1872,34 +1885,34 @@
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C35" s="11">
         <v>11</v>
       </c>
       <c r="D35" s="4">
-        <v>1631</v>
+        <v>1669</v>
       </c>
       <c r="E35" s="11">
-        <v>0.318</v>
+        <v>0.505</v>
       </c>
       <c r="F35" s="3">
-        <v>3107</v>
+        <v>3230</v>
       </c>
       <c r="G35" s="11">
-        <v>0.872</v>
+        <v>1.33</v>
       </c>
       <c r="H35" s="3">
-        <v>1673</v>
+        <v>1740</v>
       </c>
       <c r="I35" s="11">
-        <v>0.23799999999999999</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="J35" s="3">
-        <v>3193</v>
+        <v>3256</v>
       </c>
       <c r="K35" s="11">
-        <v>0.876</v>
+        <v>1.1240000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -1907,34 +1920,34 @@
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C36" s="11">
         <v>36</v>
       </c>
       <c r="D36" s="4">
-        <v>4486</v>
+        <v>16225</v>
       </c>
       <c r="E36" s="11">
-        <v>0.93899999999999995</v>
+        <v>3.9470000000000001</v>
       </c>
       <c r="F36" s="3">
-        <v>6801</v>
+        <v>7518</v>
       </c>
       <c r="G36" s="11">
-        <v>2.0049999999999999</v>
+        <v>1.8759999999999999</v>
       </c>
       <c r="H36" s="3">
-        <v>4520</v>
+        <v>16292</v>
       </c>
       <c r="I36" s="11">
-        <v>0.749</v>
+        <v>2.8</v>
       </c>
       <c r="J36" s="3">
-        <v>6944</v>
+        <v>7879</v>
       </c>
       <c r="K36" s="11">
-        <v>2.2719999999999998</v>
+        <v>2.0960000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1942,34 +1955,34 @@
         <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C37" s="11">
         <v>48</v>
       </c>
       <c r="D37" s="4">
-        <v>5610</v>
+        <v>10017</v>
       </c>
       <c r="E37" s="11">
-        <v>0.85199999999999998</v>
+        <v>1.665</v>
       </c>
       <c r="F37" s="3">
-        <v>8361</v>
+        <v>12803</v>
       </c>
       <c r="G37" s="11">
-        <v>2.2879999999999998</v>
+        <v>2.883</v>
       </c>
       <c r="H37" s="3">
-        <v>5672</v>
+        <v>10165</v>
       </c>
       <c r="I37" s="11">
-        <v>0.64900000000000002</v>
+        <v>1.2370000000000001</v>
       </c>
       <c r="J37" s="3">
-        <v>8368</v>
+        <v>13145</v>
       </c>
       <c r="K37" s="11">
-        <v>2.444</v>
+        <v>2.8079999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1977,34 +1990,34 @@
         <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C38" s="11">
         <v>36</v>
       </c>
       <c r="D38" s="4">
-        <v>4176</v>
+        <v>6673</v>
       </c>
       <c r="E38" s="11">
-        <v>1.071</v>
+        <v>2.415</v>
       </c>
       <c r="F38" s="3">
-        <v>4658</v>
+        <v>7442</v>
       </c>
       <c r="G38" s="11">
-        <v>1.42</v>
+        <v>2.4540000000000002</v>
       </c>
       <c r="H38" s="3">
-        <v>4246</v>
+        <v>6743</v>
       </c>
       <c r="I38" s="11">
-        <v>1.044</v>
+        <v>1.833</v>
       </c>
       <c r="J38" s="3">
-        <v>4753</v>
+        <v>7793</v>
       </c>
       <c r="K38" s="11">
-        <v>1.4219999999999999</v>
+        <v>2.839</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2012,34 +2025,34 @@
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C39" s="11">
         <v>40</v>
       </c>
       <c r="D39" s="4">
-        <v>4897</v>
+        <v>4355</v>
       </c>
       <c r="E39" s="11">
-        <v>0.64100000000000001</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="F39" s="3">
-        <v>5271</v>
+        <v>4865</v>
       </c>
       <c r="G39" s="11">
-        <v>0.68100000000000005</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="H39" s="3">
-        <v>4914</v>
+        <v>4469</v>
       </c>
       <c r="I39" s="11">
-        <v>0.54</v>
+        <v>0.49</v>
       </c>
       <c r="J39" s="3">
-        <v>5126</v>
+        <v>4986</v>
       </c>
       <c r="K39" s="11">
-        <v>0.67700000000000005</v>
+        <v>0.63700000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2047,34 +2060,34 @@
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C40" s="11">
         <v>36</v>
       </c>
       <c r="D40" s="4">
-        <v>4202</v>
+        <v>6687</v>
       </c>
       <c r="E40" s="11">
-        <v>1.677</v>
+        <v>3.7679999999999998</v>
       </c>
       <c r="F40" s="3">
-        <v>4670</v>
+        <v>8888</v>
       </c>
       <c r="G40" s="11">
-        <v>2.0859999999999999</v>
+        <v>3.61</v>
       </c>
       <c r="H40" s="3">
-        <v>4213</v>
+        <v>6793</v>
       </c>
       <c r="I40" s="11">
-        <v>1.6439999999999999</v>
+        <v>2.774</v>
       </c>
       <c r="J40" s="3">
-        <v>4589</v>
+        <v>9921</v>
       </c>
       <c r="K40" s="11">
-        <v>2.0009999999999999</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2082,34 +2095,34 @@
         <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C41" s="11">
         <v>36</v>
       </c>
       <c r="D41" s="4">
-        <v>4580</v>
+        <v>7002</v>
       </c>
       <c r="E41" s="11">
-        <v>1.373</v>
+        <v>3.0459999999999998</v>
       </c>
       <c r="F41" s="3">
-        <v>4548</v>
+        <v>8332</v>
       </c>
       <c r="G41" s="11">
-        <v>1.407</v>
+        <v>3.407</v>
       </c>
       <c r="H41" s="3">
-        <v>4745</v>
+        <v>7120</v>
       </c>
       <c r="I41" s="11">
-        <v>1.3280000000000001</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J41" s="3">
-        <v>4605</v>
+        <v>8859</v>
       </c>
       <c r="K41" s="11">
-        <v>1.5640000000000001</v>
+        <v>3.597</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2117,34 +2130,34 @@
         <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C42" s="11">
         <v>40</v>
       </c>
       <c r="D42" s="4">
-        <v>6000</v>
+        <v>8714</v>
       </c>
       <c r="E42" s="11">
-        <v>0.71799999999999997</v>
+        <v>1.5509999999999999</v>
       </c>
       <c r="F42" s="3">
-        <v>6408</v>
+        <v>9081</v>
       </c>
       <c r="G42" s="11">
-        <v>0.86599999999999999</v>
+        <v>1.347</v>
       </c>
       <c r="H42" s="3">
-        <v>6419</v>
+        <v>8915</v>
       </c>
       <c r="I42" s="11">
-        <v>0.73399999999999999</v>
+        <v>1.208</v>
       </c>
       <c r="J42" s="3">
-        <v>6765</v>
+        <v>9486</v>
       </c>
       <c r="K42" s="11">
-        <v>0.93500000000000005</v>
+        <v>1.5529999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2152,34 +2165,34 @@
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C43" s="11">
         <v>10</v>
       </c>
       <c r="D43" s="4">
-        <v>1208</v>
+        <v>1227</v>
       </c>
       <c r="E43" s="11">
-        <v>0.53900000000000003</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="F43" s="3">
-        <v>1421</v>
+        <v>1398</v>
       </c>
       <c r="G43" s="11">
-        <v>0.45400000000000001</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="H43" s="3">
-        <v>1246</v>
+        <v>1266</v>
       </c>
       <c r="I43" s="11">
-        <v>0.27</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="J43" s="3">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="K43" s="11">
-        <v>0.42599999999999999</v>
+        <v>0.51400000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -2187,34 +2200,34 @@
         <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C44" s="11">
         <v>24</v>
       </c>
       <c r="D44" s="4">
-        <v>8220</v>
+        <v>8662</v>
       </c>
       <c r="E44" s="11">
-        <v>4.0890000000000004</v>
+        <v>5.5750000000000002</v>
       </c>
       <c r="F44" s="3">
-        <v>6651</v>
+        <v>7021</v>
       </c>
       <c r="G44" s="11">
-        <v>5.3159999999999998</v>
+        <v>5.6420000000000003</v>
       </c>
       <c r="H44" s="3">
-        <v>8193</v>
+        <v>8383</v>
       </c>
       <c r="I44" s="11">
-        <v>3.81</v>
+        <v>4.3410000000000002</v>
       </c>
       <c r="J44" s="3">
-        <v>6729</v>
+        <v>7150</v>
       </c>
       <c r="K44" s="11">
-        <v>5.3440000000000003</v>
+        <v>6.7770000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -2222,34 +2235,34 @@
         <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C45" s="11">
         <v>30</v>
       </c>
       <c r="D45" s="4">
-        <v>4242</v>
+        <v>4189</v>
       </c>
       <c r="E45" s="11">
-        <v>2.9809999999999999</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="F45" s="3">
-        <v>4242</v>
+        <v>4195</v>
       </c>
       <c r="G45" s="11">
-        <v>2.5579999999999998</v>
+        <v>1.748</v>
       </c>
       <c r="H45" s="3">
-        <v>4242</v>
+        <v>4175</v>
       </c>
       <c r="I45" s="11">
-        <v>2.9809999999999999</v>
+        <v>1.619</v>
       </c>
       <c r="J45" s="3">
-        <v>4242</v>
+        <v>4262</v>
       </c>
       <c r="K45" s="11">
-        <v>2.5710000000000002</v>
+        <v>1.9810000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -2257,34 +2270,34 @@
         <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="C46" s="11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D46" s="4">
-        <v>5515</v>
+        <v>4337</v>
       </c>
       <c r="E46" s="11">
-        <v>3.7170000000000001</v>
+        <v>3.8359999999999999</v>
       </c>
       <c r="F46" s="3">
-        <v>9462</v>
+        <v>4337</v>
       </c>
       <c r="G46" s="11">
-        <v>6.9489999999999998</v>
+        <v>2.6059999999999999</v>
       </c>
       <c r="H46" s="3">
-        <v>5558</v>
+        <v>4337</v>
       </c>
       <c r="I46" s="11">
-        <v>3.22</v>
+        <v>2.7269999999999999</v>
       </c>
       <c r="J46" s="3">
-        <v>9667</v>
+        <v>4337</v>
       </c>
       <c r="K46" s="11">
-        <v>7.3250000000000002</v>
+        <v>2.5659999999999998</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -2292,34 +2305,34 @@
         <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C47" s="11">
-        <v>33.72</v>
+        <v>50</v>
       </c>
       <c r="D47" s="4">
-        <v>9375</v>
+        <v>5535</v>
       </c>
       <c r="E47" s="11">
-        <v>5.2859999999999996</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J47" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K47" s="10" t="s">
-        <v>44</v>
+        <v>4.4249999999999998</v>
+      </c>
+      <c r="F47" s="10">
+        <v>9437</v>
+      </c>
+      <c r="G47" s="10">
+        <v>6.4290000000000003</v>
+      </c>
+      <c r="H47" s="10">
+        <v>5565</v>
+      </c>
+      <c r="I47" s="10">
+        <v>3.258</v>
+      </c>
+      <c r="J47" s="10">
+        <v>9610</v>
+      </c>
+      <c r="K47" s="10">
+        <v>7.0439999999999996</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -2327,34 +2340,34 @@
         <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C48" s="11">
-        <v>32.19</v>
+        <v>33.72</v>
       </c>
       <c r="D48" s="4">
-        <v>8828</v>
+        <v>9375</v>
       </c>
       <c r="E48" s="11">
-        <v>5.0209999999999999</v>
+        <v>5.6829999999999998</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
@@ -2362,34 +2375,34 @@
         <v>46</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C49" s="11">
-        <v>59.18</v>
+        <v>32.19</v>
       </c>
       <c r="D49" s="4">
-        <v>15140</v>
+        <v>8828</v>
       </c>
       <c r="E49" s="11">
-        <v>11.003</v>
+        <v>5.4429999999999996</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
@@ -2397,34 +2410,34 @@
         <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C50" s="11">
-        <v>39.020000000000003</v>
+        <v>59.18</v>
       </c>
       <c r="D50" s="4">
-        <v>11499</v>
+        <v>15140</v>
       </c>
       <c r="E50" s="11">
-        <v>7.7409999999999997</v>
+        <v>9.6310000000000002</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
@@ -2432,34 +2445,34 @@
         <v>48</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C51" s="11">
-        <v>34.68</v>
+        <v>39.020000000000003</v>
       </c>
       <c r="D51" s="4">
-        <v>9443</v>
+        <v>11499</v>
       </c>
       <c r="E51" s="11">
-        <v>5.1580000000000004</v>
+        <v>7.5910000000000002</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
@@ -2467,34 +2480,34 @@
         <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C52" s="11">
-        <v>40.82</v>
+        <v>34.68</v>
       </c>
       <c r="D52" s="4">
-        <v>11825</v>
+        <v>9443</v>
       </c>
       <c r="E52" s="11">
-        <v>11.680999999999999</v>
+        <v>4.8490000000000002</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
@@ -2502,34 +2515,34 @@
         <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C53" s="2">
-        <v>41.28</v>
+        <v>40.82</v>
       </c>
       <c r="D53" s="2">
-        <v>11517</v>
+        <v>11825</v>
       </c>
       <c r="E53" s="11">
-        <v>10.426</v>
+        <v>10.99</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
@@ -2537,34 +2550,34 @@
         <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C54" s="2">
-        <v>45.27</v>
+        <v>41.28</v>
       </c>
       <c r="D54" s="2">
-        <v>12245</v>
+        <v>11517</v>
       </c>
       <c r="E54" s="11">
-        <v>14.163</v>
+        <v>8.3740000000000006</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
@@ -2572,34 +2585,69 @@
         <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C55" s="2">
+        <v>45.27</v>
+      </c>
+      <c r="D55" s="2">
+        <v>12245</v>
+      </c>
+      <c r="E55" s="11">
+        <v>13.752000000000001</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56">
         <v>27.71</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D56">
         <v>8945</v>
       </c>
-      <c r="E55" s="11">
-        <v>8.5510000000000002</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I55" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J55" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K55" s="10" t="s">
-        <v>44</v>
+      <c r="E56">
+        <v>8.9930000000000003</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" t="s">
+        <v>11</v>
+      </c>
+      <c r="I56" t="s">
+        <v>11</v>
+      </c>
+      <c r="J56" t="s">
+        <v>11</v>
+      </c>
+      <c r="K56" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>